<commit_message>
Updated KiCost BOM file w manf# field
</commit_message>
<xml_diff>
--- a/kicad/hack.xlsx
+++ b/kicad/hack.xlsx
@@ -11,10 +11,10 @@
   </sheets>
   <definedNames>
     <definedName name="BoardQty">KiCost!$I$1</definedName>
-    <definedName name="digikey_part_data">KiCost!$J$5:$O$31</definedName>
-    <definedName name="global_part_data">KiCost!$A$5:$I$31</definedName>
-    <definedName name="mouser_part_data">KiCost!$P$5:$U$31</definedName>
-    <definedName name="newark_part_data">KiCost!$V$5:$AA$31</definedName>
+    <definedName name="digikey_part_data">KiCost!$J$5:$O$30</definedName>
+    <definedName name="global_part_data">KiCost!$A$5:$I$30</definedName>
+    <definedName name="mouser_part_data">KiCost!$P$5:$U$30</definedName>
+    <definedName name="newark_part_data">KiCost!$V$5:$AA$30</definedName>
     <definedName name="TotalCost">KiCost!$I$2</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -383,7 +383,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="126">
   <si>
     <t>Global Part Info</t>
   </si>
@@ -424,55 +424,223 @@
     <t>hack-footprints:SPST-PTS_810</t>
   </si>
   <si>
+    <t>311020045</t>
+  </si>
+  <si>
+    <t>C5</t>
+  </si>
+  <si>
+    <t>4.7nF</t>
+  </si>
+  <si>
+    <t>hack:C_0603_HandSoldering</t>
+  </si>
+  <si>
+    <t>302010144</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>1M</t>
+  </si>
+  <si>
+    <t>hack:R_0603_HandSoldering</t>
+  </si>
+  <si>
+    <t>301010151</t>
+  </si>
+  <si>
+    <t>U1</t>
+  </si>
+  <si>
+    <t>MIC5528</t>
+  </si>
+  <si>
+    <t>hack:DFN-6-1EP_1.2x1.2mm_Pitch0.4mm</t>
+  </si>
+  <si>
+    <t>MIC5528-3.3YMT-TR</t>
+  </si>
+  <si>
+    <t>L1</t>
+  </si>
+  <si>
+    <t>BLM18EG221</t>
+  </si>
+  <si>
+    <t>hack:L_0603_HandSoldering</t>
+  </si>
+  <si>
+    <t>BLM18EG221SN1D</t>
+  </si>
+  <si>
+    <t>U2</t>
+  </si>
+  <si>
+    <t>STF202</t>
+  </si>
+  <si>
+    <t>hack:TSOP-6</t>
+  </si>
+  <si>
+    <t>STF202-22T1G</t>
+  </si>
+  <si>
+    <t>L2</t>
+  </si>
+  <si>
+    <t>10uH</t>
+  </si>
+  <si>
+    <t>hack:ELLVFG</t>
+  </si>
+  <si>
+    <t>ELL-VFG100MC</t>
+  </si>
+  <si>
+    <t>LOGO1</t>
+  </si>
+  <si>
+    <t>OSHW</t>
+  </si>
+  <si>
+    <t>hack:OSHW-LOGO</t>
+  </si>
+  <si>
+    <t>mfr_pn</t>
+  </si>
+  <si>
+    <t>C6,C7</t>
+  </si>
+  <si>
+    <t>10pF</t>
+  </si>
+  <si>
+    <t>302010097</t>
+  </si>
+  <si>
+    <t>X1</t>
+  </si>
+  <si>
+    <t>ABS07</t>
+  </si>
+  <si>
+    <t>306010055</t>
+  </si>
+  <si>
+    <t>R2,R4</t>
+  </si>
+  <si>
+    <t>330</t>
+  </si>
+  <si>
+    <t>301010300</t>
+  </si>
+  <si>
+    <t>FID1-FID3</t>
+  </si>
+  <si>
+    <t>FIDUCIAL</t>
+  </si>
+  <si>
+    <t>hack:FIDUCIAL</t>
+  </si>
+  <si>
+    <t>C3,C4</t>
+  </si>
+  <si>
+    <t>10uF</t>
+  </si>
+  <si>
+    <t>hack:c_elec_3x5.3</t>
+  </si>
+  <si>
+    <t>UWX1C100MCL2GB</t>
+  </si>
+  <si>
+    <t>LOGO3</t>
+  </si>
+  <si>
+    <t>HACK</t>
+  </si>
+  <si>
+    <t>U3</t>
+  </si>
+  <si>
+    <t>ATSAMD21E</t>
+  </si>
+  <si>
+    <t>hack:QFN-32-1EP_5x5mm_Pitch0.5mm</t>
+  </si>
+  <si>
+    <t>ATSAMD21E18A-MU</t>
+  </si>
+  <si>
     <t>D1</t>
   </si>
   <si>
-    <t>BLUE</t>
+    <t>RED</t>
   </si>
   <si>
     <t>hack:LED_0603_HandSoldering</t>
   </si>
   <si>
-    <t>R1</t>
-  </si>
-  <si>
-    <t>1M</t>
-  </si>
-  <si>
-    <t>hack:R_0603_HandSoldering</t>
-  </si>
-  <si>
-    <t>C5</t>
-  </si>
-  <si>
-    <t>4.5nF</t>
-  </si>
-  <si>
-    <t>hack:C_0603_HandSoldering</t>
-  </si>
-  <si>
-    <t>LOGO1</t>
-  </si>
-  <si>
-    <t>OSHW</t>
-  </si>
-  <si>
-    <t>hack:OSHW-LOGO</t>
-  </si>
-  <si>
-    <t>mfr_pn</t>
-  </si>
-  <si>
-    <t>C6,C7</t>
-  </si>
-  <si>
-    <t>10pF</t>
-  </si>
-  <si>
-    <t>R4</t>
-  </si>
-  <si>
-    <t>330</t>
+    <t>304090042</t>
+  </si>
+  <si>
+    <t>R3</t>
+  </si>
+  <si>
+    <t>10k</t>
+  </si>
+  <si>
+    <t>301010299</t>
+  </si>
+  <si>
+    <t>P2,P3</t>
+  </si>
+  <si>
+    <t>CONN_01X13</t>
+  </si>
+  <si>
+    <t>hack-footprints:Pin_Castellated_1x13</t>
+  </si>
+  <si>
+    <t>JP1</t>
+  </si>
+  <si>
+    <t>Jumper_NO_Small</t>
+  </si>
+  <si>
+    <t>hack:SMD_Jumper</t>
+  </si>
+  <si>
+    <t>LOGO2</t>
+  </si>
+  <si>
+    <t>HACKADAY</t>
+  </si>
+  <si>
+    <t>hack:HACKADAY-LOGO</t>
+  </si>
+  <si>
+    <t>C8-C11</t>
+  </si>
+  <si>
+    <t>100nF</t>
+  </si>
+  <si>
+    <t>302010138</t>
+  </si>
+  <si>
+    <t>P4</t>
+  </si>
+  <si>
+    <t>CONN_01X01</t>
+  </si>
+  <si>
+    <t>hack-footprints:Pin_Castellated_1x01</t>
   </si>
   <si>
     <t>P1</t>
@@ -484,136 +652,7 @@
     <t>hack:47346-0001</t>
   </si>
   <si>
-    <t>FID1-FID3</t>
-  </si>
-  <si>
-    <t>FIDUCIAL</t>
-  </si>
-  <si>
-    <t>hack:FIDUCIAL</t>
-  </si>
-  <si>
-    <t>C3,C4</t>
-  </si>
-  <si>
-    <t>10uF</t>
-  </si>
-  <si>
-    <t>hack:c_elec_3x5.3</t>
-  </si>
-  <si>
-    <t>U2</t>
-  </si>
-  <si>
-    <t>STF202</t>
-  </si>
-  <si>
-    <t>hack:TSOP-6</t>
-  </si>
-  <si>
-    <t>LOGO3</t>
-  </si>
-  <si>
-    <t>HACK</t>
-  </si>
-  <si>
-    <t>U1</t>
-  </si>
-  <si>
-    <t>MIC5528</t>
-  </si>
-  <si>
-    <t>hack:DFN-6-1EP_1.2x1.2mm_Pitch0.4mm</t>
-  </si>
-  <si>
-    <t>U3</t>
-  </si>
-  <si>
-    <t>ATSAMD21E</t>
-  </si>
-  <si>
-    <t>hack:QFN-32-1EP_5x5mm_Pitch0.5mm</t>
-  </si>
-  <si>
-    <t>X1</t>
-  </si>
-  <si>
-    <t>ABS07</t>
-  </si>
-  <si>
-    <t>ABS07-32.768KHZ-7-T</t>
-  </si>
-  <si>
-    <t>R3</t>
-  </si>
-  <si>
-    <t>10k</t>
-  </si>
-  <si>
-    <t>P2,P3</t>
-  </si>
-  <si>
-    <t>CONN_01X13</t>
-  </si>
-  <si>
-    <t>hack-footprints:Pin_Castellated_1x13</t>
-  </si>
-  <si>
-    <t>L2</t>
-  </si>
-  <si>
-    <t>10uH</t>
-  </si>
-  <si>
-    <t>hack:ELLVFG</t>
-  </si>
-  <si>
-    <t>L1</t>
-  </si>
-  <si>
-    <t>BLM18EG221</t>
-  </si>
-  <si>
-    <t>hack:L_0603_HandSoldering</t>
-  </si>
-  <si>
-    <t>JP1</t>
-  </si>
-  <si>
-    <t>Jumper_NO_Small</t>
-  </si>
-  <si>
-    <t>hack:SMD_Jumper</t>
-  </si>
-  <si>
-    <t>LOGO2</t>
-  </si>
-  <si>
-    <t>HACKADAY</t>
-  </si>
-  <si>
-    <t>hack:HACKADAY-LOGO</t>
-  </si>
-  <si>
-    <t>C8-C11</t>
-  </si>
-  <si>
-    <t>100nF</t>
-  </si>
-  <si>
-    <t>P4</t>
-  </si>
-  <si>
-    <t>CONN_01X01</t>
-  </si>
-  <si>
-    <t>hack-footprints:Pin_Castellated_1x01</t>
-  </si>
-  <si>
-    <t>R2</t>
-  </si>
-  <si>
-    <t>68</t>
+    <t>320010000</t>
   </si>
   <si>
     <t>C1,C2</t>
@@ -622,6 +661,9 @@
     <t>2.2uF</t>
   </si>
   <si>
+    <t>302010054</t>
+  </si>
+  <si>
     <t>Board Qty:</t>
   </si>
   <si>
@@ -646,25 +688,79 @@
     <t>Cat#</t>
   </si>
   <si>
-    <t>535-9543-1-ND</t>
+    <t>576-4766-1-ND</t>
   </si>
   <si>
     <t>Link</t>
   </si>
   <si>
+    <t>490-3992-1-ND</t>
+  </si>
+  <si>
+    <t>STF202-22T1GOSCT-ND</t>
+  </si>
+  <si>
+    <t>PCD2293CT-ND</t>
+  </si>
+  <si>
+    <t>493-2099-1-ND</t>
+  </si>
+  <si>
+    <t>ATSAMD21E18A-MU-ND</t>
+  </si>
+  <si>
+    <t>13410-63200100000-ND</t>
+  </si>
+  <si>
     <t>Mouser</t>
   </si>
   <si>
+    <t>998-MIC5528-3.3YMTTR</t>
+  </si>
+  <si>
+    <t>81-BLM18EG221SN1D</t>
+  </si>
+  <si>
+    <t>863-STF202-22T1G</t>
+  </si>
+  <si>
+    <t>667-ELL-VFG100MC</t>
+  </si>
+  <si>
+    <t>575-3301010300240000</t>
+  </si>
+  <si>
+    <t>647-UWX1C100MCL2</t>
+  </si>
+  <si>
     <t>653-VAL</t>
   </si>
   <si>
-    <t>815-ABS07-32.768K7T</t>
+    <t>556-ATSAMD21E18A-MU</t>
+  </si>
+  <si>
+    <t>972-XLH3200100004X</t>
   </si>
   <si>
     <t>Newark</t>
   </si>
   <si>
-    <t>14N8750</t>
+    <t>73M9090</t>
+  </si>
+  <si>
+    <t>45J2271</t>
+  </si>
+  <si>
+    <t>15R1033</t>
+  </si>
+  <si>
+    <t>76T1133</t>
+  </si>
+  <si>
+    <t>58R3619</t>
+  </si>
+  <si>
+    <t>45X9914</t>
   </si>
 </sst>
 </file>
@@ -1111,7 +1207,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AA57"/>
+  <dimension ref="A1:AA55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="9" ySplit="6" topLeftCell="J7" activePane="bottomRight" state="frozen"/>
@@ -1153,7 +1249,7 @@
   <sheetData>
     <row r="1" spans="1:27">
       <c r="H1" s="2" t="s">
-        <v>79</v>
+        <v>93</v>
       </c>
       <c r="I1" s="2">
         <v>100</v>
@@ -1161,28 +1257,28 @@
     </row>
     <row r="2" spans="1:27">
       <c r="H2" s="3" t="s">
-        <v>80</v>
+        <v>94</v>
       </c>
       <c r="I2" s="4">
-        <f>sum(I7:I31)</f>
+        <f>sum(I7:I30)</f>
         <v>0</v>
       </c>
       <c r="M2" s="4">
-        <f>sum(M7:M31)</f>
+        <f>sum(M7:M30)</f>
         <v>0</v>
       </c>
       <c r="S2" s="4">
-        <f>sum(S7:S31)</f>
+        <f>sum(S7:S30)</f>
         <v>0</v>
       </c>
       <c r="Y2" s="4">
-        <f>sum(Y7:Y31)</f>
+        <f>sum(Y7:Y30)</f>
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:27">
       <c r="H3" s="3" t="s">
-        <v>81</v>
+        <v>95</v>
       </c>
       <c r="I3" s="5">
         <f>TotalCost/BoardQty</f>
@@ -1202,7 +1298,7 @@
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
       <c r="J5" s="7" t="s">
-        <v>82</v>
+        <v>96</v>
       </c>
       <c r="K5" s="7"/>
       <c r="L5" s="7"/>
@@ -1210,7 +1306,7 @@
       <c r="N5" s="7"/>
       <c r="O5" s="7"/>
       <c r="P5" s="8" t="s">
-        <v>89</v>
+        <v>109</v>
       </c>
       <c r="Q5" s="8"/>
       <c r="R5" s="8"/>
@@ -1218,7 +1314,7 @@
       <c r="T5" s="8"/>
       <c r="U5" s="8"/>
       <c r="V5" s="9" t="s">
-        <v>92</v>
+        <v>119</v>
       </c>
       <c r="W5" s="9"/>
       <c r="X5" s="9"/>
@@ -1255,10 +1351,10 @@
         <v>2</v>
       </c>
       <c r="J6" s="10" t="s">
-        <v>84</v>
+        <v>98</v>
       </c>
       <c r="K6" s="10" t="s">
-        <v>85</v>
+        <v>99</v>
       </c>
       <c r="L6" s="10" t="s">
         <v>3</v>
@@ -1267,16 +1363,16 @@
         <v>2</v>
       </c>
       <c r="N6" s="10" t="s">
-        <v>86</v>
+        <v>100</v>
       </c>
       <c r="O6" s="10" t="s">
-        <v>83</v>
+        <v>97</v>
       </c>
       <c r="P6" s="10" t="s">
-        <v>84</v>
+        <v>98</v>
       </c>
       <c r="Q6" s="10" t="s">
-        <v>85</v>
+        <v>99</v>
       </c>
       <c r="R6" s="10" t="s">
         <v>3</v>
@@ -1285,16 +1381,16 @@
         <v>2</v>
       </c>
       <c r="T6" s="10" t="s">
-        <v>86</v>
+        <v>100</v>
       </c>
       <c r="U6" s="10" t="s">
-        <v>83</v>
+        <v>97</v>
       </c>
       <c r="V6" s="10" t="s">
-        <v>84</v>
+        <v>98</v>
       </c>
       <c r="W6" s="10" t="s">
-        <v>85</v>
+        <v>99</v>
       </c>
       <c r="X6" s="10" t="s">
         <v>3</v>
@@ -1303,10 +1399,10 @@
         <v>2</v>
       </c>
       <c r="Z6" s="10" t="s">
-        <v>86</v>
+        <v>100</v>
       </c>
       <c r="AA6" s="10" t="s">
-        <v>83</v>
+        <v>97</v>
       </c>
     </row>
     <row r="7" spans="1:27">
@@ -1319,6 +1415,9 @@
       <c r="D7" t="s">
         <v>12</v>
       </c>
+      <c r="F7" t="s">
+        <v>13</v>
+      </c>
       <c r="G7">
         <f>BoardQty*1</f>
         <v>0</v>
@@ -1334,13 +1433,16 @@
     </row>
     <row r="8" spans="1:27">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D8" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="F8" t="s">
+        <v>17</v>
       </c>
       <c r="G8">
         <f>BoardQty*1</f>
@@ -1357,13 +1459,16 @@
     </row>
     <row r="9" spans="1:27">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D9" t="s">
-        <v>18</v>
+        <v>20</v>
+      </c>
+      <c r="F9" t="s">
+        <v>21</v>
       </c>
       <c r="G9">
         <f>BoardQty*1</f>
@@ -1380,13 +1485,16 @@
     </row>
     <row r="10" spans="1:27">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B10" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D10" t="s">
-        <v>21</v>
+        <v>24</v>
+      </c>
+      <c r="F10" t="s">
+        <v>25</v>
       </c>
       <c r="G10">
         <f>BoardQty*1</f>
@@ -1400,19 +1508,53 @@
         <f>iferror(G10*H10,"")</f>
         <v>0</v>
       </c>
+      <c r="J10">
+        <v>5000</v>
+      </c>
+      <c r="L10" s="11">
+        <f>iferror(lookup(if(K10="",G10,K10),{0,1,25,100,4500,5000},{0.0,0.19,0.16,0.14,0.24,0.14}),"")</f>
+        <v>0</v>
+      </c>
+      <c r="M10" s="11">
+        <f>iferror(if(K10="",G10,K10)*L10,"")</f>
+        <v>0</v>
+      </c>
+      <c r="N10" t="s">
+        <v>101</v>
+      </c>
+      <c r="O10" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="P10">
+        <v>4797</v>
+      </c>
+      <c r="R10" s="11">
+        <f>iferror(lookup(if(Q10="",G10,Q10),{0,1,10,25,100,5000},{0.0,0.197,0.187,0.158,0.138,0.138}),"")</f>
+        <v>0</v>
+      </c>
+      <c r="S10" s="11">
+        <f>iferror(if(Q10="",G10,Q10)*R10,"")</f>
+        <v>0</v>
+      </c>
+      <c r="T10" t="s">
+        <v>110</v>
+      </c>
+      <c r="U10" s="12" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="11" spans="1:27">
       <c r="A11" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B11" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="D11" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="F11" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="G11">
         <f>BoardQty*1</f>
@@ -1426,19 +1568,73 @@
         <f>iferror(G11*H11,"")</f>
         <v>0</v>
       </c>
+      <c r="J11">
+        <v>317364</v>
+      </c>
+      <c r="L11" s="11">
+        <f>iferror(lookup(if(K11="",G11,K11),{0,1,10,50,100,250,500,1000,4000,8000,12000},{0.0,0.23,0.175,0.1252,0.1126,0.09508,0.08508,0.07257,0.0637,0.05847,0.05688}),"")</f>
+        <v>0</v>
+      </c>
+      <c r="M11" s="11">
+        <f>iferror(if(K11="",G11,K11)*L11,"")</f>
+        <v>0</v>
+      </c>
+      <c r="N11" t="s">
+        <v>103</v>
+      </c>
+      <c r="O11" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="P11">
+        <v>82768</v>
+      </c>
+      <c r="R11" s="11">
+        <f>iferror(lookup(if(Q11="",G11,Q11),{0,1,10,100,500,1000,4000,8000},{0.0,0.227,0.124,0.095,0.085,0.072,0.063,0.06}),"")</f>
+        <v>0</v>
+      </c>
+      <c r="S11" s="11">
+        <f>iferror(if(Q11="",G11,Q11)*R11,"")</f>
+        <v>0</v>
+      </c>
+      <c r="T11" t="s">
+        <v>111</v>
+      </c>
+      <c r="U11" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="V11">
+        <v>6460</v>
+      </c>
+      <c r="X11" s="11">
+        <f>iferror(lookup(if(W11="",G11,W11),{0,1,50,100,500,1000,2500,5000,10000},{0.0,0.103,0.093,0.075,0.067,0.061,0.056,0.053,0.05}),"")</f>
+        <v>0</v>
+      </c>
+      <c r="Y11" s="11">
+        <f>iferror(if(W11="",G11,W11)*X11,"")</f>
+        <v>0</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>120</v>
+      </c>
+      <c r="AA11" s="12" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="12" spans="1:27">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B12" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="D12" t="s">
-        <v>21</v>
+        <v>32</v>
+      </c>
+      <c r="F12" t="s">
+        <v>33</v>
       </c>
       <c r="G12">
-        <f>BoardQty*2</f>
+        <f>BoardQty*1</f>
         <v>0</v>
       </c>
       <c r="H12" s="11">
@@ -1449,16 +1645,70 @@
         <f>iferror(G12*H12,"")</f>
         <v>0</v>
       </c>
+      <c r="J12">
+        <v>11398</v>
+      </c>
+      <c r="L12" s="11">
+        <f>iferror(lookup(if(K12="",G12,K12),{0,1,10,25,100,250,500,1000,3000,6000,15000,30000,75000,150000},{0.0,0.67,0.569,0.498,0.4264,0.36984,0.31326,0.2415,0.2139,0.2001,0.1863,0.17664,0.1725,0.1656}),"")</f>
+        <v>0</v>
+      </c>
+      <c r="M12" s="11">
+        <f>iferror(if(K12="",G12,K12)*L12,"")</f>
+        <v>0</v>
+      </c>
+      <c r="N12" t="s">
+        <v>104</v>
+      </c>
+      <c r="O12" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="P12">
+        <v>13023</v>
+      </c>
+      <c r="R12" s="11">
+        <f>iferror(lookup(if(Q12="",G12,Q12),{0,1,10,100,1000,3000,9000,24000},{0.0,0.651,0.492,0.308,0.232,0.197,0.183,0.18}),"")</f>
+        <v>0</v>
+      </c>
+      <c r="S12" s="11">
+        <f>iferror(if(Q12="",G12,Q12)*R12,"")</f>
+        <v>0</v>
+      </c>
+      <c r="T12" t="s">
+        <v>112</v>
+      </c>
+      <c r="U12" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="V12">
+        <v>7937</v>
+      </c>
+      <c r="X12" s="11">
+        <f>iferror(lookup(if(W12="",G12,W12),{0,1,25,100,250,500,1000,3000,9000},{0.0,0.66,0.483,0.304,0.294,0.286,0.235,0.201,0.187}),"")</f>
+        <v>0</v>
+      </c>
+      <c r="Y12" s="11">
+        <f>iferror(if(W12="",G12,W12)*X12,"")</f>
+        <v>0</v>
+      </c>
+      <c r="Z12" t="s">
+        <v>121</v>
+      </c>
+      <c r="AA12" s="12" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="13" spans="1:27">
       <c r="A13" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="B13" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="D13" t="s">
-        <v>18</v>
+        <v>36</v>
+      </c>
+      <c r="F13" t="s">
+        <v>37</v>
       </c>
       <c r="G13">
         <f>BoardQty*1</f>
@@ -1472,16 +1722,70 @@
         <f>iferror(G13*H13,"")</f>
         <v>0</v>
       </c>
+      <c r="J13">
+        <v>2526</v>
+      </c>
+      <c r="L13" s="11">
+        <f>iferror(lookup(if(K13="",G13,K13),{0,1,10,50,100,500,2000,4000,6000,10000,20000},{0.0,0.54,0.51,0.4786,0.4466,0.3509,0.1914,0.18502,0.17864,0.17226,0.16397}),"")</f>
+        <v>0</v>
+      </c>
+      <c r="M13" s="11">
+        <f>iferror(if(K13="",G13,K13)*L13,"")</f>
+        <v>0</v>
+      </c>
+      <c r="N13" t="s">
+        <v>105</v>
+      </c>
+      <c r="O13" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="P13">
+        <v>1767</v>
+      </c>
+      <c r="R13" s="11">
+        <f>iferror(lookup(if(Q13="",G13,Q13),{0,1,10,100,1000,2000,10000,24000,50000},{0.0,0.533,0.472,0.347,0.283,0.182,0.177,0.17,0.167}),"")</f>
+        <v>0</v>
+      </c>
+      <c r="S13" s="11">
+        <f>iferror(if(Q13="",G13,Q13)*R13,"")</f>
+        <v>0</v>
+      </c>
+      <c r="T13" t="s">
+        <v>113</v>
+      </c>
+      <c r="U13" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="V13">
+        <v>0</v>
+      </c>
+      <c r="X13" s="11">
+        <f>iferror(lookup(if(W13="",G13,W13),{0,1,2000,4000,10000,20000,40000},{0.0,0.212,0.212,0.203,0.191,0.179,0.166}),"")</f>
+        <v>0</v>
+      </c>
+      <c r="Y13" s="11">
+        <f>iferror(if(W13="",G13,W13)*X13,"")</f>
+        <v>0</v>
+      </c>
+      <c r="Z13" t="s">
+        <v>122</v>
+      </c>
+      <c r="AA13" s="12" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="14" spans="1:27">
       <c r="A14" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="B14" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="D14" t="s">
-        <v>32</v>
+        <v>40</v>
+      </c>
+      <c r="F14" t="s">
+        <v>41</v>
       </c>
       <c r="G14">
         <f>BoardQty*1</f>
@@ -1498,16 +1802,19 @@
     </row>
     <row r="15" spans="1:27">
       <c r="A15" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="B15" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="D15" t="s">
-        <v>35</v>
+        <v>16</v>
+      </c>
+      <c r="F15" t="s">
+        <v>44</v>
       </c>
       <c r="G15">
-        <f>BoardQty*3</f>
+        <f>BoardQty*2</f>
         <v>0</v>
       </c>
       <c r="H15" s="11">
@@ -1521,16 +1828,16 @@
     </row>
     <row r="16" spans="1:27">
       <c r="A16" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="B16" t="s">
-        <v>37</v>
-      </c>
-      <c r="D16" t="s">
-        <v>38</v>
+        <v>46</v>
+      </c>
+      <c r="F16" t="s">
+        <v>47</v>
       </c>
       <c r="G16">
-        <f>BoardQty*2</f>
+        <f>BoardQty*1</f>
         <v>0</v>
       </c>
       <c r="H16" s="11">
@@ -1544,16 +1851,19 @@
     </row>
     <row r="17" spans="1:27">
       <c r="A17" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="B17" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="D17" t="s">
-        <v>41</v>
+        <v>20</v>
+      </c>
+      <c r="F17" t="s">
+        <v>50</v>
       </c>
       <c r="G17">
-        <f>BoardQty*1</f>
+        <f>BoardQty*2</f>
         <v>0</v>
       </c>
       <c r="H17" s="11">
@@ -1564,19 +1874,53 @@
         <f>iferror(G17*H17,"")</f>
         <v>0</v>
       </c>
+      <c r="P17">
+        <v>0</v>
+      </c>
+      <c r="R17" s="11">
+        <f>iferror(lookup(if(Q17="",G17,Q17),{0,1,10,25,50,100,250},{0.0,18.29,15.4,14.21,12.43,11.71,9.76}),"")</f>
+        <v>0</v>
+      </c>
+      <c r="S17" s="11">
+        <f>iferror(if(Q17="",G17,Q17)*R17,"")</f>
+        <v>0</v>
+      </c>
+      <c r="T17" t="s">
+        <v>114</v>
+      </c>
+      <c r="U17" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="V17">
+        <v>6</v>
+      </c>
+      <c r="X17" s="11">
+        <f>iferror(lookup(if(W17="",G17,W17),{0,1,25,50,100,250},{0.0,85.14,81.25,79.09,76.5,73.91}),"")</f>
+        <v>0</v>
+      </c>
+      <c r="Y17" s="11">
+        <f>iferror(if(W17="",G17,W17)*X17,"")</f>
+        <v>0</v>
+      </c>
+      <c r="Z17" t="s">
+        <v>123</v>
+      </c>
+      <c r="AA17" s="12" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="18" spans="1:27">
       <c r="A18" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="B18" t="s">
-        <v>43</v>
-      </c>
-      <c r="F18" t="s">
-        <v>8</v>
+        <v>52</v>
+      </c>
+      <c r="D18" t="s">
+        <v>53</v>
       </c>
       <c r="G18">
-        <f>BoardQty*1</f>
+        <f>BoardQty*3</f>
         <v>0</v>
       </c>
       <c r="H18" s="11">
@@ -1587,36 +1931,22 @@
         <f>iferror(G18*H18,"")</f>
         <v>0</v>
       </c>
-      <c r="P18">
-        <v>149</v>
-      </c>
-      <c r="R18" s="11">
-        <f>iferror(lookup(if(Q18="",G18,Q18),{0,1,25,50,100,200,500},{0.0,1.1,1.02,0.937,0.859,0.799,0.749}),"")</f>
-        <v>0</v>
-      </c>
-      <c r="S18" s="11">
-        <f>iferror(if(Q18="",G18,Q18)*R18,"")</f>
-        <v>0</v>
-      </c>
-      <c r="T18" t="s">
-        <v>90</v>
-      </c>
-      <c r="U18" s="12" t="s">
-        <v>88</v>
-      </c>
     </row>
     <row r="19" spans="1:27">
       <c r="A19" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="B19" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="D19" t="s">
-        <v>46</v>
+        <v>56</v>
+      </c>
+      <c r="F19" t="s">
+        <v>57</v>
       </c>
       <c r="G19">
-        <f>BoardQty*1</f>
+        <f>BoardQty*2</f>
         <v>0</v>
       </c>
       <c r="H19" s="11">
@@ -1627,16 +1957,67 @@
         <f>iferror(G19*H19,"")</f>
         <v>0</v>
       </c>
+      <c r="J19">
+        <v>147965</v>
+      </c>
+      <c r="L19" s="11">
+        <f>iferror(lookup(if(K19="",G19,K19),{0,1,10,25,50,100,250,500,1000,2000,4000,10000,14000,50000,100000},{0.0,0.28,0.237,0.1628,0.1332,0.1184,0.0888,0.07844,0.06956,0.0592,0.05476,0.0518,0.04914,0.0444,0.03922}),"")</f>
+        <v>0</v>
+      </c>
+      <c r="M19" s="11">
+        <f>iferror(if(K19="",G19,K19)*L19,"")</f>
+        <v>0</v>
+      </c>
+      <c r="N19" t="s">
+        <v>106</v>
+      </c>
+      <c r="O19" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="P19">
+        <v>23340</v>
+      </c>
+      <c r="R19" s="11">
+        <f>iferror(lookup(if(Q19="",G19,Q19),{0,1,10,100,1000,2000,10000,24000,50000,100000},{0.0,0.279,0.134,0.078,0.07,0.055,0.05,0.048,0.045,0.04}),"")</f>
+        <v>0</v>
+      </c>
+      <c r="S19" s="11">
+        <f>iferror(if(Q19="",G19,Q19)*R19,"")</f>
+        <v>0</v>
+      </c>
+      <c r="T19" t="s">
+        <v>115</v>
+      </c>
+      <c r="U19" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="V19">
+        <v>1079</v>
+      </c>
+      <c r="X19" s="11">
+        <f>iferror(lookup(if(W19="",G19,W19),{0,1,10,25,50,100,250,500,1000},{0.0,0.318,0.296,0.195,0.162,0.138,0.111,0.098,0.087}),"")</f>
+        <v>0</v>
+      </c>
+      <c r="Y19" s="11">
+        <f>iferror(if(W19="",G19,W19)*X19,"")</f>
+        <v>0</v>
+      </c>
+      <c r="Z19" t="s">
+        <v>124</v>
+      </c>
+      <c r="AA19" s="12" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="20" spans="1:27">
       <c r="A20" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="B20" t="s">
-        <v>48</v>
-      </c>
-      <c r="D20" t="s">
-        <v>49</v>
+        <v>59</v>
+      </c>
+      <c r="F20" t="s">
+        <v>8</v>
       </c>
       <c r="G20">
         <f>BoardQty*1</f>
@@ -1650,16 +2031,36 @@
         <f>iferror(G20*H20,"")</f>
         <v>0</v>
       </c>
+      <c r="P20">
+        <v>149</v>
+      </c>
+      <c r="R20" s="11">
+        <f>iferror(lookup(if(Q20="",G20,Q20),{0,1,25,50,100,200,500},{0.0,1.1,1.02,0.937,0.859,0.799,0.749}),"")</f>
+        <v>0</v>
+      </c>
+      <c r="S20" s="11">
+        <f>iferror(if(Q20="",G20,Q20)*R20,"")</f>
+        <v>0</v>
+      </c>
+      <c r="T20" t="s">
+        <v>116</v>
+      </c>
+      <c r="U20" s="12" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="21" spans="1:27">
       <c r="A21" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="B21" t="s">
-        <v>51</v>
+        <v>61</v>
+      </c>
+      <c r="D21" t="s">
+        <v>62</v>
       </c>
       <c r="F21" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="G21">
         <f>BoardQty*1</f>
@@ -1674,10 +2075,10 @@
         <v>0</v>
       </c>
       <c r="J21">
-        <v>30434</v>
+        <v>956</v>
       </c>
       <c r="L21" s="11">
-        <f>iferror(lookup(if(K21="",G21,K21),{0,1,10,50,100,500,1000,3000,6000,15000},{0.0,0.71,0.592,0.531,0.4725,0.45,0.378,0.3375,0.32625,0.315}),"")</f>
+        <f>iferror(lookup(if(K21="",G21,K21),{0,1,10,100,250,500,1000},{0.0,5.03,4.493,3.6845,3.325,2.98352,2.51622}),"")</f>
         <v>0</v>
       </c>
       <c r="M21" s="11">
@@ -1685,16 +2086,16 @@
         <v>0</v>
       </c>
       <c r="N21" t="s">
-        <v>87</v>
+        <v>107</v>
       </c>
       <c r="O21" s="12" t="s">
-        <v>88</v>
+        <v>102</v>
       </c>
       <c r="P21">
-        <v>27312</v>
+        <v>328</v>
       </c>
       <c r="R21" s="11">
-        <f>iferror(lookup(if(Q21="",G21,Q21),{0,1,10,50,100,500,1500,3000,6000,9000},{0.0,0.643,0.572,0.535,0.473,0.374,0.359,0.343,0.331,0.325}),"")</f>
+        <f>iferror(lookup(if(Q21="",G21,Q21),{0,1,10,25,50,100,250,500,1000},{0.0,4.96,4.43,3.99,3.74,3.63,3.27,2.92,2.61}),"")</f>
         <v>0</v>
       </c>
       <c r="S21" s="11">
@@ -1702,16 +2103,16 @@
         <v>0</v>
       </c>
       <c r="T21" t="s">
-        <v>91</v>
+        <v>117</v>
       </c>
       <c r="U21" s="12" t="s">
-        <v>88</v>
+        <v>102</v>
       </c>
       <c r="V21">
-        <v>7896</v>
+        <v>0</v>
       </c>
       <c r="X21" s="11">
-        <f>iferror(lookup(if(W21="",G21,W21),{0,1,10,50,100,500,750,1000},{0.0,1.05,0.92,0.859,0.76,0.719,0.681,0.601}),"")</f>
+        <f>iferror(lookup(if(W21="",G21,W21),{0,1,500,1000},{0.0,3.04,3.04,2.68}),"")</f>
         <v>0</v>
       </c>
       <c r="Y21" s="11">
@@ -1719,21 +2120,24 @@
         <v>0</v>
       </c>
       <c r="Z21" t="s">
-        <v>93</v>
+        <v>125</v>
       </c>
       <c r="AA21" s="12" t="s">
-        <v>88</v>
+        <v>102</v>
       </c>
     </row>
     <row r="22" spans="1:27">
       <c r="A22" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="B22" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="D22" t="s">
-        <v>18</v>
+        <v>66</v>
+      </c>
+      <c r="F22" t="s">
+        <v>67</v>
       </c>
       <c r="G22">
         <f>BoardQty*1</f>
@@ -1750,16 +2154,19 @@
     </row>
     <row r="23" spans="1:27">
       <c r="A23" t="s">
-        <v>55</v>
+        <v>68</v>
       </c>
       <c r="B23" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="D23" t="s">
-        <v>57</v>
+        <v>20</v>
+      </c>
+      <c r="F23" t="s">
+        <v>70</v>
       </c>
       <c r="G23">
-        <f>BoardQty*2</f>
+        <f>BoardQty*1</f>
         <v>0</v>
       </c>
       <c r="H23" s="11">
@@ -1773,16 +2180,16 @@
     </row>
     <row r="24" spans="1:27">
       <c r="A24" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
       <c r="B24" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
       <c r="D24" t="s">
-        <v>60</v>
+        <v>73</v>
       </c>
       <c r="G24">
-        <f>BoardQty*1</f>
+        <f>BoardQty*2</f>
         <v>0</v>
       </c>
       <c r="H24" s="11">
@@ -1796,13 +2203,13 @@
     </row>
     <row r="25" spans="1:27">
       <c r="A25" t="s">
-        <v>61</v>
+        <v>74</v>
       </c>
       <c r="B25" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="D25" t="s">
-        <v>63</v>
+        <v>76</v>
       </c>
       <c r="G25">
         <f>BoardQty*1</f>
@@ -1819,13 +2226,16 @@
     </row>
     <row r="26" spans="1:27">
       <c r="A26" t="s">
-        <v>64</v>
+        <v>77</v>
       </c>
       <c r="B26" t="s">
-        <v>65</v>
+        <v>78</v>
       </c>
       <c r="D26" t="s">
-        <v>66</v>
+        <v>79</v>
+      </c>
+      <c r="F26" t="s">
+        <v>41</v>
       </c>
       <c r="G26">
         <f>BoardQty*1</f>
@@ -1842,19 +2252,19 @@
     </row>
     <row r="27" spans="1:27">
       <c r="A27" t="s">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="B27" t="s">
-        <v>68</v>
+        <v>81</v>
       </c>
       <c r="D27" t="s">
-        <v>69</v>
+        <v>16</v>
       </c>
       <c r="F27" t="s">
-        <v>25</v>
+        <v>82</v>
       </c>
       <c r="G27">
-        <f>BoardQty*1</f>
+        <f>BoardQty*4</f>
         <v>0</v>
       </c>
       <c r="H27" s="11">
@@ -1868,16 +2278,16 @@
     </row>
     <row r="28" spans="1:27">
       <c r="A28" t="s">
-        <v>70</v>
+        <v>83</v>
       </c>
       <c r="B28" t="s">
-        <v>71</v>
+        <v>84</v>
       </c>
       <c r="D28" t="s">
-        <v>21</v>
+        <v>85</v>
       </c>
       <c r="G28">
-        <f>BoardQty*4</f>
+        <f>BoardQty*1</f>
         <v>0</v>
       </c>
       <c r="H28" s="11">
@@ -1891,13 +2301,16 @@
     </row>
     <row r="29" spans="1:27">
       <c r="A29" t="s">
-        <v>72</v>
+        <v>86</v>
       </c>
       <c r="B29" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
       <c r="D29" t="s">
-        <v>74</v>
+        <v>88</v>
+      </c>
+      <c r="F29" t="s">
+        <v>89</v>
       </c>
       <c r="G29">
         <f>BoardQty*1</f>
@@ -1911,19 +2324,56 @@
         <f>iferror(G29*H29,"")</f>
         <v>0</v>
       </c>
+      <c r="J29">
+        <v>0</v>
+      </c>
+      <c r="L29" s="11">
+        <f>iferror(lookup(if(K29="",G29,K29),{0,1,60,120,300},{0.0,22.5085,22.5085,16.58542,12.8061}),"")</f>
+        <v>0</v>
+      </c>
+      <c r="M29" s="11">
+        <f>iferror(if(K29="",G29,K29)*L29,"")</f>
+        <v>0</v>
+      </c>
+      <c r="N29" t="s">
+        <v>108</v>
+      </c>
+      <c r="O29" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="P29">
+        <v>0</v>
+      </c>
+      <c r="R29" s="11">
+        <f>iferror(lookup(if(Q29="",G29,Q29),{0,1,100,200,500,1000,2000,5000},{0.0,1.93,1.93,1.83,1.69,1.4,1.3,1.29}),"")</f>
+        <v>0</v>
+      </c>
+      <c r="S29" s="11">
+        <f>iferror(if(Q29="",G29,Q29)*R29,"")</f>
+        <v>0</v>
+      </c>
+      <c r="T29" t="s">
+        <v>118</v>
+      </c>
+      <c r="U29" s="12" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="30" spans="1:27">
       <c r="A30" t="s">
-        <v>75</v>
+        <v>90</v>
       </c>
       <c r="B30" t="s">
-        <v>76</v>
+        <v>91</v>
       </c>
       <c r="D30" t="s">
-        <v>18</v>
+        <v>16</v>
+      </c>
+      <c r="F30" t="s">
+        <v>92</v>
       </c>
       <c r="G30">
-        <f>BoardQty*1</f>
+        <f>BoardQty*2</f>
         <v>0</v>
       </c>
       <c r="H30" s="11">
@@ -1935,976 +2385,915 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:27">
-      <c r="A31" t="s">
-        <v>77</v>
-      </c>
-      <c r="B31" t="s">
-        <v>78</v>
-      </c>
-      <c r="D31" t="s">
-        <v>21</v>
-      </c>
-      <c r="G31">
-        <f>BoardQty*2</f>
-        <v>0</v>
-      </c>
-      <c r="H31" s="11">
-        <f>MINA(INDIRECT(ADDRESS(ROW(),COLUMN(newark_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(digikey_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(mouser_part_data)+2)))</f>
-        <v>0</v>
-      </c>
-      <c r="I31" s="11">
-        <f>iferror(G31*H31,"")</f>
+    <row r="32" spans="1:27">
+      <c r="K32">
+        <f t="array" ref="K32">IFERROR(CONCATENATE(TEXT(INDEX($K$7:$K$30,SMALL(IF($N$7:$N$30&lt;&gt;"",IF($K$7:$K$30&lt;&gt;"",ROW($K$7:$K$30)-MIN(ROW($K$7:$K$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0"),","),"")</f>
+        <v>0</v>
+      </c>
+      <c r="L32">
+        <f t="array" ref="L32">IFERROR(CONCATENATE((INDEX($N$7:$N$30,SMALL(IF($N$7:$N$30&lt;&gt;"",IF($K$7:$K$30&lt;&gt;"",ROW($K$7:$K$30)-MIN(ROW($K$7:$K$30))+1,""),""),ROW()-ROW(A$32)+1))),","),"")</f>
+        <v>0</v>
+      </c>
+      <c r="M32">
+        <f t="array" ref="M32">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($N$7:$N$30&lt;&gt;"",IF($K$7:$K$30&lt;&gt;"",ROW($K$7:$K$30)-MIN(ROW($K$7:$K$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
+        <v>0</v>
+      </c>
+      <c r="Q32">
+        <f t="array" ref="Q32">IFERROR(CONCATENATE((INDEX($T$7:$T$30,SMALL(IF($T$7:$T$30&lt;&gt;"",IF($Q$7:$Q$30&lt;&gt;"",ROW($Q$7:$Q$30)-MIN(ROW($Q$7:$Q$30))+1,""),""),ROW()-ROW(A$32)+1)))," "),"")</f>
+        <v>0</v>
+      </c>
+      <c r="R32">
+        <f t="array" ref="R32">IFERROR(CONCATENATE(TEXT(INDEX($Q$7:$Q$30,SMALL(IF($T$7:$T$30&lt;&gt;"",IF($Q$7:$Q$30&lt;&gt;"",ROW($Q$7:$Q$30)-MIN(ROW($Q$7:$Q$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0")," "),"")</f>
+        <v>0</v>
+      </c>
+      <c r="S32">
+        <f t="array" ref="S32">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($T$7:$T$30&lt;&gt;"",IF($Q$7:$Q$30&lt;&gt;"",ROW($Q$7:$Q$30)-MIN(ROW($Q$7:$Q$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
+        <v>0</v>
+      </c>
+      <c r="W32">
+        <f t="array" ref="W32">IFERROR(CONCATENATE((INDEX($Z$7:$Z$30,SMALL(IF($Z$7:$Z$30&lt;&gt;"",IF($W$7:$W$30&lt;&gt;"",ROW($W$7:$W$30)-MIN(ROW($W$7:$W$30))+1,""),""),ROW()-ROW(A$32)+1))),","),"")</f>
+        <v>0</v>
+      </c>
+      <c r="X32">
+        <f t="array" ref="X32">IFERROR(CONCATENATE(TEXT(INDEX($W$7:$W$30,SMALL(IF($Z$7:$Z$30&lt;&gt;"",IF($W$7:$W$30&lt;&gt;"",ROW($W$7:$W$30)-MIN(ROW($W$7:$W$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0"),","),"")</f>
+        <v>0</v>
+      </c>
+      <c r="Y32">
+        <f t="array" ref="Y32">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($Z$7:$Z$30&lt;&gt;"",IF($W$7:$W$30&lt;&gt;"",ROW($W$7:$W$30)-MIN(ROW($W$7:$W$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="33" spans="11:25">
       <c r="K33">
-        <f t="array" ref="K33">IFERROR(CONCATENATE(TEXT(INDEX($K$7:$K$31,SMALL(IF($N$7:$N$31&lt;&gt;"",IF($K$7:$K$31&lt;&gt;"",ROW($K$7:$K$31)-MIN(ROW($K$7:$K$31))+1,""),""),ROW()-ROW(A$33)+1)),"##0"),","),"")</f>
+        <f t="array" ref="K33">IFERROR(CONCATENATE(TEXT(INDEX($K$7:$K$30,SMALL(IF($N$7:$N$30&lt;&gt;"",IF($K$7:$K$30&lt;&gt;"",ROW($K$7:$K$30)-MIN(ROW($K$7:$K$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0"),","),"")</f>
         <v>0</v>
       </c>
       <c r="L33">
-        <f t="array" ref="L33">IFERROR(CONCATENATE((INDEX($N$7:$N$31,SMALL(IF($N$7:$N$31&lt;&gt;"",IF($K$7:$K$31&lt;&gt;"",ROW($K$7:$K$31)-MIN(ROW($K$7:$K$31))+1,""),""),ROW()-ROW(A$33)+1))),","),"")</f>
+        <f t="array" ref="L33">IFERROR(CONCATENATE((INDEX($N$7:$N$30,SMALL(IF($N$7:$N$30&lt;&gt;"",IF($K$7:$K$30&lt;&gt;"",ROW($K$7:$K$30)-MIN(ROW($K$7:$K$30))+1,""),""),ROW()-ROW(A$32)+1))),","),"")</f>
         <v>0</v>
       </c>
       <c r="M33">
-        <f t="array" ref="M33">IFERROR(CONCATENATE((INDEX($A$7:$A$31,SMALL(IF($N$7:$N$31&lt;&gt;"",IF($K$7:$K$31&lt;&gt;"",ROW($K$7:$K$31)-MIN(ROW($K$7:$K$31))+1,""),""),ROW()-ROW(A$33)+1))),),"")</f>
+        <f t="array" ref="M33">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($N$7:$N$30&lt;&gt;"",IF($K$7:$K$30&lt;&gt;"",ROW($K$7:$K$30)-MIN(ROW($K$7:$K$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
         <v>0</v>
       </c>
       <c r="Q33">
-        <f t="array" ref="Q33">IFERROR(CONCATENATE((INDEX($T$7:$T$31,SMALL(IF($T$7:$T$31&lt;&gt;"",IF($Q$7:$Q$31&lt;&gt;"",ROW($Q$7:$Q$31)-MIN(ROW($Q$7:$Q$31))+1,""),""),ROW()-ROW(A$33)+1)))," "),"")</f>
+        <f t="array" ref="Q33">IFERROR(CONCATENATE((INDEX($T$7:$T$30,SMALL(IF($T$7:$T$30&lt;&gt;"",IF($Q$7:$Q$30&lt;&gt;"",ROW($Q$7:$Q$30)-MIN(ROW($Q$7:$Q$30))+1,""),""),ROW()-ROW(A$32)+1)))," "),"")</f>
         <v>0</v>
       </c>
       <c r="R33">
-        <f t="array" ref="R33">IFERROR(CONCATENATE(TEXT(INDEX($Q$7:$Q$31,SMALL(IF($T$7:$T$31&lt;&gt;"",IF($Q$7:$Q$31&lt;&gt;"",ROW($Q$7:$Q$31)-MIN(ROW($Q$7:$Q$31))+1,""),""),ROW()-ROW(A$33)+1)),"##0")," "),"")</f>
+        <f t="array" ref="R33">IFERROR(CONCATENATE(TEXT(INDEX($Q$7:$Q$30,SMALL(IF($T$7:$T$30&lt;&gt;"",IF($Q$7:$Q$30&lt;&gt;"",ROW($Q$7:$Q$30)-MIN(ROW($Q$7:$Q$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0")," "),"")</f>
         <v>0</v>
       </c>
       <c r="S33">
-        <f t="array" ref="S33">IFERROR(CONCATENATE((INDEX($A$7:$A$31,SMALL(IF($T$7:$T$31&lt;&gt;"",IF($Q$7:$Q$31&lt;&gt;"",ROW($Q$7:$Q$31)-MIN(ROW($Q$7:$Q$31))+1,""),""),ROW()-ROW(A$33)+1))),),"")</f>
+        <f t="array" ref="S33">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($T$7:$T$30&lt;&gt;"",IF($Q$7:$Q$30&lt;&gt;"",ROW($Q$7:$Q$30)-MIN(ROW($Q$7:$Q$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
         <v>0</v>
       </c>
       <c r="W33">
-        <f t="array" ref="W33">IFERROR(CONCATENATE((INDEX($Z$7:$Z$31,SMALL(IF($Z$7:$Z$31&lt;&gt;"",IF($W$7:$W$31&lt;&gt;"",ROW($W$7:$W$31)-MIN(ROW($W$7:$W$31))+1,""),""),ROW()-ROW(A$33)+1))),","),"")</f>
+        <f t="array" ref="W33">IFERROR(CONCATENATE((INDEX($Z$7:$Z$30,SMALL(IF($Z$7:$Z$30&lt;&gt;"",IF($W$7:$W$30&lt;&gt;"",ROW($W$7:$W$30)-MIN(ROW($W$7:$W$30))+1,""),""),ROW()-ROW(A$32)+1))),","),"")</f>
         <v>0</v>
       </c>
       <c r="X33">
-        <f t="array" ref="X33">IFERROR(CONCATENATE(TEXT(INDEX($W$7:$W$31,SMALL(IF($Z$7:$Z$31&lt;&gt;"",IF($W$7:$W$31&lt;&gt;"",ROW($W$7:$W$31)-MIN(ROW($W$7:$W$31))+1,""),""),ROW()-ROW(A$33)+1)),"##0"),","),"")</f>
+        <f t="array" ref="X33">IFERROR(CONCATENATE(TEXT(INDEX($W$7:$W$30,SMALL(IF($Z$7:$Z$30&lt;&gt;"",IF($W$7:$W$30&lt;&gt;"",ROW($W$7:$W$30)-MIN(ROW($W$7:$W$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0"),","),"")</f>
         <v>0</v>
       </c>
       <c r="Y33">
-        <f t="array" ref="Y33">IFERROR(CONCATENATE((INDEX($A$7:$A$31,SMALL(IF($Z$7:$Z$31&lt;&gt;"",IF($W$7:$W$31&lt;&gt;"",ROW($W$7:$W$31)-MIN(ROW($W$7:$W$31))+1,""),""),ROW()-ROW(A$33)+1))),),"")</f>
+        <f t="array" ref="Y33">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($Z$7:$Z$30&lt;&gt;"",IF($W$7:$W$30&lt;&gt;"",ROW($W$7:$W$30)-MIN(ROW($W$7:$W$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="34" spans="11:25">
       <c r="K34">
-        <f t="array" ref="K34">IFERROR(CONCATENATE(TEXT(INDEX($K$7:$K$31,SMALL(IF($N$7:$N$31&lt;&gt;"",IF($K$7:$K$31&lt;&gt;"",ROW($K$7:$K$31)-MIN(ROW($K$7:$K$31))+1,""),""),ROW()-ROW(A$33)+1)),"##0"),","),"")</f>
+        <f t="array" ref="K34">IFERROR(CONCATENATE(TEXT(INDEX($K$7:$K$30,SMALL(IF($N$7:$N$30&lt;&gt;"",IF($K$7:$K$30&lt;&gt;"",ROW($K$7:$K$30)-MIN(ROW($K$7:$K$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0"),","),"")</f>
         <v>0</v>
       </c>
       <c r="L34">
-        <f t="array" ref="L34">IFERROR(CONCATENATE((INDEX($N$7:$N$31,SMALL(IF($N$7:$N$31&lt;&gt;"",IF($K$7:$K$31&lt;&gt;"",ROW($K$7:$K$31)-MIN(ROW($K$7:$K$31))+1,""),""),ROW()-ROW(A$33)+1))),","),"")</f>
+        <f t="array" ref="L34">IFERROR(CONCATENATE((INDEX($N$7:$N$30,SMALL(IF($N$7:$N$30&lt;&gt;"",IF($K$7:$K$30&lt;&gt;"",ROW($K$7:$K$30)-MIN(ROW($K$7:$K$30))+1,""),""),ROW()-ROW(A$32)+1))),","),"")</f>
         <v>0</v>
       </c>
       <c r="M34">
-        <f t="array" ref="M34">IFERROR(CONCATENATE((INDEX($A$7:$A$31,SMALL(IF($N$7:$N$31&lt;&gt;"",IF($K$7:$K$31&lt;&gt;"",ROW($K$7:$K$31)-MIN(ROW($K$7:$K$31))+1,""),""),ROW()-ROW(A$33)+1))),),"")</f>
+        <f t="array" ref="M34">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($N$7:$N$30&lt;&gt;"",IF($K$7:$K$30&lt;&gt;"",ROW($K$7:$K$30)-MIN(ROW($K$7:$K$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
         <v>0</v>
       </c>
       <c r="Q34">
-        <f t="array" ref="Q34">IFERROR(CONCATENATE((INDEX($T$7:$T$31,SMALL(IF($T$7:$T$31&lt;&gt;"",IF($Q$7:$Q$31&lt;&gt;"",ROW($Q$7:$Q$31)-MIN(ROW($Q$7:$Q$31))+1,""),""),ROW()-ROW(A$33)+1)))," "),"")</f>
+        <f t="array" ref="Q34">IFERROR(CONCATENATE((INDEX($T$7:$T$30,SMALL(IF($T$7:$T$30&lt;&gt;"",IF($Q$7:$Q$30&lt;&gt;"",ROW($Q$7:$Q$30)-MIN(ROW($Q$7:$Q$30))+1,""),""),ROW()-ROW(A$32)+1)))," "),"")</f>
         <v>0</v>
       </c>
       <c r="R34">
-        <f t="array" ref="R34">IFERROR(CONCATENATE(TEXT(INDEX($Q$7:$Q$31,SMALL(IF($T$7:$T$31&lt;&gt;"",IF($Q$7:$Q$31&lt;&gt;"",ROW($Q$7:$Q$31)-MIN(ROW($Q$7:$Q$31))+1,""),""),ROW()-ROW(A$33)+1)),"##0")," "),"")</f>
+        <f t="array" ref="R34">IFERROR(CONCATENATE(TEXT(INDEX($Q$7:$Q$30,SMALL(IF($T$7:$T$30&lt;&gt;"",IF($Q$7:$Q$30&lt;&gt;"",ROW($Q$7:$Q$30)-MIN(ROW($Q$7:$Q$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0")," "),"")</f>
         <v>0</v>
       </c>
       <c r="S34">
-        <f t="array" ref="S34">IFERROR(CONCATENATE((INDEX($A$7:$A$31,SMALL(IF($T$7:$T$31&lt;&gt;"",IF($Q$7:$Q$31&lt;&gt;"",ROW($Q$7:$Q$31)-MIN(ROW($Q$7:$Q$31))+1,""),""),ROW()-ROW(A$33)+1))),),"")</f>
+        <f t="array" ref="S34">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($T$7:$T$30&lt;&gt;"",IF($Q$7:$Q$30&lt;&gt;"",ROW($Q$7:$Q$30)-MIN(ROW($Q$7:$Q$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
         <v>0</v>
       </c>
       <c r="W34">
-        <f t="array" ref="W34">IFERROR(CONCATENATE((INDEX($Z$7:$Z$31,SMALL(IF($Z$7:$Z$31&lt;&gt;"",IF($W$7:$W$31&lt;&gt;"",ROW($W$7:$W$31)-MIN(ROW($W$7:$W$31))+1,""),""),ROW()-ROW(A$33)+1))),","),"")</f>
+        <f t="array" ref="W34">IFERROR(CONCATENATE((INDEX($Z$7:$Z$30,SMALL(IF($Z$7:$Z$30&lt;&gt;"",IF($W$7:$W$30&lt;&gt;"",ROW($W$7:$W$30)-MIN(ROW($W$7:$W$30))+1,""),""),ROW()-ROW(A$32)+1))),","),"")</f>
         <v>0</v>
       </c>
       <c r="X34">
-        <f t="array" ref="X34">IFERROR(CONCATENATE(TEXT(INDEX($W$7:$W$31,SMALL(IF($Z$7:$Z$31&lt;&gt;"",IF($W$7:$W$31&lt;&gt;"",ROW($W$7:$W$31)-MIN(ROW($W$7:$W$31))+1,""),""),ROW()-ROW(A$33)+1)),"##0"),","),"")</f>
+        <f t="array" ref="X34">IFERROR(CONCATENATE(TEXT(INDEX($W$7:$W$30,SMALL(IF($Z$7:$Z$30&lt;&gt;"",IF($W$7:$W$30&lt;&gt;"",ROW($W$7:$W$30)-MIN(ROW($W$7:$W$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0"),","),"")</f>
         <v>0</v>
       </c>
       <c r="Y34">
-        <f t="array" ref="Y34">IFERROR(CONCATENATE((INDEX($A$7:$A$31,SMALL(IF($Z$7:$Z$31&lt;&gt;"",IF($W$7:$W$31&lt;&gt;"",ROW($W$7:$W$31)-MIN(ROW($W$7:$W$31))+1,""),""),ROW()-ROW(A$33)+1))),),"")</f>
+        <f t="array" ref="Y34">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($Z$7:$Z$30&lt;&gt;"",IF($W$7:$W$30&lt;&gt;"",ROW($W$7:$W$30)-MIN(ROW($W$7:$W$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="35" spans="11:25">
       <c r="K35">
-        <f t="array" ref="K35">IFERROR(CONCATENATE(TEXT(INDEX($K$7:$K$31,SMALL(IF($N$7:$N$31&lt;&gt;"",IF($K$7:$K$31&lt;&gt;"",ROW($K$7:$K$31)-MIN(ROW($K$7:$K$31))+1,""),""),ROW()-ROW(A$33)+1)),"##0"),","),"")</f>
+        <f t="array" ref="K35">IFERROR(CONCATENATE(TEXT(INDEX($K$7:$K$30,SMALL(IF($N$7:$N$30&lt;&gt;"",IF($K$7:$K$30&lt;&gt;"",ROW($K$7:$K$30)-MIN(ROW($K$7:$K$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0"),","),"")</f>
         <v>0</v>
       </c>
       <c r="L35">
-        <f t="array" ref="L35">IFERROR(CONCATENATE((INDEX($N$7:$N$31,SMALL(IF($N$7:$N$31&lt;&gt;"",IF($K$7:$K$31&lt;&gt;"",ROW($K$7:$K$31)-MIN(ROW($K$7:$K$31))+1,""),""),ROW()-ROW(A$33)+1))),","),"")</f>
+        <f t="array" ref="L35">IFERROR(CONCATENATE((INDEX($N$7:$N$30,SMALL(IF($N$7:$N$30&lt;&gt;"",IF($K$7:$K$30&lt;&gt;"",ROW($K$7:$K$30)-MIN(ROW($K$7:$K$30))+1,""),""),ROW()-ROW(A$32)+1))),","),"")</f>
         <v>0</v>
       </c>
       <c r="M35">
-        <f t="array" ref="M35">IFERROR(CONCATENATE((INDEX($A$7:$A$31,SMALL(IF($N$7:$N$31&lt;&gt;"",IF($K$7:$K$31&lt;&gt;"",ROW($K$7:$K$31)-MIN(ROW($K$7:$K$31))+1,""),""),ROW()-ROW(A$33)+1))),),"")</f>
+        <f t="array" ref="M35">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($N$7:$N$30&lt;&gt;"",IF($K$7:$K$30&lt;&gt;"",ROW($K$7:$K$30)-MIN(ROW($K$7:$K$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
         <v>0</v>
       </c>
       <c r="Q35">
-        <f t="array" ref="Q35">IFERROR(CONCATENATE((INDEX($T$7:$T$31,SMALL(IF($T$7:$T$31&lt;&gt;"",IF($Q$7:$Q$31&lt;&gt;"",ROW($Q$7:$Q$31)-MIN(ROW($Q$7:$Q$31))+1,""),""),ROW()-ROW(A$33)+1)))," "),"")</f>
+        <f t="array" ref="Q35">IFERROR(CONCATENATE((INDEX($T$7:$T$30,SMALL(IF($T$7:$T$30&lt;&gt;"",IF($Q$7:$Q$30&lt;&gt;"",ROW($Q$7:$Q$30)-MIN(ROW($Q$7:$Q$30))+1,""),""),ROW()-ROW(A$32)+1)))," "),"")</f>
         <v>0</v>
       </c>
       <c r="R35">
-        <f t="array" ref="R35">IFERROR(CONCATENATE(TEXT(INDEX($Q$7:$Q$31,SMALL(IF($T$7:$T$31&lt;&gt;"",IF($Q$7:$Q$31&lt;&gt;"",ROW($Q$7:$Q$31)-MIN(ROW($Q$7:$Q$31))+1,""),""),ROW()-ROW(A$33)+1)),"##0")," "),"")</f>
+        <f t="array" ref="R35">IFERROR(CONCATENATE(TEXT(INDEX($Q$7:$Q$30,SMALL(IF($T$7:$T$30&lt;&gt;"",IF($Q$7:$Q$30&lt;&gt;"",ROW($Q$7:$Q$30)-MIN(ROW($Q$7:$Q$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0")," "),"")</f>
         <v>0</v>
       </c>
       <c r="S35">
-        <f t="array" ref="S35">IFERROR(CONCATENATE((INDEX($A$7:$A$31,SMALL(IF($T$7:$T$31&lt;&gt;"",IF($Q$7:$Q$31&lt;&gt;"",ROW($Q$7:$Q$31)-MIN(ROW($Q$7:$Q$31))+1,""),""),ROW()-ROW(A$33)+1))),),"")</f>
+        <f t="array" ref="S35">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($T$7:$T$30&lt;&gt;"",IF($Q$7:$Q$30&lt;&gt;"",ROW($Q$7:$Q$30)-MIN(ROW($Q$7:$Q$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
         <v>0</v>
       </c>
       <c r="W35">
-        <f t="array" ref="W35">IFERROR(CONCATENATE((INDEX($Z$7:$Z$31,SMALL(IF($Z$7:$Z$31&lt;&gt;"",IF($W$7:$W$31&lt;&gt;"",ROW($W$7:$W$31)-MIN(ROW($W$7:$W$31))+1,""),""),ROW()-ROW(A$33)+1))),","),"")</f>
+        <f t="array" ref="W35">IFERROR(CONCATENATE((INDEX($Z$7:$Z$30,SMALL(IF($Z$7:$Z$30&lt;&gt;"",IF($W$7:$W$30&lt;&gt;"",ROW($W$7:$W$30)-MIN(ROW($W$7:$W$30))+1,""),""),ROW()-ROW(A$32)+1))),","),"")</f>
         <v>0</v>
       </c>
       <c r="X35">
-        <f t="array" ref="X35">IFERROR(CONCATENATE(TEXT(INDEX($W$7:$W$31,SMALL(IF($Z$7:$Z$31&lt;&gt;"",IF($W$7:$W$31&lt;&gt;"",ROW($W$7:$W$31)-MIN(ROW($W$7:$W$31))+1,""),""),ROW()-ROW(A$33)+1)),"##0"),","),"")</f>
+        <f t="array" ref="X35">IFERROR(CONCATENATE(TEXT(INDEX($W$7:$W$30,SMALL(IF($Z$7:$Z$30&lt;&gt;"",IF($W$7:$W$30&lt;&gt;"",ROW($W$7:$W$30)-MIN(ROW($W$7:$W$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0"),","),"")</f>
         <v>0</v>
       </c>
       <c r="Y35">
-        <f t="array" ref="Y35">IFERROR(CONCATENATE((INDEX($A$7:$A$31,SMALL(IF($Z$7:$Z$31&lt;&gt;"",IF($W$7:$W$31&lt;&gt;"",ROW($W$7:$W$31)-MIN(ROW($W$7:$W$31))+1,""),""),ROW()-ROW(A$33)+1))),),"")</f>
+        <f t="array" ref="Y35">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($Z$7:$Z$30&lt;&gt;"",IF($W$7:$W$30&lt;&gt;"",ROW($W$7:$W$30)-MIN(ROW($W$7:$W$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="36" spans="11:25">
       <c r="K36">
-        <f t="array" ref="K36">IFERROR(CONCATENATE(TEXT(INDEX($K$7:$K$31,SMALL(IF($N$7:$N$31&lt;&gt;"",IF($K$7:$K$31&lt;&gt;"",ROW($K$7:$K$31)-MIN(ROW($K$7:$K$31))+1,""),""),ROW()-ROW(A$33)+1)),"##0"),","),"")</f>
+        <f t="array" ref="K36">IFERROR(CONCATENATE(TEXT(INDEX($K$7:$K$30,SMALL(IF($N$7:$N$30&lt;&gt;"",IF($K$7:$K$30&lt;&gt;"",ROW($K$7:$K$30)-MIN(ROW($K$7:$K$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0"),","),"")</f>
         <v>0</v>
       </c>
       <c r="L36">
-        <f t="array" ref="L36">IFERROR(CONCATENATE((INDEX($N$7:$N$31,SMALL(IF($N$7:$N$31&lt;&gt;"",IF($K$7:$K$31&lt;&gt;"",ROW($K$7:$K$31)-MIN(ROW($K$7:$K$31))+1,""),""),ROW()-ROW(A$33)+1))),","),"")</f>
+        <f t="array" ref="L36">IFERROR(CONCATENATE((INDEX($N$7:$N$30,SMALL(IF($N$7:$N$30&lt;&gt;"",IF($K$7:$K$30&lt;&gt;"",ROW($K$7:$K$30)-MIN(ROW($K$7:$K$30))+1,""),""),ROW()-ROW(A$32)+1))),","),"")</f>
         <v>0</v>
       </c>
       <c r="M36">
-        <f t="array" ref="M36">IFERROR(CONCATENATE((INDEX($A$7:$A$31,SMALL(IF($N$7:$N$31&lt;&gt;"",IF($K$7:$K$31&lt;&gt;"",ROW($K$7:$K$31)-MIN(ROW($K$7:$K$31))+1,""),""),ROW()-ROW(A$33)+1))),),"")</f>
+        <f t="array" ref="M36">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($N$7:$N$30&lt;&gt;"",IF($K$7:$K$30&lt;&gt;"",ROW($K$7:$K$30)-MIN(ROW($K$7:$K$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
         <v>0</v>
       </c>
       <c r="Q36">
-        <f t="array" ref="Q36">IFERROR(CONCATENATE((INDEX($T$7:$T$31,SMALL(IF($T$7:$T$31&lt;&gt;"",IF($Q$7:$Q$31&lt;&gt;"",ROW($Q$7:$Q$31)-MIN(ROW($Q$7:$Q$31))+1,""),""),ROW()-ROW(A$33)+1)))," "),"")</f>
+        <f t="array" ref="Q36">IFERROR(CONCATENATE((INDEX($T$7:$T$30,SMALL(IF($T$7:$T$30&lt;&gt;"",IF($Q$7:$Q$30&lt;&gt;"",ROW($Q$7:$Q$30)-MIN(ROW($Q$7:$Q$30))+1,""),""),ROW()-ROW(A$32)+1)))," "),"")</f>
         <v>0</v>
       </c>
       <c r="R36">
-        <f t="array" ref="R36">IFERROR(CONCATENATE(TEXT(INDEX($Q$7:$Q$31,SMALL(IF($T$7:$T$31&lt;&gt;"",IF($Q$7:$Q$31&lt;&gt;"",ROW($Q$7:$Q$31)-MIN(ROW($Q$7:$Q$31))+1,""),""),ROW()-ROW(A$33)+1)),"##0")," "),"")</f>
+        <f t="array" ref="R36">IFERROR(CONCATENATE(TEXT(INDEX($Q$7:$Q$30,SMALL(IF($T$7:$T$30&lt;&gt;"",IF($Q$7:$Q$30&lt;&gt;"",ROW($Q$7:$Q$30)-MIN(ROW($Q$7:$Q$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0")," "),"")</f>
         <v>0</v>
       </c>
       <c r="S36">
-        <f t="array" ref="S36">IFERROR(CONCATENATE((INDEX($A$7:$A$31,SMALL(IF($T$7:$T$31&lt;&gt;"",IF($Q$7:$Q$31&lt;&gt;"",ROW($Q$7:$Q$31)-MIN(ROW($Q$7:$Q$31))+1,""),""),ROW()-ROW(A$33)+1))),),"")</f>
+        <f t="array" ref="S36">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($T$7:$T$30&lt;&gt;"",IF($Q$7:$Q$30&lt;&gt;"",ROW($Q$7:$Q$30)-MIN(ROW($Q$7:$Q$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
         <v>0</v>
       </c>
       <c r="W36">
-        <f t="array" ref="W36">IFERROR(CONCATENATE((INDEX($Z$7:$Z$31,SMALL(IF($Z$7:$Z$31&lt;&gt;"",IF($W$7:$W$31&lt;&gt;"",ROW($W$7:$W$31)-MIN(ROW($W$7:$W$31))+1,""),""),ROW()-ROW(A$33)+1))),","),"")</f>
+        <f t="array" ref="W36">IFERROR(CONCATENATE((INDEX($Z$7:$Z$30,SMALL(IF($Z$7:$Z$30&lt;&gt;"",IF($W$7:$W$30&lt;&gt;"",ROW($W$7:$W$30)-MIN(ROW($W$7:$W$30))+1,""),""),ROW()-ROW(A$32)+1))),","),"")</f>
         <v>0</v>
       </c>
       <c r="X36">
-        <f t="array" ref="X36">IFERROR(CONCATENATE(TEXT(INDEX($W$7:$W$31,SMALL(IF($Z$7:$Z$31&lt;&gt;"",IF($W$7:$W$31&lt;&gt;"",ROW($W$7:$W$31)-MIN(ROW($W$7:$W$31))+1,""),""),ROW()-ROW(A$33)+1)),"##0"),","),"")</f>
+        <f t="array" ref="X36">IFERROR(CONCATENATE(TEXT(INDEX($W$7:$W$30,SMALL(IF($Z$7:$Z$30&lt;&gt;"",IF($W$7:$W$30&lt;&gt;"",ROW($W$7:$W$30)-MIN(ROW($W$7:$W$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0"),","),"")</f>
         <v>0</v>
       </c>
       <c r="Y36">
-        <f t="array" ref="Y36">IFERROR(CONCATENATE((INDEX($A$7:$A$31,SMALL(IF($Z$7:$Z$31&lt;&gt;"",IF($W$7:$W$31&lt;&gt;"",ROW($W$7:$W$31)-MIN(ROW($W$7:$W$31))+1,""),""),ROW()-ROW(A$33)+1))),),"")</f>
+        <f t="array" ref="Y36">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($Z$7:$Z$30&lt;&gt;"",IF($W$7:$W$30&lt;&gt;"",ROW($W$7:$W$30)-MIN(ROW($W$7:$W$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="37" spans="11:25">
       <c r="K37">
-        <f t="array" ref="K37">IFERROR(CONCATENATE(TEXT(INDEX($K$7:$K$31,SMALL(IF($N$7:$N$31&lt;&gt;"",IF($K$7:$K$31&lt;&gt;"",ROW($K$7:$K$31)-MIN(ROW($K$7:$K$31))+1,""),""),ROW()-ROW(A$33)+1)),"##0"),","),"")</f>
+        <f t="array" ref="K37">IFERROR(CONCATENATE(TEXT(INDEX($K$7:$K$30,SMALL(IF($N$7:$N$30&lt;&gt;"",IF($K$7:$K$30&lt;&gt;"",ROW($K$7:$K$30)-MIN(ROW($K$7:$K$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0"),","),"")</f>
         <v>0</v>
       </c>
       <c r="L37">
-        <f t="array" ref="L37">IFERROR(CONCATENATE((INDEX($N$7:$N$31,SMALL(IF($N$7:$N$31&lt;&gt;"",IF($K$7:$K$31&lt;&gt;"",ROW($K$7:$K$31)-MIN(ROW($K$7:$K$31))+1,""),""),ROW()-ROW(A$33)+1))),","),"")</f>
+        <f t="array" ref="L37">IFERROR(CONCATENATE((INDEX($N$7:$N$30,SMALL(IF($N$7:$N$30&lt;&gt;"",IF($K$7:$K$30&lt;&gt;"",ROW($K$7:$K$30)-MIN(ROW($K$7:$K$30))+1,""),""),ROW()-ROW(A$32)+1))),","),"")</f>
         <v>0</v>
       </c>
       <c r="M37">
-        <f t="array" ref="M37">IFERROR(CONCATENATE((INDEX($A$7:$A$31,SMALL(IF($N$7:$N$31&lt;&gt;"",IF($K$7:$K$31&lt;&gt;"",ROW($K$7:$K$31)-MIN(ROW($K$7:$K$31))+1,""),""),ROW()-ROW(A$33)+1))),),"")</f>
+        <f t="array" ref="M37">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($N$7:$N$30&lt;&gt;"",IF($K$7:$K$30&lt;&gt;"",ROW($K$7:$K$30)-MIN(ROW($K$7:$K$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
         <v>0</v>
       </c>
       <c r="Q37">
-        <f t="array" ref="Q37">IFERROR(CONCATENATE((INDEX($T$7:$T$31,SMALL(IF($T$7:$T$31&lt;&gt;"",IF($Q$7:$Q$31&lt;&gt;"",ROW($Q$7:$Q$31)-MIN(ROW($Q$7:$Q$31))+1,""),""),ROW()-ROW(A$33)+1)))," "),"")</f>
+        <f t="array" ref="Q37">IFERROR(CONCATENATE((INDEX($T$7:$T$30,SMALL(IF($T$7:$T$30&lt;&gt;"",IF($Q$7:$Q$30&lt;&gt;"",ROW($Q$7:$Q$30)-MIN(ROW($Q$7:$Q$30))+1,""),""),ROW()-ROW(A$32)+1)))," "),"")</f>
         <v>0</v>
       </c>
       <c r="R37">
-        <f t="array" ref="R37">IFERROR(CONCATENATE(TEXT(INDEX($Q$7:$Q$31,SMALL(IF($T$7:$T$31&lt;&gt;"",IF($Q$7:$Q$31&lt;&gt;"",ROW($Q$7:$Q$31)-MIN(ROW($Q$7:$Q$31))+1,""),""),ROW()-ROW(A$33)+1)),"##0")," "),"")</f>
+        <f t="array" ref="R37">IFERROR(CONCATENATE(TEXT(INDEX($Q$7:$Q$30,SMALL(IF($T$7:$T$30&lt;&gt;"",IF($Q$7:$Q$30&lt;&gt;"",ROW($Q$7:$Q$30)-MIN(ROW($Q$7:$Q$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0")," "),"")</f>
         <v>0</v>
       </c>
       <c r="S37">
-        <f t="array" ref="S37">IFERROR(CONCATENATE((INDEX($A$7:$A$31,SMALL(IF($T$7:$T$31&lt;&gt;"",IF($Q$7:$Q$31&lt;&gt;"",ROW($Q$7:$Q$31)-MIN(ROW($Q$7:$Q$31))+1,""),""),ROW()-ROW(A$33)+1))),),"")</f>
+        <f t="array" ref="S37">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($T$7:$T$30&lt;&gt;"",IF($Q$7:$Q$30&lt;&gt;"",ROW($Q$7:$Q$30)-MIN(ROW($Q$7:$Q$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
         <v>0</v>
       </c>
       <c r="W37">
-        <f t="array" ref="W37">IFERROR(CONCATENATE((INDEX($Z$7:$Z$31,SMALL(IF($Z$7:$Z$31&lt;&gt;"",IF($W$7:$W$31&lt;&gt;"",ROW($W$7:$W$31)-MIN(ROW($W$7:$W$31))+1,""),""),ROW()-ROW(A$33)+1))),","),"")</f>
+        <f t="array" ref="W37">IFERROR(CONCATENATE((INDEX($Z$7:$Z$30,SMALL(IF($Z$7:$Z$30&lt;&gt;"",IF($W$7:$W$30&lt;&gt;"",ROW($W$7:$W$30)-MIN(ROW($W$7:$W$30))+1,""),""),ROW()-ROW(A$32)+1))),","),"")</f>
         <v>0</v>
       </c>
       <c r="X37">
-        <f t="array" ref="X37">IFERROR(CONCATENATE(TEXT(INDEX($W$7:$W$31,SMALL(IF($Z$7:$Z$31&lt;&gt;"",IF($W$7:$W$31&lt;&gt;"",ROW($W$7:$W$31)-MIN(ROW($W$7:$W$31))+1,""),""),ROW()-ROW(A$33)+1)),"##0"),","),"")</f>
+        <f t="array" ref="X37">IFERROR(CONCATENATE(TEXT(INDEX($W$7:$W$30,SMALL(IF($Z$7:$Z$30&lt;&gt;"",IF($W$7:$W$30&lt;&gt;"",ROW($W$7:$W$30)-MIN(ROW($W$7:$W$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0"),","),"")</f>
         <v>0</v>
       </c>
       <c r="Y37">
-        <f t="array" ref="Y37">IFERROR(CONCATENATE((INDEX($A$7:$A$31,SMALL(IF($Z$7:$Z$31&lt;&gt;"",IF($W$7:$W$31&lt;&gt;"",ROW($W$7:$W$31)-MIN(ROW($W$7:$W$31))+1,""),""),ROW()-ROW(A$33)+1))),),"")</f>
+        <f t="array" ref="Y37">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($Z$7:$Z$30&lt;&gt;"",IF($W$7:$W$30&lt;&gt;"",ROW($W$7:$W$30)-MIN(ROW($W$7:$W$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="38" spans="11:25">
       <c r="K38">
-        <f t="array" ref="K38">IFERROR(CONCATENATE(TEXT(INDEX($K$7:$K$31,SMALL(IF($N$7:$N$31&lt;&gt;"",IF($K$7:$K$31&lt;&gt;"",ROW($K$7:$K$31)-MIN(ROW($K$7:$K$31))+1,""),""),ROW()-ROW(A$33)+1)),"##0"),","),"")</f>
+        <f t="array" ref="K38">IFERROR(CONCATENATE(TEXT(INDEX($K$7:$K$30,SMALL(IF($N$7:$N$30&lt;&gt;"",IF($K$7:$K$30&lt;&gt;"",ROW($K$7:$K$30)-MIN(ROW($K$7:$K$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0"),","),"")</f>
         <v>0</v>
       </c>
       <c r="L38">
-        <f t="array" ref="L38">IFERROR(CONCATENATE((INDEX($N$7:$N$31,SMALL(IF($N$7:$N$31&lt;&gt;"",IF($K$7:$K$31&lt;&gt;"",ROW($K$7:$K$31)-MIN(ROW($K$7:$K$31))+1,""),""),ROW()-ROW(A$33)+1))),","),"")</f>
+        <f t="array" ref="L38">IFERROR(CONCATENATE((INDEX($N$7:$N$30,SMALL(IF($N$7:$N$30&lt;&gt;"",IF($K$7:$K$30&lt;&gt;"",ROW($K$7:$K$30)-MIN(ROW($K$7:$K$30))+1,""),""),ROW()-ROW(A$32)+1))),","),"")</f>
         <v>0</v>
       </c>
       <c r="M38">
-        <f t="array" ref="M38">IFERROR(CONCATENATE((INDEX($A$7:$A$31,SMALL(IF($N$7:$N$31&lt;&gt;"",IF($K$7:$K$31&lt;&gt;"",ROW($K$7:$K$31)-MIN(ROW($K$7:$K$31))+1,""),""),ROW()-ROW(A$33)+1))),),"")</f>
+        <f t="array" ref="M38">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($N$7:$N$30&lt;&gt;"",IF($K$7:$K$30&lt;&gt;"",ROW($K$7:$K$30)-MIN(ROW($K$7:$K$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
         <v>0</v>
       </c>
       <c r="Q38">
-        <f t="array" ref="Q38">IFERROR(CONCATENATE((INDEX($T$7:$T$31,SMALL(IF($T$7:$T$31&lt;&gt;"",IF($Q$7:$Q$31&lt;&gt;"",ROW($Q$7:$Q$31)-MIN(ROW($Q$7:$Q$31))+1,""),""),ROW()-ROW(A$33)+1)))," "),"")</f>
+        <f t="array" ref="Q38">IFERROR(CONCATENATE((INDEX($T$7:$T$30,SMALL(IF($T$7:$T$30&lt;&gt;"",IF($Q$7:$Q$30&lt;&gt;"",ROW($Q$7:$Q$30)-MIN(ROW($Q$7:$Q$30))+1,""),""),ROW()-ROW(A$32)+1)))," "),"")</f>
         <v>0</v>
       </c>
       <c r="R38">
-        <f t="array" ref="R38">IFERROR(CONCATENATE(TEXT(INDEX($Q$7:$Q$31,SMALL(IF($T$7:$T$31&lt;&gt;"",IF($Q$7:$Q$31&lt;&gt;"",ROW($Q$7:$Q$31)-MIN(ROW($Q$7:$Q$31))+1,""),""),ROW()-ROW(A$33)+1)),"##0")," "),"")</f>
+        <f t="array" ref="R38">IFERROR(CONCATENATE(TEXT(INDEX($Q$7:$Q$30,SMALL(IF($T$7:$T$30&lt;&gt;"",IF($Q$7:$Q$30&lt;&gt;"",ROW($Q$7:$Q$30)-MIN(ROW($Q$7:$Q$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0")," "),"")</f>
         <v>0</v>
       </c>
       <c r="S38">
-        <f t="array" ref="S38">IFERROR(CONCATENATE((INDEX($A$7:$A$31,SMALL(IF($T$7:$T$31&lt;&gt;"",IF($Q$7:$Q$31&lt;&gt;"",ROW($Q$7:$Q$31)-MIN(ROW($Q$7:$Q$31))+1,""),""),ROW()-ROW(A$33)+1))),),"")</f>
+        <f t="array" ref="S38">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($T$7:$T$30&lt;&gt;"",IF($Q$7:$Q$30&lt;&gt;"",ROW($Q$7:$Q$30)-MIN(ROW($Q$7:$Q$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
         <v>0</v>
       </c>
       <c r="W38">
-        <f t="array" ref="W38">IFERROR(CONCATENATE((INDEX($Z$7:$Z$31,SMALL(IF($Z$7:$Z$31&lt;&gt;"",IF($W$7:$W$31&lt;&gt;"",ROW($W$7:$W$31)-MIN(ROW($W$7:$W$31))+1,""),""),ROW()-ROW(A$33)+1))),","),"")</f>
+        <f t="array" ref="W38">IFERROR(CONCATENATE((INDEX($Z$7:$Z$30,SMALL(IF($Z$7:$Z$30&lt;&gt;"",IF($W$7:$W$30&lt;&gt;"",ROW($W$7:$W$30)-MIN(ROW($W$7:$W$30))+1,""),""),ROW()-ROW(A$32)+1))),","),"")</f>
         <v>0</v>
       </c>
       <c r="X38">
-        <f t="array" ref="X38">IFERROR(CONCATENATE(TEXT(INDEX($W$7:$W$31,SMALL(IF($Z$7:$Z$31&lt;&gt;"",IF($W$7:$W$31&lt;&gt;"",ROW($W$7:$W$31)-MIN(ROW($W$7:$W$31))+1,""),""),ROW()-ROW(A$33)+1)),"##0"),","),"")</f>
+        <f t="array" ref="X38">IFERROR(CONCATENATE(TEXT(INDEX($W$7:$W$30,SMALL(IF($Z$7:$Z$30&lt;&gt;"",IF($W$7:$W$30&lt;&gt;"",ROW($W$7:$W$30)-MIN(ROW($W$7:$W$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0"),","),"")</f>
         <v>0</v>
       </c>
       <c r="Y38">
-        <f t="array" ref="Y38">IFERROR(CONCATENATE((INDEX($A$7:$A$31,SMALL(IF($Z$7:$Z$31&lt;&gt;"",IF($W$7:$W$31&lt;&gt;"",ROW($W$7:$W$31)-MIN(ROW($W$7:$W$31))+1,""),""),ROW()-ROW(A$33)+1))),),"")</f>
+        <f t="array" ref="Y38">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($Z$7:$Z$30&lt;&gt;"",IF($W$7:$W$30&lt;&gt;"",ROW($W$7:$W$30)-MIN(ROW($W$7:$W$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="39" spans="11:25">
       <c r="K39">
-        <f t="array" ref="K39">IFERROR(CONCATENATE(TEXT(INDEX($K$7:$K$31,SMALL(IF($N$7:$N$31&lt;&gt;"",IF($K$7:$K$31&lt;&gt;"",ROW($K$7:$K$31)-MIN(ROW($K$7:$K$31))+1,""),""),ROW()-ROW(A$33)+1)),"##0"),","),"")</f>
+        <f t="array" ref="K39">IFERROR(CONCATENATE(TEXT(INDEX($K$7:$K$30,SMALL(IF($N$7:$N$30&lt;&gt;"",IF($K$7:$K$30&lt;&gt;"",ROW($K$7:$K$30)-MIN(ROW($K$7:$K$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0"),","),"")</f>
         <v>0</v>
       </c>
       <c r="L39">
-        <f t="array" ref="L39">IFERROR(CONCATENATE((INDEX($N$7:$N$31,SMALL(IF($N$7:$N$31&lt;&gt;"",IF($K$7:$K$31&lt;&gt;"",ROW($K$7:$K$31)-MIN(ROW($K$7:$K$31))+1,""),""),ROW()-ROW(A$33)+1))),","),"")</f>
+        <f t="array" ref="L39">IFERROR(CONCATENATE((INDEX($N$7:$N$30,SMALL(IF($N$7:$N$30&lt;&gt;"",IF($K$7:$K$30&lt;&gt;"",ROW($K$7:$K$30)-MIN(ROW($K$7:$K$30))+1,""),""),ROW()-ROW(A$32)+1))),","),"")</f>
         <v>0</v>
       </c>
       <c r="M39">
-        <f t="array" ref="M39">IFERROR(CONCATENATE((INDEX($A$7:$A$31,SMALL(IF($N$7:$N$31&lt;&gt;"",IF($K$7:$K$31&lt;&gt;"",ROW($K$7:$K$31)-MIN(ROW($K$7:$K$31))+1,""),""),ROW()-ROW(A$33)+1))),),"")</f>
+        <f t="array" ref="M39">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($N$7:$N$30&lt;&gt;"",IF($K$7:$K$30&lt;&gt;"",ROW($K$7:$K$30)-MIN(ROW($K$7:$K$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
         <v>0</v>
       </c>
       <c r="Q39">
-        <f t="array" ref="Q39">IFERROR(CONCATENATE((INDEX($T$7:$T$31,SMALL(IF($T$7:$T$31&lt;&gt;"",IF($Q$7:$Q$31&lt;&gt;"",ROW($Q$7:$Q$31)-MIN(ROW($Q$7:$Q$31))+1,""),""),ROW()-ROW(A$33)+1)))," "),"")</f>
+        <f t="array" ref="Q39">IFERROR(CONCATENATE((INDEX($T$7:$T$30,SMALL(IF($T$7:$T$30&lt;&gt;"",IF($Q$7:$Q$30&lt;&gt;"",ROW($Q$7:$Q$30)-MIN(ROW($Q$7:$Q$30))+1,""),""),ROW()-ROW(A$32)+1)))," "),"")</f>
         <v>0</v>
       </c>
       <c r="R39">
-        <f t="array" ref="R39">IFERROR(CONCATENATE(TEXT(INDEX($Q$7:$Q$31,SMALL(IF($T$7:$T$31&lt;&gt;"",IF($Q$7:$Q$31&lt;&gt;"",ROW($Q$7:$Q$31)-MIN(ROW($Q$7:$Q$31))+1,""),""),ROW()-ROW(A$33)+1)),"##0")," "),"")</f>
+        <f t="array" ref="R39">IFERROR(CONCATENATE(TEXT(INDEX($Q$7:$Q$30,SMALL(IF($T$7:$T$30&lt;&gt;"",IF($Q$7:$Q$30&lt;&gt;"",ROW($Q$7:$Q$30)-MIN(ROW($Q$7:$Q$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0")," "),"")</f>
         <v>0</v>
       </c>
       <c r="S39">
-        <f t="array" ref="S39">IFERROR(CONCATENATE((INDEX($A$7:$A$31,SMALL(IF($T$7:$T$31&lt;&gt;"",IF($Q$7:$Q$31&lt;&gt;"",ROW($Q$7:$Q$31)-MIN(ROW($Q$7:$Q$31))+1,""),""),ROW()-ROW(A$33)+1))),),"")</f>
+        <f t="array" ref="S39">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($T$7:$T$30&lt;&gt;"",IF($Q$7:$Q$30&lt;&gt;"",ROW($Q$7:$Q$30)-MIN(ROW($Q$7:$Q$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
         <v>0</v>
       </c>
       <c r="W39">
-        <f t="array" ref="W39">IFERROR(CONCATENATE((INDEX($Z$7:$Z$31,SMALL(IF($Z$7:$Z$31&lt;&gt;"",IF($W$7:$W$31&lt;&gt;"",ROW($W$7:$W$31)-MIN(ROW($W$7:$W$31))+1,""),""),ROW()-ROW(A$33)+1))),","),"")</f>
+        <f t="array" ref="W39">IFERROR(CONCATENATE((INDEX($Z$7:$Z$30,SMALL(IF($Z$7:$Z$30&lt;&gt;"",IF($W$7:$W$30&lt;&gt;"",ROW($W$7:$W$30)-MIN(ROW($W$7:$W$30))+1,""),""),ROW()-ROW(A$32)+1))),","),"")</f>
         <v>0</v>
       </c>
       <c r="X39">
-        <f t="array" ref="X39">IFERROR(CONCATENATE(TEXT(INDEX($W$7:$W$31,SMALL(IF($Z$7:$Z$31&lt;&gt;"",IF($W$7:$W$31&lt;&gt;"",ROW($W$7:$W$31)-MIN(ROW($W$7:$W$31))+1,""),""),ROW()-ROW(A$33)+1)),"##0"),","),"")</f>
+        <f t="array" ref="X39">IFERROR(CONCATENATE(TEXT(INDEX($W$7:$W$30,SMALL(IF($Z$7:$Z$30&lt;&gt;"",IF($W$7:$W$30&lt;&gt;"",ROW($W$7:$W$30)-MIN(ROW($W$7:$W$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0"),","),"")</f>
         <v>0</v>
       </c>
       <c r="Y39">
-        <f t="array" ref="Y39">IFERROR(CONCATENATE((INDEX($A$7:$A$31,SMALL(IF($Z$7:$Z$31&lt;&gt;"",IF($W$7:$W$31&lt;&gt;"",ROW($W$7:$W$31)-MIN(ROW($W$7:$W$31))+1,""),""),ROW()-ROW(A$33)+1))),),"")</f>
+        <f t="array" ref="Y39">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($Z$7:$Z$30&lt;&gt;"",IF($W$7:$W$30&lt;&gt;"",ROW($W$7:$W$30)-MIN(ROW($W$7:$W$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="40" spans="11:25">
       <c r="K40">
-        <f t="array" ref="K40">IFERROR(CONCATENATE(TEXT(INDEX($K$7:$K$31,SMALL(IF($N$7:$N$31&lt;&gt;"",IF($K$7:$K$31&lt;&gt;"",ROW($K$7:$K$31)-MIN(ROW($K$7:$K$31))+1,""),""),ROW()-ROW(A$33)+1)),"##0"),","),"")</f>
+        <f t="array" ref="K40">IFERROR(CONCATENATE(TEXT(INDEX($K$7:$K$30,SMALL(IF($N$7:$N$30&lt;&gt;"",IF($K$7:$K$30&lt;&gt;"",ROW($K$7:$K$30)-MIN(ROW($K$7:$K$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0"),","),"")</f>
         <v>0</v>
       </c>
       <c r="L40">
-        <f t="array" ref="L40">IFERROR(CONCATENATE((INDEX($N$7:$N$31,SMALL(IF($N$7:$N$31&lt;&gt;"",IF($K$7:$K$31&lt;&gt;"",ROW($K$7:$K$31)-MIN(ROW($K$7:$K$31))+1,""),""),ROW()-ROW(A$33)+1))),","),"")</f>
+        <f t="array" ref="L40">IFERROR(CONCATENATE((INDEX($N$7:$N$30,SMALL(IF($N$7:$N$30&lt;&gt;"",IF($K$7:$K$30&lt;&gt;"",ROW($K$7:$K$30)-MIN(ROW($K$7:$K$30))+1,""),""),ROW()-ROW(A$32)+1))),","),"")</f>
         <v>0</v>
       </c>
       <c r="M40">
-        <f t="array" ref="M40">IFERROR(CONCATENATE((INDEX($A$7:$A$31,SMALL(IF($N$7:$N$31&lt;&gt;"",IF($K$7:$K$31&lt;&gt;"",ROW($K$7:$K$31)-MIN(ROW($K$7:$K$31))+1,""),""),ROW()-ROW(A$33)+1))),),"")</f>
+        <f t="array" ref="M40">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($N$7:$N$30&lt;&gt;"",IF($K$7:$K$30&lt;&gt;"",ROW($K$7:$K$30)-MIN(ROW($K$7:$K$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
         <v>0</v>
       </c>
       <c r="Q40">
-        <f t="array" ref="Q40">IFERROR(CONCATENATE((INDEX($T$7:$T$31,SMALL(IF($T$7:$T$31&lt;&gt;"",IF($Q$7:$Q$31&lt;&gt;"",ROW($Q$7:$Q$31)-MIN(ROW($Q$7:$Q$31))+1,""),""),ROW()-ROW(A$33)+1)))," "),"")</f>
+        <f t="array" ref="Q40">IFERROR(CONCATENATE((INDEX($T$7:$T$30,SMALL(IF($T$7:$T$30&lt;&gt;"",IF($Q$7:$Q$30&lt;&gt;"",ROW($Q$7:$Q$30)-MIN(ROW($Q$7:$Q$30))+1,""),""),ROW()-ROW(A$32)+1)))," "),"")</f>
         <v>0</v>
       </c>
       <c r="R40">
-        <f t="array" ref="R40">IFERROR(CONCATENATE(TEXT(INDEX($Q$7:$Q$31,SMALL(IF($T$7:$T$31&lt;&gt;"",IF($Q$7:$Q$31&lt;&gt;"",ROW($Q$7:$Q$31)-MIN(ROW($Q$7:$Q$31))+1,""),""),ROW()-ROW(A$33)+1)),"##0")," "),"")</f>
+        <f t="array" ref="R40">IFERROR(CONCATENATE(TEXT(INDEX($Q$7:$Q$30,SMALL(IF($T$7:$T$30&lt;&gt;"",IF($Q$7:$Q$30&lt;&gt;"",ROW($Q$7:$Q$30)-MIN(ROW($Q$7:$Q$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0")," "),"")</f>
         <v>0</v>
       </c>
       <c r="S40">
-        <f t="array" ref="S40">IFERROR(CONCATENATE((INDEX($A$7:$A$31,SMALL(IF($T$7:$T$31&lt;&gt;"",IF($Q$7:$Q$31&lt;&gt;"",ROW($Q$7:$Q$31)-MIN(ROW($Q$7:$Q$31))+1,""),""),ROW()-ROW(A$33)+1))),),"")</f>
+        <f t="array" ref="S40">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($T$7:$T$30&lt;&gt;"",IF($Q$7:$Q$30&lt;&gt;"",ROW($Q$7:$Q$30)-MIN(ROW($Q$7:$Q$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
         <v>0</v>
       </c>
       <c r="W40">
-        <f t="array" ref="W40">IFERROR(CONCATENATE((INDEX($Z$7:$Z$31,SMALL(IF($Z$7:$Z$31&lt;&gt;"",IF($W$7:$W$31&lt;&gt;"",ROW($W$7:$W$31)-MIN(ROW($W$7:$W$31))+1,""),""),ROW()-ROW(A$33)+1))),","),"")</f>
+        <f t="array" ref="W40">IFERROR(CONCATENATE((INDEX($Z$7:$Z$30,SMALL(IF($Z$7:$Z$30&lt;&gt;"",IF($W$7:$W$30&lt;&gt;"",ROW($W$7:$W$30)-MIN(ROW($W$7:$W$30))+1,""),""),ROW()-ROW(A$32)+1))),","),"")</f>
         <v>0</v>
       </c>
       <c r="X40">
-        <f t="array" ref="X40">IFERROR(CONCATENATE(TEXT(INDEX($W$7:$W$31,SMALL(IF($Z$7:$Z$31&lt;&gt;"",IF($W$7:$W$31&lt;&gt;"",ROW($W$7:$W$31)-MIN(ROW($W$7:$W$31))+1,""),""),ROW()-ROW(A$33)+1)),"##0"),","),"")</f>
+        <f t="array" ref="X40">IFERROR(CONCATENATE(TEXT(INDEX($W$7:$W$30,SMALL(IF($Z$7:$Z$30&lt;&gt;"",IF($W$7:$W$30&lt;&gt;"",ROW($W$7:$W$30)-MIN(ROW($W$7:$W$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0"),","),"")</f>
         <v>0</v>
       </c>
       <c r="Y40">
-        <f t="array" ref="Y40">IFERROR(CONCATENATE((INDEX($A$7:$A$31,SMALL(IF($Z$7:$Z$31&lt;&gt;"",IF($W$7:$W$31&lt;&gt;"",ROW($W$7:$W$31)-MIN(ROW($W$7:$W$31))+1,""),""),ROW()-ROW(A$33)+1))),),"")</f>
+        <f t="array" ref="Y40">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($Z$7:$Z$30&lt;&gt;"",IF($W$7:$W$30&lt;&gt;"",ROW($W$7:$W$30)-MIN(ROW($W$7:$W$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="41" spans="11:25">
       <c r="K41">
-        <f t="array" ref="K41">IFERROR(CONCATENATE(TEXT(INDEX($K$7:$K$31,SMALL(IF($N$7:$N$31&lt;&gt;"",IF($K$7:$K$31&lt;&gt;"",ROW($K$7:$K$31)-MIN(ROW($K$7:$K$31))+1,""),""),ROW()-ROW(A$33)+1)),"##0"),","),"")</f>
+        <f t="array" ref="K41">IFERROR(CONCATENATE(TEXT(INDEX($K$7:$K$30,SMALL(IF($N$7:$N$30&lt;&gt;"",IF($K$7:$K$30&lt;&gt;"",ROW($K$7:$K$30)-MIN(ROW($K$7:$K$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0"),","),"")</f>
         <v>0</v>
       </c>
       <c r="L41">
-        <f t="array" ref="L41">IFERROR(CONCATENATE((INDEX($N$7:$N$31,SMALL(IF($N$7:$N$31&lt;&gt;"",IF($K$7:$K$31&lt;&gt;"",ROW($K$7:$K$31)-MIN(ROW($K$7:$K$31))+1,""),""),ROW()-ROW(A$33)+1))),","),"")</f>
+        <f t="array" ref="L41">IFERROR(CONCATENATE((INDEX($N$7:$N$30,SMALL(IF($N$7:$N$30&lt;&gt;"",IF($K$7:$K$30&lt;&gt;"",ROW($K$7:$K$30)-MIN(ROW($K$7:$K$30))+1,""),""),ROW()-ROW(A$32)+1))),","),"")</f>
         <v>0</v>
       </c>
       <c r="M41">
-        <f t="array" ref="M41">IFERROR(CONCATENATE((INDEX($A$7:$A$31,SMALL(IF($N$7:$N$31&lt;&gt;"",IF($K$7:$K$31&lt;&gt;"",ROW($K$7:$K$31)-MIN(ROW($K$7:$K$31))+1,""),""),ROW()-ROW(A$33)+1))),),"")</f>
+        <f t="array" ref="M41">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($N$7:$N$30&lt;&gt;"",IF($K$7:$K$30&lt;&gt;"",ROW($K$7:$K$30)-MIN(ROW($K$7:$K$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
         <v>0</v>
       </c>
       <c r="Q41">
-        <f t="array" ref="Q41">IFERROR(CONCATENATE((INDEX($T$7:$T$31,SMALL(IF($T$7:$T$31&lt;&gt;"",IF($Q$7:$Q$31&lt;&gt;"",ROW($Q$7:$Q$31)-MIN(ROW($Q$7:$Q$31))+1,""),""),ROW()-ROW(A$33)+1)))," "),"")</f>
+        <f t="array" ref="Q41">IFERROR(CONCATENATE((INDEX($T$7:$T$30,SMALL(IF($T$7:$T$30&lt;&gt;"",IF($Q$7:$Q$30&lt;&gt;"",ROW($Q$7:$Q$30)-MIN(ROW($Q$7:$Q$30))+1,""),""),ROW()-ROW(A$32)+1)))," "),"")</f>
         <v>0</v>
       </c>
       <c r="R41">
-        <f t="array" ref="R41">IFERROR(CONCATENATE(TEXT(INDEX($Q$7:$Q$31,SMALL(IF($T$7:$T$31&lt;&gt;"",IF($Q$7:$Q$31&lt;&gt;"",ROW($Q$7:$Q$31)-MIN(ROW($Q$7:$Q$31))+1,""),""),ROW()-ROW(A$33)+1)),"##0")," "),"")</f>
+        <f t="array" ref="R41">IFERROR(CONCATENATE(TEXT(INDEX($Q$7:$Q$30,SMALL(IF($T$7:$T$30&lt;&gt;"",IF($Q$7:$Q$30&lt;&gt;"",ROW($Q$7:$Q$30)-MIN(ROW($Q$7:$Q$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0")," "),"")</f>
         <v>0</v>
       </c>
       <c r="S41">
-        <f t="array" ref="S41">IFERROR(CONCATENATE((INDEX($A$7:$A$31,SMALL(IF($T$7:$T$31&lt;&gt;"",IF($Q$7:$Q$31&lt;&gt;"",ROW($Q$7:$Q$31)-MIN(ROW($Q$7:$Q$31))+1,""),""),ROW()-ROW(A$33)+1))),),"")</f>
+        <f t="array" ref="S41">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($T$7:$T$30&lt;&gt;"",IF($Q$7:$Q$30&lt;&gt;"",ROW($Q$7:$Q$30)-MIN(ROW($Q$7:$Q$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
         <v>0</v>
       </c>
       <c r="W41">
-        <f t="array" ref="W41">IFERROR(CONCATENATE((INDEX($Z$7:$Z$31,SMALL(IF($Z$7:$Z$31&lt;&gt;"",IF($W$7:$W$31&lt;&gt;"",ROW($W$7:$W$31)-MIN(ROW($W$7:$W$31))+1,""),""),ROW()-ROW(A$33)+1))),","),"")</f>
+        <f t="array" ref="W41">IFERROR(CONCATENATE((INDEX($Z$7:$Z$30,SMALL(IF($Z$7:$Z$30&lt;&gt;"",IF($W$7:$W$30&lt;&gt;"",ROW($W$7:$W$30)-MIN(ROW($W$7:$W$30))+1,""),""),ROW()-ROW(A$32)+1))),","),"")</f>
         <v>0</v>
       </c>
       <c r="X41">
-        <f t="array" ref="X41">IFERROR(CONCATENATE(TEXT(INDEX($W$7:$W$31,SMALL(IF($Z$7:$Z$31&lt;&gt;"",IF($W$7:$W$31&lt;&gt;"",ROW($W$7:$W$31)-MIN(ROW($W$7:$W$31))+1,""),""),ROW()-ROW(A$33)+1)),"##0"),","),"")</f>
+        <f t="array" ref="X41">IFERROR(CONCATENATE(TEXT(INDEX($W$7:$W$30,SMALL(IF($Z$7:$Z$30&lt;&gt;"",IF($W$7:$W$30&lt;&gt;"",ROW($W$7:$W$30)-MIN(ROW($W$7:$W$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0"),","),"")</f>
         <v>0</v>
       </c>
       <c r="Y41">
-        <f t="array" ref="Y41">IFERROR(CONCATENATE((INDEX($A$7:$A$31,SMALL(IF($Z$7:$Z$31&lt;&gt;"",IF($W$7:$W$31&lt;&gt;"",ROW($W$7:$W$31)-MIN(ROW($W$7:$W$31))+1,""),""),ROW()-ROW(A$33)+1))),),"")</f>
+        <f t="array" ref="Y41">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($Z$7:$Z$30&lt;&gt;"",IF($W$7:$W$30&lt;&gt;"",ROW($W$7:$W$30)-MIN(ROW($W$7:$W$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="42" spans="11:25">
       <c r="K42">
-        <f t="array" ref="K42">IFERROR(CONCATENATE(TEXT(INDEX($K$7:$K$31,SMALL(IF($N$7:$N$31&lt;&gt;"",IF($K$7:$K$31&lt;&gt;"",ROW($K$7:$K$31)-MIN(ROW($K$7:$K$31))+1,""),""),ROW()-ROW(A$33)+1)),"##0"),","),"")</f>
+        <f t="array" ref="K42">IFERROR(CONCATENATE(TEXT(INDEX($K$7:$K$30,SMALL(IF($N$7:$N$30&lt;&gt;"",IF($K$7:$K$30&lt;&gt;"",ROW($K$7:$K$30)-MIN(ROW($K$7:$K$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0"),","),"")</f>
         <v>0</v>
       </c>
       <c r="L42">
-        <f t="array" ref="L42">IFERROR(CONCATENATE((INDEX($N$7:$N$31,SMALL(IF($N$7:$N$31&lt;&gt;"",IF($K$7:$K$31&lt;&gt;"",ROW($K$7:$K$31)-MIN(ROW($K$7:$K$31))+1,""),""),ROW()-ROW(A$33)+1))),","),"")</f>
+        <f t="array" ref="L42">IFERROR(CONCATENATE((INDEX($N$7:$N$30,SMALL(IF($N$7:$N$30&lt;&gt;"",IF($K$7:$K$30&lt;&gt;"",ROW($K$7:$K$30)-MIN(ROW($K$7:$K$30))+1,""),""),ROW()-ROW(A$32)+1))),","),"")</f>
         <v>0</v>
       </c>
       <c r="M42">
-        <f t="array" ref="M42">IFERROR(CONCATENATE((INDEX($A$7:$A$31,SMALL(IF($N$7:$N$31&lt;&gt;"",IF($K$7:$K$31&lt;&gt;"",ROW($K$7:$K$31)-MIN(ROW($K$7:$K$31))+1,""),""),ROW()-ROW(A$33)+1))),),"")</f>
+        <f t="array" ref="M42">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($N$7:$N$30&lt;&gt;"",IF($K$7:$K$30&lt;&gt;"",ROW($K$7:$K$30)-MIN(ROW($K$7:$K$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
         <v>0</v>
       </c>
       <c r="Q42">
-        <f t="array" ref="Q42">IFERROR(CONCATENATE((INDEX($T$7:$T$31,SMALL(IF($T$7:$T$31&lt;&gt;"",IF($Q$7:$Q$31&lt;&gt;"",ROW($Q$7:$Q$31)-MIN(ROW($Q$7:$Q$31))+1,""),""),ROW()-ROW(A$33)+1)))," "),"")</f>
+        <f t="array" ref="Q42">IFERROR(CONCATENATE((INDEX($T$7:$T$30,SMALL(IF($T$7:$T$30&lt;&gt;"",IF($Q$7:$Q$30&lt;&gt;"",ROW($Q$7:$Q$30)-MIN(ROW($Q$7:$Q$30))+1,""),""),ROW()-ROW(A$32)+1)))," "),"")</f>
         <v>0</v>
       </c>
       <c r="R42">
-        <f t="array" ref="R42">IFERROR(CONCATENATE(TEXT(INDEX($Q$7:$Q$31,SMALL(IF($T$7:$T$31&lt;&gt;"",IF($Q$7:$Q$31&lt;&gt;"",ROW($Q$7:$Q$31)-MIN(ROW($Q$7:$Q$31))+1,""),""),ROW()-ROW(A$33)+1)),"##0")," "),"")</f>
+        <f t="array" ref="R42">IFERROR(CONCATENATE(TEXT(INDEX($Q$7:$Q$30,SMALL(IF($T$7:$T$30&lt;&gt;"",IF($Q$7:$Q$30&lt;&gt;"",ROW($Q$7:$Q$30)-MIN(ROW($Q$7:$Q$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0")," "),"")</f>
         <v>0</v>
       </c>
       <c r="S42">
-        <f t="array" ref="S42">IFERROR(CONCATENATE((INDEX($A$7:$A$31,SMALL(IF($T$7:$T$31&lt;&gt;"",IF($Q$7:$Q$31&lt;&gt;"",ROW($Q$7:$Q$31)-MIN(ROW($Q$7:$Q$31))+1,""),""),ROW()-ROW(A$33)+1))),),"")</f>
+        <f t="array" ref="S42">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($T$7:$T$30&lt;&gt;"",IF($Q$7:$Q$30&lt;&gt;"",ROW($Q$7:$Q$30)-MIN(ROW($Q$7:$Q$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
         <v>0</v>
       </c>
       <c r="W42">
-        <f t="array" ref="W42">IFERROR(CONCATENATE((INDEX($Z$7:$Z$31,SMALL(IF($Z$7:$Z$31&lt;&gt;"",IF($W$7:$W$31&lt;&gt;"",ROW($W$7:$W$31)-MIN(ROW($W$7:$W$31))+1,""),""),ROW()-ROW(A$33)+1))),","),"")</f>
+        <f t="array" ref="W42">IFERROR(CONCATENATE((INDEX($Z$7:$Z$30,SMALL(IF($Z$7:$Z$30&lt;&gt;"",IF($W$7:$W$30&lt;&gt;"",ROW($W$7:$W$30)-MIN(ROW($W$7:$W$30))+1,""),""),ROW()-ROW(A$32)+1))),","),"")</f>
         <v>0</v>
       </c>
       <c r="X42">
-        <f t="array" ref="X42">IFERROR(CONCATENATE(TEXT(INDEX($W$7:$W$31,SMALL(IF($Z$7:$Z$31&lt;&gt;"",IF($W$7:$W$31&lt;&gt;"",ROW($W$7:$W$31)-MIN(ROW($W$7:$W$31))+1,""),""),ROW()-ROW(A$33)+1)),"##0"),","),"")</f>
+        <f t="array" ref="X42">IFERROR(CONCATENATE(TEXT(INDEX($W$7:$W$30,SMALL(IF($Z$7:$Z$30&lt;&gt;"",IF($W$7:$W$30&lt;&gt;"",ROW($W$7:$W$30)-MIN(ROW($W$7:$W$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0"),","),"")</f>
         <v>0</v>
       </c>
       <c r="Y42">
-        <f t="array" ref="Y42">IFERROR(CONCATENATE((INDEX($A$7:$A$31,SMALL(IF($Z$7:$Z$31&lt;&gt;"",IF($W$7:$W$31&lt;&gt;"",ROW($W$7:$W$31)-MIN(ROW($W$7:$W$31))+1,""),""),ROW()-ROW(A$33)+1))),),"")</f>
+        <f t="array" ref="Y42">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($Z$7:$Z$30&lt;&gt;"",IF($W$7:$W$30&lt;&gt;"",ROW($W$7:$W$30)-MIN(ROW($W$7:$W$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="43" spans="11:25">
       <c r="K43">
-        <f t="array" ref="K43">IFERROR(CONCATENATE(TEXT(INDEX($K$7:$K$31,SMALL(IF($N$7:$N$31&lt;&gt;"",IF($K$7:$K$31&lt;&gt;"",ROW($K$7:$K$31)-MIN(ROW($K$7:$K$31))+1,""),""),ROW()-ROW(A$33)+1)),"##0"),","),"")</f>
+        <f t="array" ref="K43">IFERROR(CONCATENATE(TEXT(INDEX($K$7:$K$30,SMALL(IF($N$7:$N$30&lt;&gt;"",IF($K$7:$K$30&lt;&gt;"",ROW($K$7:$K$30)-MIN(ROW($K$7:$K$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0"),","),"")</f>
         <v>0</v>
       </c>
       <c r="L43">
-        <f t="array" ref="L43">IFERROR(CONCATENATE((INDEX($N$7:$N$31,SMALL(IF($N$7:$N$31&lt;&gt;"",IF($K$7:$K$31&lt;&gt;"",ROW($K$7:$K$31)-MIN(ROW($K$7:$K$31))+1,""),""),ROW()-ROW(A$33)+1))),","),"")</f>
+        <f t="array" ref="L43">IFERROR(CONCATENATE((INDEX($N$7:$N$30,SMALL(IF($N$7:$N$30&lt;&gt;"",IF($K$7:$K$30&lt;&gt;"",ROW($K$7:$K$30)-MIN(ROW($K$7:$K$30))+1,""),""),ROW()-ROW(A$32)+1))),","),"")</f>
         <v>0</v>
       </c>
       <c r="M43">
-        <f t="array" ref="M43">IFERROR(CONCATENATE((INDEX($A$7:$A$31,SMALL(IF($N$7:$N$31&lt;&gt;"",IF($K$7:$K$31&lt;&gt;"",ROW($K$7:$K$31)-MIN(ROW($K$7:$K$31))+1,""),""),ROW()-ROW(A$33)+1))),),"")</f>
+        <f t="array" ref="M43">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($N$7:$N$30&lt;&gt;"",IF($K$7:$K$30&lt;&gt;"",ROW($K$7:$K$30)-MIN(ROW($K$7:$K$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
         <v>0</v>
       </c>
       <c r="Q43">
-        <f t="array" ref="Q43">IFERROR(CONCATENATE((INDEX($T$7:$T$31,SMALL(IF($T$7:$T$31&lt;&gt;"",IF($Q$7:$Q$31&lt;&gt;"",ROW($Q$7:$Q$31)-MIN(ROW($Q$7:$Q$31))+1,""),""),ROW()-ROW(A$33)+1)))," "),"")</f>
+        <f t="array" ref="Q43">IFERROR(CONCATENATE((INDEX($T$7:$T$30,SMALL(IF($T$7:$T$30&lt;&gt;"",IF($Q$7:$Q$30&lt;&gt;"",ROW($Q$7:$Q$30)-MIN(ROW($Q$7:$Q$30))+1,""),""),ROW()-ROW(A$32)+1)))," "),"")</f>
         <v>0</v>
       </c>
       <c r="R43">
-        <f t="array" ref="R43">IFERROR(CONCATENATE(TEXT(INDEX($Q$7:$Q$31,SMALL(IF($T$7:$T$31&lt;&gt;"",IF($Q$7:$Q$31&lt;&gt;"",ROW($Q$7:$Q$31)-MIN(ROW($Q$7:$Q$31))+1,""),""),ROW()-ROW(A$33)+1)),"##0")," "),"")</f>
+        <f t="array" ref="R43">IFERROR(CONCATENATE(TEXT(INDEX($Q$7:$Q$30,SMALL(IF($T$7:$T$30&lt;&gt;"",IF($Q$7:$Q$30&lt;&gt;"",ROW($Q$7:$Q$30)-MIN(ROW($Q$7:$Q$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0")," "),"")</f>
         <v>0</v>
       </c>
       <c r="S43">
-        <f t="array" ref="S43">IFERROR(CONCATENATE((INDEX($A$7:$A$31,SMALL(IF($T$7:$T$31&lt;&gt;"",IF($Q$7:$Q$31&lt;&gt;"",ROW($Q$7:$Q$31)-MIN(ROW($Q$7:$Q$31))+1,""),""),ROW()-ROW(A$33)+1))),),"")</f>
+        <f t="array" ref="S43">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($T$7:$T$30&lt;&gt;"",IF($Q$7:$Q$30&lt;&gt;"",ROW($Q$7:$Q$30)-MIN(ROW($Q$7:$Q$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
         <v>0</v>
       </c>
       <c r="W43">
-        <f t="array" ref="W43">IFERROR(CONCATENATE((INDEX($Z$7:$Z$31,SMALL(IF($Z$7:$Z$31&lt;&gt;"",IF($W$7:$W$31&lt;&gt;"",ROW($W$7:$W$31)-MIN(ROW($W$7:$W$31))+1,""),""),ROW()-ROW(A$33)+1))),","),"")</f>
+        <f t="array" ref="W43">IFERROR(CONCATENATE((INDEX($Z$7:$Z$30,SMALL(IF($Z$7:$Z$30&lt;&gt;"",IF($W$7:$W$30&lt;&gt;"",ROW($W$7:$W$30)-MIN(ROW($W$7:$W$30))+1,""),""),ROW()-ROW(A$32)+1))),","),"")</f>
         <v>0</v>
       </c>
       <c r="X43">
-        <f t="array" ref="X43">IFERROR(CONCATENATE(TEXT(INDEX($W$7:$W$31,SMALL(IF($Z$7:$Z$31&lt;&gt;"",IF($W$7:$W$31&lt;&gt;"",ROW($W$7:$W$31)-MIN(ROW($W$7:$W$31))+1,""),""),ROW()-ROW(A$33)+1)),"##0"),","),"")</f>
+        <f t="array" ref="X43">IFERROR(CONCATENATE(TEXT(INDEX($W$7:$W$30,SMALL(IF($Z$7:$Z$30&lt;&gt;"",IF($W$7:$W$30&lt;&gt;"",ROW($W$7:$W$30)-MIN(ROW($W$7:$W$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0"),","),"")</f>
         <v>0</v>
       </c>
       <c r="Y43">
-        <f t="array" ref="Y43">IFERROR(CONCATENATE((INDEX($A$7:$A$31,SMALL(IF($Z$7:$Z$31&lt;&gt;"",IF($W$7:$W$31&lt;&gt;"",ROW($W$7:$W$31)-MIN(ROW($W$7:$W$31))+1,""),""),ROW()-ROW(A$33)+1))),),"")</f>
+        <f t="array" ref="Y43">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($Z$7:$Z$30&lt;&gt;"",IF($W$7:$W$30&lt;&gt;"",ROW($W$7:$W$30)-MIN(ROW($W$7:$W$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="44" spans="11:25">
       <c r="K44">
-        <f t="array" ref="K44">IFERROR(CONCATENATE(TEXT(INDEX($K$7:$K$31,SMALL(IF($N$7:$N$31&lt;&gt;"",IF($K$7:$K$31&lt;&gt;"",ROW($K$7:$K$31)-MIN(ROW($K$7:$K$31))+1,""),""),ROW()-ROW(A$33)+1)),"##0"),","),"")</f>
+        <f t="array" ref="K44">IFERROR(CONCATENATE(TEXT(INDEX($K$7:$K$30,SMALL(IF($N$7:$N$30&lt;&gt;"",IF($K$7:$K$30&lt;&gt;"",ROW($K$7:$K$30)-MIN(ROW($K$7:$K$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0"),","),"")</f>
         <v>0</v>
       </c>
       <c r="L44">
-        <f t="array" ref="L44">IFERROR(CONCATENATE((INDEX($N$7:$N$31,SMALL(IF($N$7:$N$31&lt;&gt;"",IF($K$7:$K$31&lt;&gt;"",ROW($K$7:$K$31)-MIN(ROW($K$7:$K$31))+1,""),""),ROW()-ROW(A$33)+1))),","),"")</f>
+        <f t="array" ref="L44">IFERROR(CONCATENATE((INDEX($N$7:$N$30,SMALL(IF($N$7:$N$30&lt;&gt;"",IF($K$7:$K$30&lt;&gt;"",ROW($K$7:$K$30)-MIN(ROW($K$7:$K$30))+1,""),""),ROW()-ROW(A$32)+1))),","),"")</f>
         <v>0</v>
       </c>
       <c r="M44">
-        <f t="array" ref="M44">IFERROR(CONCATENATE((INDEX($A$7:$A$31,SMALL(IF($N$7:$N$31&lt;&gt;"",IF($K$7:$K$31&lt;&gt;"",ROW($K$7:$K$31)-MIN(ROW($K$7:$K$31))+1,""),""),ROW()-ROW(A$33)+1))),),"")</f>
+        <f t="array" ref="M44">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($N$7:$N$30&lt;&gt;"",IF($K$7:$K$30&lt;&gt;"",ROW($K$7:$K$30)-MIN(ROW($K$7:$K$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
         <v>0</v>
       </c>
       <c r="Q44">
-        <f t="array" ref="Q44">IFERROR(CONCATENATE((INDEX($T$7:$T$31,SMALL(IF($T$7:$T$31&lt;&gt;"",IF($Q$7:$Q$31&lt;&gt;"",ROW($Q$7:$Q$31)-MIN(ROW($Q$7:$Q$31))+1,""),""),ROW()-ROW(A$33)+1)))," "),"")</f>
+        <f t="array" ref="Q44">IFERROR(CONCATENATE((INDEX($T$7:$T$30,SMALL(IF($T$7:$T$30&lt;&gt;"",IF($Q$7:$Q$30&lt;&gt;"",ROW($Q$7:$Q$30)-MIN(ROW($Q$7:$Q$30))+1,""),""),ROW()-ROW(A$32)+1)))," "),"")</f>
         <v>0</v>
       </c>
       <c r="R44">
-        <f t="array" ref="R44">IFERROR(CONCATENATE(TEXT(INDEX($Q$7:$Q$31,SMALL(IF($T$7:$T$31&lt;&gt;"",IF($Q$7:$Q$31&lt;&gt;"",ROW($Q$7:$Q$31)-MIN(ROW($Q$7:$Q$31))+1,""),""),ROW()-ROW(A$33)+1)),"##0")," "),"")</f>
+        <f t="array" ref="R44">IFERROR(CONCATENATE(TEXT(INDEX($Q$7:$Q$30,SMALL(IF($T$7:$T$30&lt;&gt;"",IF($Q$7:$Q$30&lt;&gt;"",ROW($Q$7:$Q$30)-MIN(ROW($Q$7:$Q$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0")," "),"")</f>
         <v>0</v>
       </c>
       <c r="S44">
-        <f t="array" ref="S44">IFERROR(CONCATENATE((INDEX($A$7:$A$31,SMALL(IF($T$7:$T$31&lt;&gt;"",IF($Q$7:$Q$31&lt;&gt;"",ROW($Q$7:$Q$31)-MIN(ROW($Q$7:$Q$31))+1,""),""),ROW()-ROW(A$33)+1))),),"")</f>
+        <f t="array" ref="S44">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($T$7:$T$30&lt;&gt;"",IF($Q$7:$Q$30&lt;&gt;"",ROW($Q$7:$Q$30)-MIN(ROW($Q$7:$Q$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
         <v>0</v>
       </c>
       <c r="W44">
-        <f t="array" ref="W44">IFERROR(CONCATENATE((INDEX($Z$7:$Z$31,SMALL(IF($Z$7:$Z$31&lt;&gt;"",IF($W$7:$W$31&lt;&gt;"",ROW($W$7:$W$31)-MIN(ROW($W$7:$W$31))+1,""),""),ROW()-ROW(A$33)+1))),","),"")</f>
+        <f t="array" ref="W44">IFERROR(CONCATENATE((INDEX($Z$7:$Z$30,SMALL(IF($Z$7:$Z$30&lt;&gt;"",IF($W$7:$W$30&lt;&gt;"",ROW($W$7:$W$30)-MIN(ROW($W$7:$W$30))+1,""),""),ROW()-ROW(A$32)+1))),","),"")</f>
         <v>0</v>
       </c>
       <c r="X44">
-        <f t="array" ref="X44">IFERROR(CONCATENATE(TEXT(INDEX($W$7:$W$31,SMALL(IF($Z$7:$Z$31&lt;&gt;"",IF($W$7:$W$31&lt;&gt;"",ROW($W$7:$W$31)-MIN(ROW($W$7:$W$31))+1,""),""),ROW()-ROW(A$33)+1)),"##0"),","),"")</f>
+        <f t="array" ref="X44">IFERROR(CONCATENATE(TEXT(INDEX($W$7:$W$30,SMALL(IF($Z$7:$Z$30&lt;&gt;"",IF($W$7:$W$30&lt;&gt;"",ROW($W$7:$W$30)-MIN(ROW($W$7:$W$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0"),","),"")</f>
         <v>0</v>
       </c>
       <c r="Y44">
-        <f t="array" ref="Y44">IFERROR(CONCATENATE((INDEX($A$7:$A$31,SMALL(IF($Z$7:$Z$31&lt;&gt;"",IF($W$7:$W$31&lt;&gt;"",ROW($W$7:$W$31)-MIN(ROW($W$7:$W$31))+1,""),""),ROW()-ROW(A$33)+1))),),"")</f>
+        <f t="array" ref="Y44">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($Z$7:$Z$30&lt;&gt;"",IF($W$7:$W$30&lt;&gt;"",ROW($W$7:$W$30)-MIN(ROW($W$7:$W$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="45" spans="11:25">
       <c r="K45">
-        <f t="array" ref="K45">IFERROR(CONCATENATE(TEXT(INDEX($K$7:$K$31,SMALL(IF($N$7:$N$31&lt;&gt;"",IF($K$7:$K$31&lt;&gt;"",ROW($K$7:$K$31)-MIN(ROW($K$7:$K$31))+1,""),""),ROW()-ROW(A$33)+1)),"##0"),","),"")</f>
+        <f t="array" ref="K45">IFERROR(CONCATENATE(TEXT(INDEX($K$7:$K$30,SMALL(IF($N$7:$N$30&lt;&gt;"",IF($K$7:$K$30&lt;&gt;"",ROW($K$7:$K$30)-MIN(ROW($K$7:$K$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0"),","),"")</f>
         <v>0</v>
       </c>
       <c r="L45">
-        <f t="array" ref="L45">IFERROR(CONCATENATE((INDEX($N$7:$N$31,SMALL(IF($N$7:$N$31&lt;&gt;"",IF($K$7:$K$31&lt;&gt;"",ROW($K$7:$K$31)-MIN(ROW($K$7:$K$31))+1,""),""),ROW()-ROW(A$33)+1))),","),"")</f>
+        <f t="array" ref="L45">IFERROR(CONCATENATE((INDEX($N$7:$N$30,SMALL(IF($N$7:$N$30&lt;&gt;"",IF($K$7:$K$30&lt;&gt;"",ROW($K$7:$K$30)-MIN(ROW($K$7:$K$30))+1,""),""),ROW()-ROW(A$32)+1))),","),"")</f>
         <v>0</v>
       </c>
       <c r="M45">
-        <f t="array" ref="M45">IFERROR(CONCATENATE((INDEX($A$7:$A$31,SMALL(IF($N$7:$N$31&lt;&gt;"",IF($K$7:$K$31&lt;&gt;"",ROW($K$7:$K$31)-MIN(ROW($K$7:$K$31))+1,""),""),ROW()-ROW(A$33)+1))),),"")</f>
+        <f t="array" ref="M45">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($N$7:$N$30&lt;&gt;"",IF($K$7:$K$30&lt;&gt;"",ROW($K$7:$K$30)-MIN(ROW($K$7:$K$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
         <v>0</v>
       </c>
       <c r="Q45">
-        <f t="array" ref="Q45">IFERROR(CONCATENATE((INDEX($T$7:$T$31,SMALL(IF($T$7:$T$31&lt;&gt;"",IF($Q$7:$Q$31&lt;&gt;"",ROW($Q$7:$Q$31)-MIN(ROW($Q$7:$Q$31))+1,""),""),ROW()-ROW(A$33)+1)))," "),"")</f>
+        <f t="array" ref="Q45">IFERROR(CONCATENATE((INDEX($T$7:$T$30,SMALL(IF($T$7:$T$30&lt;&gt;"",IF($Q$7:$Q$30&lt;&gt;"",ROW($Q$7:$Q$30)-MIN(ROW($Q$7:$Q$30))+1,""),""),ROW()-ROW(A$32)+1)))," "),"")</f>
         <v>0</v>
       </c>
       <c r="R45">
-        <f t="array" ref="R45">IFERROR(CONCATENATE(TEXT(INDEX($Q$7:$Q$31,SMALL(IF($T$7:$T$31&lt;&gt;"",IF($Q$7:$Q$31&lt;&gt;"",ROW($Q$7:$Q$31)-MIN(ROW($Q$7:$Q$31))+1,""),""),ROW()-ROW(A$33)+1)),"##0")," "),"")</f>
+        <f t="array" ref="R45">IFERROR(CONCATENATE(TEXT(INDEX($Q$7:$Q$30,SMALL(IF($T$7:$T$30&lt;&gt;"",IF($Q$7:$Q$30&lt;&gt;"",ROW($Q$7:$Q$30)-MIN(ROW($Q$7:$Q$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0")," "),"")</f>
         <v>0</v>
       </c>
       <c r="S45">
-        <f t="array" ref="S45">IFERROR(CONCATENATE((INDEX($A$7:$A$31,SMALL(IF($T$7:$T$31&lt;&gt;"",IF($Q$7:$Q$31&lt;&gt;"",ROW($Q$7:$Q$31)-MIN(ROW($Q$7:$Q$31))+1,""),""),ROW()-ROW(A$33)+1))),),"")</f>
+        <f t="array" ref="S45">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($T$7:$T$30&lt;&gt;"",IF($Q$7:$Q$30&lt;&gt;"",ROW($Q$7:$Q$30)-MIN(ROW($Q$7:$Q$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
         <v>0</v>
       </c>
       <c r="W45">
-        <f t="array" ref="W45">IFERROR(CONCATENATE((INDEX($Z$7:$Z$31,SMALL(IF($Z$7:$Z$31&lt;&gt;"",IF($W$7:$W$31&lt;&gt;"",ROW($W$7:$W$31)-MIN(ROW($W$7:$W$31))+1,""),""),ROW()-ROW(A$33)+1))),","),"")</f>
+        <f t="array" ref="W45">IFERROR(CONCATENATE((INDEX($Z$7:$Z$30,SMALL(IF($Z$7:$Z$30&lt;&gt;"",IF($W$7:$W$30&lt;&gt;"",ROW($W$7:$W$30)-MIN(ROW($W$7:$W$30))+1,""),""),ROW()-ROW(A$32)+1))),","),"")</f>
         <v>0</v>
       </c>
       <c r="X45">
-        <f t="array" ref="X45">IFERROR(CONCATENATE(TEXT(INDEX($W$7:$W$31,SMALL(IF($Z$7:$Z$31&lt;&gt;"",IF($W$7:$W$31&lt;&gt;"",ROW($W$7:$W$31)-MIN(ROW($W$7:$W$31))+1,""),""),ROW()-ROW(A$33)+1)),"##0"),","),"")</f>
+        <f t="array" ref="X45">IFERROR(CONCATENATE(TEXT(INDEX($W$7:$W$30,SMALL(IF($Z$7:$Z$30&lt;&gt;"",IF($W$7:$W$30&lt;&gt;"",ROW($W$7:$W$30)-MIN(ROW($W$7:$W$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0"),","),"")</f>
         <v>0</v>
       </c>
       <c r="Y45">
-        <f t="array" ref="Y45">IFERROR(CONCATENATE((INDEX($A$7:$A$31,SMALL(IF($Z$7:$Z$31&lt;&gt;"",IF($W$7:$W$31&lt;&gt;"",ROW($W$7:$W$31)-MIN(ROW($W$7:$W$31))+1,""),""),ROW()-ROW(A$33)+1))),),"")</f>
+        <f t="array" ref="Y45">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($Z$7:$Z$30&lt;&gt;"",IF($W$7:$W$30&lt;&gt;"",ROW($W$7:$W$30)-MIN(ROW($W$7:$W$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="46" spans="11:25">
       <c r="K46">
-        <f t="array" ref="K46">IFERROR(CONCATENATE(TEXT(INDEX($K$7:$K$31,SMALL(IF($N$7:$N$31&lt;&gt;"",IF($K$7:$K$31&lt;&gt;"",ROW($K$7:$K$31)-MIN(ROW($K$7:$K$31))+1,""),""),ROW()-ROW(A$33)+1)),"##0"),","),"")</f>
+        <f t="array" ref="K46">IFERROR(CONCATENATE(TEXT(INDEX($K$7:$K$30,SMALL(IF($N$7:$N$30&lt;&gt;"",IF($K$7:$K$30&lt;&gt;"",ROW($K$7:$K$30)-MIN(ROW($K$7:$K$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0"),","),"")</f>
         <v>0</v>
       </c>
       <c r="L46">
-        <f t="array" ref="L46">IFERROR(CONCATENATE((INDEX($N$7:$N$31,SMALL(IF($N$7:$N$31&lt;&gt;"",IF($K$7:$K$31&lt;&gt;"",ROW($K$7:$K$31)-MIN(ROW($K$7:$K$31))+1,""),""),ROW()-ROW(A$33)+1))),","),"")</f>
+        <f t="array" ref="L46">IFERROR(CONCATENATE((INDEX($N$7:$N$30,SMALL(IF($N$7:$N$30&lt;&gt;"",IF($K$7:$K$30&lt;&gt;"",ROW($K$7:$K$30)-MIN(ROW($K$7:$K$30))+1,""),""),ROW()-ROW(A$32)+1))),","),"")</f>
         <v>0</v>
       </c>
       <c r="M46">
-        <f t="array" ref="M46">IFERROR(CONCATENATE((INDEX($A$7:$A$31,SMALL(IF($N$7:$N$31&lt;&gt;"",IF($K$7:$K$31&lt;&gt;"",ROW($K$7:$K$31)-MIN(ROW($K$7:$K$31))+1,""),""),ROW()-ROW(A$33)+1))),),"")</f>
+        <f t="array" ref="M46">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($N$7:$N$30&lt;&gt;"",IF($K$7:$K$30&lt;&gt;"",ROW($K$7:$K$30)-MIN(ROW($K$7:$K$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
         <v>0</v>
       </c>
       <c r="Q46">
-        <f t="array" ref="Q46">IFERROR(CONCATENATE((INDEX($T$7:$T$31,SMALL(IF($T$7:$T$31&lt;&gt;"",IF($Q$7:$Q$31&lt;&gt;"",ROW($Q$7:$Q$31)-MIN(ROW($Q$7:$Q$31))+1,""),""),ROW()-ROW(A$33)+1)))," "),"")</f>
+        <f t="array" ref="Q46">IFERROR(CONCATENATE((INDEX($T$7:$T$30,SMALL(IF($T$7:$T$30&lt;&gt;"",IF($Q$7:$Q$30&lt;&gt;"",ROW($Q$7:$Q$30)-MIN(ROW($Q$7:$Q$30))+1,""),""),ROW()-ROW(A$32)+1)))," "),"")</f>
         <v>0</v>
       </c>
       <c r="R46">
-        <f t="array" ref="R46">IFERROR(CONCATENATE(TEXT(INDEX($Q$7:$Q$31,SMALL(IF($T$7:$T$31&lt;&gt;"",IF($Q$7:$Q$31&lt;&gt;"",ROW($Q$7:$Q$31)-MIN(ROW($Q$7:$Q$31))+1,""),""),ROW()-ROW(A$33)+1)),"##0")," "),"")</f>
+        <f t="array" ref="R46">IFERROR(CONCATENATE(TEXT(INDEX($Q$7:$Q$30,SMALL(IF($T$7:$T$30&lt;&gt;"",IF($Q$7:$Q$30&lt;&gt;"",ROW($Q$7:$Q$30)-MIN(ROW($Q$7:$Q$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0")," "),"")</f>
         <v>0</v>
       </c>
       <c r="S46">
-        <f t="array" ref="S46">IFERROR(CONCATENATE((INDEX($A$7:$A$31,SMALL(IF($T$7:$T$31&lt;&gt;"",IF($Q$7:$Q$31&lt;&gt;"",ROW($Q$7:$Q$31)-MIN(ROW($Q$7:$Q$31))+1,""),""),ROW()-ROW(A$33)+1))),),"")</f>
+        <f t="array" ref="S46">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($T$7:$T$30&lt;&gt;"",IF($Q$7:$Q$30&lt;&gt;"",ROW($Q$7:$Q$30)-MIN(ROW($Q$7:$Q$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
         <v>0</v>
       </c>
       <c r="W46">
-        <f t="array" ref="W46">IFERROR(CONCATENATE((INDEX($Z$7:$Z$31,SMALL(IF($Z$7:$Z$31&lt;&gt;"",IF($W$7:$W$31&lt;&gt;"",ROW($W$7:$W$31)-MIN(ROW($W$7:$W$31))+1,""),""),ROW()-ROW(A$33)+1))),","),"")</f>
+        <f t="array" ref="W46">IFERROR(CONCATENATE((INDEX($Z$7:$Z$30,SMALL(IF($Z$7:$Z$30&lt;&gt;"",IF($W$7:$W$30&lt;&gt;"",ROW($W$7:$W$30)-MIN(ROW($W$7:$W$30))+1,""),""),ROW()-ROW(A$32)+1))),","),"")</f>
         <v>0</v>
       </c>
       <c r="X46">
-        <f t="array" ref="X46">IFERROR(CONCATENATE(TEXT(INDEX($W$7:$W$31,SMALL(IF($Z$7:$Z$31&lt;&gt;"",IF($W$7:$W$31&lt;&gt;"",ROW($W$7:$W$31)-MIN(ROW($W$7:$W$31))+1,""),""),ROW()-ROW(A$33)+1)),"##0"),","),"")</f>
+        <f t="array" ref="X46">IFERROR(CONCATENATE(TEXT(INDEX($W$7:$W$30,SMALL(IF($Z$7:$Z$30&lt;&gt;"",IF($W$7:$W$30&lt;&gt;"",ROW($W$7:$W$30)-MIN(ROW($W$7:$W$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0"),","),"")</f>
         <v>0</v>
       </c>
       <c r="Y46">
-        <f t="array" ref="Y46">IFERROR(CONCATENATE((INDEX($A$7:$A$31,SMALL(IF($Z$7:$Z$31&lt;&gt;"",IF($W$7:$W$31&lt;&gt;"",ROW($W$7:$W$31)-MIN(ROW($W$7:$W$31))+1,""),""),ROW()-ROW(A$33)+1))),),"")</f>
+        <f t="array" ref="Y46">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($Z$7:$Z$30&lt;&gt;"",IF($W$7:$W$30&lt;&gt;"",ROW($W$7:$W$30)-MIN(ROW($W$7:$W$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="47" spans="11:25">
       <c r="K47">
-        <f t="array" ref="K47">IFERROR(CONCATENATE(TEXT(INDEX($K$7:$K$31,SMALL(IF($N$7:$N$31&lt;&gt;"",IF($K$7:$K$31&lt;&gt;"",ROW($K$7:$K$31)-MIN(ROW($K$7:$K$31))+1,""),""),ROW()-ROW(A$33)+1)),"##0"),","),"")</f>
+        <f t="array" ref="K47">IFERROR(CONCATENATE(TEXT(INDEX($K$7:$K$30,SMALL(IF($N$7:$N$30&lt;&gt;"",IF($K$7:$K$30&lt;&gt;"",ROW($K$7:$K$30)-MIN(ROW($K$7:$K$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0"),","),"")</f>
         <v>0</v>
       </c>
       <c r="L47">
-        <f t="array" ref="L47">IFERROR(CONCATENATE((INDEX($N$7:$N$31,SMALL(IF($N$7:$N$31&lt;&gt;"",IF($K$7:$K$31&lt;&gt;"",ROW($K$7:$K$31)-MIN(ROW($K$7:$K$31))+1,""),""),ROW()-ROW(A$33)+1))),","),"")</f>
+        <f t="array" ref="L47">IFERROR(CONCATENATE((INDEX($N$7:$N$30,SMALL(IF($N$7:$N$30&lt;&gt;"",IF($K$7:$K$30&lt;&gt;"",ROW($K$7:$K$30)-MIN(ROW($K$7:$K$30))+1,""),""),ROW()-ROW(A$32)+1))),","),"")</f>
         <v>0</v>
       </c>
       <c r="M47">
-        <f t="array" ref="M47">IFERROR(CONCATENATE((INDEX($A$7:$A$31,SMALL(IF($N$7:$N$31&lt;&gt;"",IF($K$7:$K$31&lt;&gt;"",ROW($K$7:$K$31)-MIN(ROW($K$7:$K$31))+1,""),""),ROW()-ROW(A$33)+1))),),"")</f>
+        <f t="array" ref="M47">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($N$7:$N$30&lt;&gt;"",IF($K$7:$K$30&lt;&gt;"",ROW($K$7:$K$30)-MIN(ROW($K$7:$K$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
         <v>0</v>
       </c>
       <c r="Q47">
-        <f t="array" ref="Q47">IFERROR(CONCATENATE((INDEX($T$7:$T$31,SMALL(IF($T$7:$T$31&lt;&gt;"",IF($Q$7:$Q$31&lt;&gt;"",ROW($Q$7:$Q$31)-MIN(ROW($Q$7:$Q$31))+1,""),""),ROW()-ROW(A$33)+1)))," "),"")</f>
+        <f t="array" ref="Q47">IFERROR(CONCATENATE((INDEX($T$7:$T$30,SMALL(IF($T$7:$T$30&lt;&gt;"",IF($Q$7:$Q$30&lt;&gt;"",ROW($Q$7:$Q$30)-MIN(ROW($Q$7:$Q$30))+1,""),""),ROW()-ROW(A$32)+1)))," "),"")</f>
         <v>0</v>
       </c>
       <c r="R47">
-        <f t="array" ref="R47">IFERROR(CONCATENATE(TEXT(INDEX($Q$7:$Q$31,SMALL(IF($T$7:$T$31&lt;&gt;"",IF($Q$7:$Q$31&lt;&gt;"",ROW($Q$7:$Q$31)-MIN(ROW($Q$7:$Q$31))+1,""),""),ROW()-ROW(A$33)+1)),"##0")," "),"")</f>
+        <f t="array" ref="R47">IFERROR(CONCATENATE(TEXT(INDEX($Q$7:$Q$30,SMALL(IF($T$7:$T$30&lt;&gt;"",IF($Q$7:$Q$30&lt;&gt;"",ROW($Q$7:$Q$30)-MIN(ROW($Q$7:$Q$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0")," "),"")</f>
         <v>0</v>
       </c>
       <c r="S47">
-        <f t="array" ref="S47">IFERROR(CONCATENATE((INDEX($A$7:$A$31,SMALL(IF($T$7:$T$31&lt;&gt;"",IF($Q$7:$Q$31&lt;&gt;"",ROW($Q$7:$Q$31)-MIN(ROW($Q$7:$Q$31))+1,""),""),ROW()-ROW(A$33)+1))),),"")</f>
+        <f t="array" ref="S47">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($T$7:$T$30&lt;&gt;"",IF($Q$7:$Q$30&lt;&gt;"",ROW($Q$7:$Q$30)-MIN(ROW($Q$7:$Q$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
         <v>0</v>
       </c>
       <c r="W47">
-        <f t="array" ref="W47">IFERROR(CONCATENATE((INDEX($Z$7:$Z$31,SMALL(IF($Z$7:$Z$31&lt;&gt;"",IF($W$7:$W$31&lt;&gt;"",ROW($W$7:$W$31)-MIN(ROW($W$7:$W$31))+1,""),""),ROW()-ROW(A$33)+1))),","),"")</f>
+        <f t="array" ref="W47">IFERROR(CONCATENATE((INDEX($Z$7:$Z$30,SMALL(IF($Z$7:$Z$30&lt;&gt;"",IF($W$7:$W$30&lt;&gt;"",ROW($W$7:$W$30)-MIN(ROW($W$7:$W$30))+1,""),""),ROW()-ROW(A$32)+1))),","),"")</f>
         <v>0</v>
       </c>
       <c r="X47">
-        <f t="array" ref="X47">IFERROR(CONCATENATE(TEXT(INDEX($W$7:$W$31,SMALL(IF($Z$7:$Z$31&lt;&gt;"",IF($W$7:$W$31&lt;&gt;"",ROW($W$7:$W$31)-MIN(ROW($W$7:$W$31))+1,""),""),ROW()-ROW(A$33)+1)),"##0"),","),"")</f>
+        <f t="array" ref="X47">IFERROR(CONCATENATE(TEXT(INDEX($W$7:$W$30,SMALL(IF($Z$7:$Z$30&lt;&gt;"",IF($W$7:$W$30&lt;&gt;"",ROW($W$7:$W$30)-MIN(ROW($W$7:$W$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0"),","),"")</f>
         <v>0</v>
       </c>
       <c r="Y47">
-        <f t="array" ref="Y47">IFERROR(CONCATENATE((INDEX($A$7:$A$31,SMALL(IF($Z$7:$Z$31&lt;&gt;"",IF($W$7:$W$31&lt;&gt;"",ROW($W$7:$W$31)-MIN(ROW($W$7:$W$31))+1,""),""),ROW()-ROW(A$33)+1))),),"")</f>
+        <f t="array" ref="Y47">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($Z$7:$Z$30&lt;&gt;"",IF($W$7:$W$30&lt;&gt;"",ROW($W$7:$W$30)-MIN(ROW($W$7:$W$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="48" spans="11:25">
       <c r="K48">
-        <f t="array" ref="K48">IFERROR(CONCATENATE(TEXT(INDEX($K$7:$K$31,SMALL(IF($N$7:$N$31&lt;&gt;"",IF($K$7:$K$31&lt;&gt;"",ROW($K$7:$K$31)-MIN(ROW($K$7:$K$31))+1,""),""),ROW()-ROW(A$33)+1)),"##0"),","),"")</f>
+        <f t="array" ref="K48">IFERROR(CONCATENATE(TEXT(INDEX($K$7:$K$30,SMALL(IF($N$7:$N$30&lt;&gt;"",IF($K$7:$K$30&lt;&gt;"",ROW($K$7:$K$30)-MIN(ROW($K$7:$K$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0"),","),"")</f>
         <v>0</v>
       </c>
       <c r="L48">
-        <f t="array" ref="L48">IFERROR(CONCATENATE((INDEX($N$7:$N$31,SMALL(IF($N$7:$N$31&lt;&gt;"",IF($K$7:$K$31&lt;&gt;"",ROW($K$7:$K$31)-MIN(ROW($K$7:$K$31))+1,""),""),ROW()-ROW(A$33)+1))),","),"")</f>
+        <f t="array" ref="L48">IFERROR(CONCATENATE((INDEX($N$7:$N$30,SMALL(IF($N$7:$N$30&lt;&gt;"",IF($K$7:$K$30&lt;&gt;"",ROW($K$7:$K$30)-MIN(ROW($K$7:$K$30))+1,""),""),ROW()-ROW(A$32)+1))),","),"")</f>
         <v>0</v>
       </c>
       <c r="M48">
-        <f t="array" ref="M48">IFERROR(CONCATENATE((INDEX($A$7:$A$31,SMALL(IF($N$7:$N$31&lt;&gt;"",IF($K$7:$K$31&lt;&gt;"",ROW($K$7:$K$31)-MIN(ROW($K$7:$K$31))+1,""),""),ROW()-ROW(A$33)+1))),),"")</f>
+        <f t="array" ref="M48">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($N$7:$N$30&lt;&gt;"",IF($K$7:$K$30&lt;&gt;"",ROW($K$7:$K$30)-MIN(ROW($K$7:$K$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
         <v>0</v>
       </c>
       <c r="Q48">
-        <f t="array" ref="Q48">IFERROR(CONCATENATE((INDEX($T$7:$T$31,SMALL(IF($T$7:$T$31&lt;&gt;"",IF($Q$7:$Q$31&lt;&gt;"",ROW($Q$7:$Q$31)-MIN(ROW($Q$7:$Q$31))+1,""),""),ROW()-ROW(A$33)+1)))," "),"")</f>
+        <f t="array" ref="Q48">IFERROR(CONCATENATE((INDEX($T$7:$T$30,SMALL(IF($T$7:$T$30&lt;&gt;"",IF($Q$7:$Q$30&lt;&gt;"",ROW($Q$7:$Q$30)-MIN(ROW($Q$7:$Q$30))+1,""),""),ROW()-ROW(A$32)+1)))," "),"")</f>
         <v>0</v>
       </c>
       <c r="R48">
-        <f t="array" ref="R48">IFERROR(CONCATENATE(TEXT(INDEX($Q$7:$Q$31,SMALL(IF($T$7:$T$31&lt;&gt;"",IF($Q$7:$Q$31&lt;&gt;"",ROW($Q$7:$Q$31)-MIN(ROW($Q$7:$Q$31))+1,""),""),ROW()-ROW(A$33)+1)),"##0")," "),"")</f>
+        <f t="array" ref="R48">IFERROR(CONCATENATE(TEXT(INDEX($Q$7:$Q$30,SMALL(IF($T$7:$T$30&lt;&gt;"",IF($Q$7:$Q$30&lt;&gt;"",ROW($Q$7:$Q$30)-MIN(ROW($Q$7:$Q$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0")," "),"")</f>
         <v>0</v>
       </c>
       <c r="S48">
-        <f t="array" ref="S48">IFERROR(CONCATENATE((INDEX($A$7:$A$31,SMALL(IF($T$7:$T$31&lt;&gt;"",IF($Q$7:$Q$31&lt;&gt;"",ROW($Q$7:$Q$31)-MIN(ROW($Q$7:$Q$31))+1,""),""),ROW()-ROW(A$33)+1))),),"")</f>
+        <f t="array" ref="S48">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($T$7:$T$30&lt;&gt;"",IF($Q$7:$Q$30&lt;&gt;"",ROW($Q$7:$Q$30)-MIN(ROW($Q$7:$Q$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
         <v>0</v>
       </c>
       <c r="W48">
-        <f t="array" ref="W48">IFERROR(CONCATENATE((INDEX($Z$7:$Z$31,SMALL(IF($Z$7:$Z$31&lt;&gt;"",IF($W$7:$W$31&lt;&gt;"",ROW($W$7:$W$31)-MIN(ROW($W$7:$W$31))+1,""),""),ROW()-ROW(A$33)+1))),","),"")</f>
+        <f t="array" ref="W48">IFERROR(CONCATENATE((INDEX($Z$7:$Z$30,SMALL(IF($Z$7:$Z$30&lt;&gt;"",IF($W$7:$W$30&lt;&gt;"",ROW($W$7:$W$30)-MIN(ROW($W$7:$W$30))+1,""),""),ROW()-ROW(A$32)+1))),","),"")</f>
         <v>0</v>
       </c>
       <c r="X48">
-        <f t="array" ref="X48">IFERROR(CONCATENATE(TEXT(INDEX($W$7:$W$31,SMALL(IF($Z$7:$Z$31&lt;&gt;"",IF($W$7:$W$31&lt;&gt;"",ROW($W$7:$W$31)-MIN(ROW($W$7:$W$31))+1,""),""),ROW()-ROW(A$33)+1)),"##0"),","),"")</f>
+        <f t="array" ref="X48">IFERROR(CONCATENATE(TEXT(INDEX($W$7:$W$30,SMALL(IF($Z$7:$Z$30&lt;&gt;"",IF($W$7:$W$30&lt;&gt;"",ROW($W$7:$W$30)-MIN(ROW($W$7:$W$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0"),","),"")</f>
         <v>0</v>
       </c>
       <c r="Y48">
-        <f t="array" ref="Y48">IFERROR(CONCATENATE((INDEX($A$7:$A$31,SMALL(IF($Z$7:$Z$31&lt;&gt;"",IF($W$7:$W$31&lt;&gt;"",ROW($W$7:$W$31)-MIN(ROW($W$7:$W$31))+1,""),""),ROW()-ROW(A$33)+1))),),"")</f>
+        <f t="array" ref="Y48">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($Z$7:$Z$30&lt;&gt;"",IF($W$7:$W$30&lt;&gt;"",ROW($W$7:$W$30)-MIN(ROW($W$7:$W$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="49" spans="11:25">
       <c r="K49">
-        <f t="array" ref="K49">IFERROR(CONCATENATE(TEXT(INDEX($K$7:$K$31,SMALL(IF($N$7:$N$31&lt;&gt;"",IF($K$7:$K$31&lt;&gt;"",ROW($K$7:$K$31)-MIN(ROW($K$7:$K$31))+1,""),""),ROW()-ROW(A$33)+1)),"##0"),","),"")</f>
+        <f t="array" ref="K49">IFERROR(CONCATENATE(TEXT(INDEX($K$7:$K$30,SMALL(IF($N$7:$N$30&lt;&gt;"",IF($K$7:$K$30&lt;&gt;"",ROW($K$7:$K$30)-MIN(ROW($K$7:$K$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0"),","),"")</f>
         <v>0</v>
       </c>
       <c r="L49">
-        <f t="array" ref="L49">IFERROR(CONCATENATE((INDEX($N$7:$N$31,SMALL(IF($N$7:$N$31&lt;&gt;"",IF($K$7:$K$31&lt;&gt;"",ROW($K$7:$K$31)-MIN(ROW($K$7:$K$31))+1,""),""),ROW()-ROW(A$33)+1))),","),"")</f>
+        <f t="array" ref="L49">IFERROR(CONCATENATE((INDEX($N$7:$N$30,SMALL(IF($N$7:$N$30&lt;&gt;"",IF($K$7:$K$30&lt;&gt;"",ROW($K$7:$K$30)-MIN(ROW($K$7:$K$30))+1,""),""),ROW()-ROW(A$32)+1))),","),"")</f>
         <v>0</v>
       </c>
       <c r="M49">
-        <f t="array" ref="M49">IFERROR(CONCATENATE((INDEX($A$7:$A$31,SMALL(IF($N$7:$N$31&lt;&gt;"",IF($K$7:$K$31&lt;&gt;"",ROW($K$7:$K$31)-MIN(ROW($K$7:$K$31))+1,""),""),ROW()-ROW(A$33)+1))),),"")</f>
+        <f t="array" ref="M49">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($N$7:$N$30&lt;&gt;"",IF($K$7:$K$30&lt;&gt;"",ROW($K$7:$K$30)-MIN(ROW($K$7:$K$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
         <v>0</v>
       </c>
       <c r="Q49">
-        <f t="array" ref="Q49">IFERROR(CONCATENATE((INDEX($T$7:$T$31,SMALL(IF($T$7:$T$31&lt;&gt;"",IF($Q$7:$Q$31&lt;&gt;"",ROW($Q$7:$Q$31)-MIN(ROW($Q$7:$Q$31))+1,""),""),ROW()-ROW(A$33)+1)))," "),"")</f>
+        <f t="array" ref="Q49">IFERROR(CONCATENATE((INDEX($T$7:$T$30,SMALL(IF($T$7:$T$30&lt;&gt;"",IF($Q$7:$Q$30&lt;&gt;"",ROW($Q$7:$Q$30)-MIN(ROW($Q$7:$Q$30))+1,""),""),ROW()-ROW(A$32)+1)))," "),"")</f>
         <v>0</v>
       </c>
       <c r="R49">
-        <f t="array" ref="R49">IFERROR(CONCATENATE(TEXT(INDEX($Q$7:$Q$31,SMALL(IF($T$7:$T$31&lt;&gt;"",IF($Q$7:$Q$31&lt;&gt;"",ROW($Q$7:$Q$31)-MIN(ROW($Q$7:$Q$31))+1,""),""),ROW()-ROW(A$33)+1)),"##0")," "),"")</f>
+        <f t="array" ref="R49">IFERROR(CONCATENATE(TEXT(INDEX($Q$7:$Q$30,SMALL(IF($T$7:$T$30&lt;&gt;"",IF($Q$7:$Q$30&lt;&gt;"",ROW($Q$7:$Q$30)-MIN(ROW($Q$7:$Q$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0")," "),"")</f>
         <v>0</v>
       </c>
       <c r="S49">
-        <f t="array" ref="S49">IFERROR(CONCATENATE((INDEX($A$7:$A$31,SMALL(IF($T$7:$T$31&lt;&gt;"",IF($Q$7:$Q$31&lt;&gt;"",ROW($Q$7:$Q$31)-MIN(ROW($Q$7:$Q$31))+1,""),""),ROW()-ROW(A$33)+1))),),"")</f>
+        <f t="array" ref="S49">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($T$7:$T$30&lt;&gt;"",IF($Q$7:$Q$30&lt;&gt;"",ROW($Q$7:$Q$30)-MIN(ROW($Q$7:$Q$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
         <v>0</v>
       </c>
       <c r="W49">
-        <f t="array" ref="W49">IFERROR(CONCATENATE((INDEX($Z$7:$Z$31,SMALL(IF($Z$7:$Z$31&lt;&gt;"",IF($W$7:$W$31&lt;&gt;"",ROW($W$7:$W$31)-MIN(ROW($W$7:$W$31))+1,""),""),ROW()-ROW(A$33)+1))),","),"")</f>
+        <f t="array" ref="W49">IFERROR(CONCATENATE((INDEX($Z$7:$Z$30,SMALL(IF($Z$7:$Z$30&lt;&gt;"",IF($W$7:$W$30&lt;&gt;"",ROW($W$7:$W$30)-MIN(ROW($W$7:$W$30))+1,""),""),ROW()-ROW(A$32)+1))),","),"")</f>
         <v>0</v>
       </c>
       <c r="X49">
-        <f t="array" ref="X49">IFERROR(CONCATENATE(TEXT(INDEX($W$7:$W$31,SMALL(IF($Z$7:$Z$31&lt;&gt;"",IF($W$7:$W$31&lt;&gt;"",ROW($W$7:$W$31)-MIN(ROW($W$7:$W$31))+1,""),""),ROW()-ROW(A$33)+1)),"##0"),","),"")</f>
+        <f t="array" ref="X49">IFERROR(CONCATENATE(TEXT(INDEX($W$7:$W$30,SMALL(IF($Z$7:$Z$30&lt;&gt;"",IF($W$7:$W$30&lt;&gt;"",ROW($W$7:$W$30)-MIN(ROW($W$7:$W$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0"),","),"")</f>
         <v>0</v>
       </c>
       <c r="Y49">
-        <f t="array" ref="Y49">IFERROR(CONCATENATE((INDEX($A$7:$A$31,SMALL(IF($Z$7:$Z$31&lt;&gt;"",IF($W$7:$W$31&lt;&gt;"",ROW($W$7:$W$31)-MIN(ROW($W$7:$W$31))+1,""),""),ROW()-ROW(A$33)+1))),),"")</f>
+        <f t="array" ref="Y49">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($Z$7:$Z$30&lt;&gt;"",IF($W$7:$W$30&lt;&gt;"",ROW($W$7:$W$30)-MIN(ROW($W$7:$W$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="50" spans="11:25">
       <c r="K50">
-        <f t="array" ref="K50">IFERROR(CONCATENATE(TEXT(INDEX($K$7:$K$31,SMALL(IF($N$7:$N$31&lt;&gt;"",IF($K$7:$K$31&lt;&gt;"",ROW($K$7:$K$31)-MIN(ROW($K$7:$K$31))+1,""),""),ROW()-ROW(A$33)+1)),"##0"),","),"")</f>
+        <f t="array" ref="K50">IFERROR(CONCATENATE(TEXT(INDEX($K$7:$K$30,SMALL(IF($N$7:$N$30&lt;&gt;"",IF($K$7:$K$30&lt;&gt;"",ROW($K$7:$K$30)-MIN(ROW($K$7:$K$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0"),","),"")</f>
         <v>0</v>
       </c>
       <c r="L50">
-        <f t="array" ref="L50">IFERROR(CONCATENATE((INDEX($N$7:$N$31,SMALL(IF($N$7:$N$31&lt;&gt;"",IF($K$7:$K$31&lt;&gt;"",ROW($K$7:$K$31)-MIN(ROW($K$7:$K$31))+1,""),""),ROW()-ROW(A$33)+1))),","),"")</f>
+        <f t="array" ref="L50">IFERROR(CONCATENATE((INDEX($N$7:$N$30,SMALL(IF($N$7:$N$30&lt;&gt;"",IF($K$7:$K$30&lt;&gt;"",ROW($K$7:$K$30)-MIN(ROW($K$7:$K$30))+1,""),""),ROW()-ROW(A$32)+1))),","),"")</f>
         <v>0</v>
       </c>
       <c r="M50">
-        <f t="array" ref="M50">IFERROR(CONCATENATE((INDEX($A$7:$A$31,SMALL(IF($N$7:$N$31&lt;&gt;"",IF($K$7:$K$31&lt;&gt;"",ROW($K$7:$K$31)-MIN(ROW($K$7:$K$31))+1,""),""),ROW()-ROW(A$33)+1))),),"")</f>
+        <f t="array" ref="M50">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($N$7:$N$30&lt;&gt;"",IF($K$7:$K$30&lt;&gt;"",ROW($K$7:$K$30)-MIN(ROW($K$7:$K$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
         <v>0</v>
       </c>
       <c r="Q50">
-        <f t="array" ref="Q50">IFERROR(CONCATENATE((INDEX($T$7:$T$31,SMALL(IF($T$7:$T$31&lt;&gt;"",IF($Q$7:$Q$31&lt;&gt;"",ROW($Q$7:$Q$31)-MIN(ROW($Q$7:$Q$31))+1,""),""),ROW()-ROW(A$33)+1)))," "),"")</f>
+        <f t="array" ref="Q50">IFERROR(CONCATENATE((INDEX($T$7:$T$30,SMALL(IF($T$7:$T$30&lt;&gt;"",IF($Q$7:$Q$30&lt;&gt;"",ROW($Q$7:$Q$30)-MIN(ROW($Q$7:$Q$30))+1,""),""),ROW()-ROW(A$32)+1)))," "),"")</f>
         <v>0</v>
       </c>
       <c r="R50">
-        <f t="array" ref="R50">IFERROR(CONCATENATE(TEXT(INDEX($Q$7:$Q$31,SMALL(IF($T$7:$T$31&lt;&gt;"",IF($Q$7:$Q$31&lt;&gt;"",ROW($Q$7:$Q$31)-MIN(ROW($Q$7:$Q$31))+1,""),""),ROW()-ROW(A$33)+1)),"##0")," "),"")</f>
+        <f t="array" ref="R50">IFERROR(CONCATENATE(TEXT(INDEX($Q$7:$Q$30,SMALL(IF($T$7:$T$30&lt;&gt;"",IF($Q$7:$Q$30&lt;&gt;"",ROW($Q$7:$Q$30)-MIN(ROW($Q$7:$Q$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0")," "),"")</f>
         <v>0</v>
       </c>
       <c r="S50">
-        <f t="array" ref="S50">IFERROR(CONCATENATE((INDEX($A$7:$A$31,SMALL(IF($T$7:$T$31&lt;&gt;"",IF($Q$7:$Q$31&lt;&gt;"",ROW($Q$7:$Q$31)-MIN(ROW($Q$7:$Q$31))+1,""),""),ROW()-ROW(A$33)+1))),),"")</f>
+        <f t="array" ref="S50">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($T$7:$T$30&lt;&gt;"",IF($Q$7:$Q$30&lt;&gt;"",ROW($Q$7:$Q$30)-MIN(ROW($Q$7:$Q$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
         <v>0</v>
       </c>
       <c r="W50">
-        <f t="array" ref="W50">IFERROR(CONCATENATE((INDEX($Z$7:$Z$31,SMALL(IF($Z$7:$Z$31&lt;&gt;"",IF($W$7:$W$31&lt;&gt;"",ROW($W$7:$W$31)-MIN(ROW($W$7:$W$31))+1,""),""),ROW()-ROW(A$33)+1))),","),"")</f>
+        <f t="array" ref="W50">IFERROR(CONCATENATE((INDEX($Z$7:$Z$30,SMALL(IF($Z$7:$Z$30&lt;&gt;"",IF($W$7:$W$30&lt;&gt;"",ROW($W$7:$W$30)-MIN(ROW($W$7:$W$30))+1,""),""),ROW()-ROW(A$32)+1))),","),"")</f>
         <v>0</v>
       </c>
       <c r="X50">
-        <f t="array" ref="X50">IFERROR(CONCATENATE(TEXT(INDEX($W$7:$W$31,SMALL(IF($Z$7:$Z$31&lt;&gt;"",IF($W$7:$W$31&lt;&gt;"",ROW($W$7:$W$31)-MIN(ROW($W$7:$W$31))+1,""),""),ROW()-ROW(A$33)+1)),"##0"),","),"")</f>
+        <f t="array" ref="X50">IFERROR(CONCATENATE(TEXT(INDEX($W$7:$W$30,SMALL(IF($Z$7:$Z$30&lt;&gt;"",IF($W$7:$W$30&lt;&gt;"",ROW($W$7:$W$30)-MIN(ROW($W$7:$W$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0"),","),"")</f>
         <v>0</v>
       </c>
       <c r="Y50">
-        <f t="array" ref="Y50">IFERROR(CONCATENATE((INDEX($A$7:$A$31,SMALL(IF($Z$7:$Z$31&lt;&gt;"",IF($W$7:$W$31&lt;&gt;"",ROW($W$7:$W$31)-MIN(ROW($W$7:$W$31))+1,""),""),ROW()-ROW(A$33)+1))),),"")</f>
+        <f t="array" ref="Y50">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($Z$7:$Z$30&lt;&gt;"",IF($W$7:$W$30&lt;&gt;"",ROW($W$7:$W$30)-MIN(ROW($W$7:$W$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="51" spans="11:25">
       <c r="K51">
-        <f t="array" ref="K51">IFERROR(CONCATENATE(TEXT(INDEX($K$7:$K$31,SMALL(IF($N$7:$N$31&lt;&gt;"",IF($K$7:$K$31&lt;&gt;"",ROW($K$7:$K$31)-MIN(ROW($K$7:$K$31))+1,""),""),ROW()-ROW(A$33)+1)),"##0"),","),"")</f>
+        <f t="array" ref="K51">IFERROR(CONCATENATE(TEXT(INDEX($K$7:$K$30,SMALL(IF($N$7:$N$30&lt;&gt;"",IF($K$7:$K$30&lt;&gt;"",ROW($K$7:$K$30)-MIN(ROW($K$7:$K$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0"),","),"")</f>
         <v>0</v>
       </c>
       <c r="L51">
-        <f t="array" ref="L51">IFERROR(CONCATENATE((INDEX($N$7:$N$31,SMALL(IF($N$7:$N$31&lt;&gt;"",IF($K$7:$K$31&lt;&gt;"",ROW($K$7:$K$31)-MIN(ROW($K$7:$K$31))+1,""),""),ROW()-ROW(A$33)+1))),","),"")</f>
+        <f t="array" ref="L51">IFERROR(CONCATENATE((INDEX($N$7:$N$30,SMALL(IF($N$7:$N$30&lt;&gt;"",IF($K$7:$K$30&lt;&gt;"",ROW($K$7:$K$30)-MIN(ROW($K$7:$K$30))+1,""),""),ROW()-ROW(A$32)+1))),","),"")</f>
         <v>0</v>
       </c>
       <c r="M51">
-        <f t="array" ref="M51">IFERROR(CONCATENATE((INDEX($A$7:$A$31,SMALL(IF($N$7:$N$31&lt;&gt;"",IF($K$7:$K$31&lt;&gt;"",ROW($K$7:$K$31)-MIN(ROW($K$7:$K$31))+1,""),""),ROW()-ROW(A$33)+1))),),"")</f>
+        <f t="array" ref="M51">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($N$7:$N$30&lt;&gt;"",IF($K$7:$K$30&lt;&gt;"",ROW($K$7:$K$30)-MIN(ROW($K$7:$K$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
         <v>0</v>
       </c>
       <c r="Q51">
-        <f t="array" ref="Q51">IFERROR(CONCATENATE((INDEX($T$7:$T$31,SMALL(IF($T$7:$T$31&lt;&gt;"",IF($Q$7:$Q$31&lt;&gt;"",ROW($Q$7:$Q$31)-MIN(ROW($Q$7:$Q$31))+1,""),""),ROW()-ROW(A$33)+1)))," "),"")</f>
+        <f t="array" ref="Q51">IFERROR(CONCATENATE((INDEX($T$7:$T$30,SMALL(IF($T$7:$T$30&lt;&gt;"",IF($Q$7:$Q$30&lt;&gt;"",ROW($Q$7:$Q$30)-MIN(ROW($Q$7:$Q$30))+1,""),""),ROW()-ROW(A$32)+1)))," "),"")</f>
         <v>0</v>
       </c>
       <c r="R51">
-        <f t="array" ref="R51">IFERROR(CONCATENATE(TEXT(INDEX($Q$7:$Q$31,SMALL(IF($T$7:$T$31&lt;&gt;"",IF($Q$7:$Q$31&lt;&gt;"",ROW($Q$7:$Q$31)-MIN(ROW($Q$7:$Q$31))+1,""),""),ROW()-ROW(A$33)+1)),"##0")," "),"")</f>
+        <f t="array" ref="R51">IFERROR(CONCATENATE(TEXT(INDEX($Q$7:$Q$30,SMALL(IF($T$7:$T$30&lt;&gt;"",IF($Q$7:$Q$30&lt;&gt;"",ROW($Q$7:$Q$30)-MIN(ROW($Q$7:$Q$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0")," "),"")</f>
         <v>0</v>
       </c>
       <c r="S51">
-        <f t="array" ref="S51">IFERROR(CONCATENATE((INDEX($A$7:$A$31,SMALL(IF($T$7:$T$31&lt;&gt;"",IF($Q$7:$Q$31&lt;&gt;"",ROW($Q$7:$Q$31)-MIN(ROW($Q$7:$Q$31))+1,""),""),ROW()-ROW(A$33)+1))),),"")</f>
+        <f t="array" ref="S51">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($T$7:$T$30&lt;&gt;"",IF($Q$7:$Q$30&lt;&gt;"",ROW($Q$7:$Q$30)-MIN(ROW($Q$7:$Q$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
         <v>0</v>
       </c>
       <c r="W51">
-        <f t="array" ref="W51">IFERROR(CONCATENATE((INDEX($Z$7:$Z$31,SMALL(IF($Z$7:$Z$31&lt;&gt;"",IF($W$7:$W$31&lt;&gt;"",ROW($W$7:$W$31)-MIN(ROW($W$7:$W$31))+1,""),""),ROW()-ROW(A$33)+1))),","),"")</f>
+        <f t="array" ref="W51">IFERROR(CONCATENATE((INDEX($Z$7:$Z$30,SMALL(IF($Z$7:$Z$30&lt;&gt;"",IF($W$7:$W$30&lt;&gt;"",ROW($W$7:$W$30)-MIN(ROW($W$7:$W$30))+1,""),""),ROW()-ROW(A$32)+1))),","),"")</f>
         <v>0</v>
       </c>
       <c r="X51">
-        <f t="array" ref="X51">IFERROR(CONCATENATE(TEXT(INDEX($W$7:$W$31,SMALL(IF($Z$7:$Z$31&lt;&gt;"",IF($W$7:$W$31&lt;&gt;"",ROW($W$7:$W$31)-MIN(ROW($W$7:$W$31))+1,""),""),ROW()-ROW(A$33)+1)),"##0"),","),"")</f>
+        <f t="array" ref="X51">IFERROR(CONCATENATE(TEXT(INDEX($W$7:$W$30,SMALL(IF($Z$7:$Z$30&lt;&gt;"",IF($W$7:$W$30&lt;&gt;"",ROW($W$7:$W$30)-MIN(ROW($W$7:$W$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0"),","),"")</f>
         <v>0</v>
       </c>
       <c r="Y51">
-        <f t="array" ref="Y51">IFERROR(CONCATENATE((INDEX($A$7:$A$31,SMALL(IF($Z$7:$Z$31&lt;&gt;"",IF($W$7:$W$31&lt;&gt;"",ROW($W$7:$W$31)-MIN(ROW($W$7:$W$31))+1,""),""),ROW()-ROW(A$33)+1))),),"")</f>
+        <f t="array" ref="Y51">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($Z$7:$Z$30&lt;&gt;"",IF($W$7:$W$30&lt;&gt;"",ROW($W$7:$W$30)-MIN(ROW($W$7:$W$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="52" spans="11:25">
       <c r="K52">
-        <f t="array" ref="K52">IFERROR(CONCATENATE(TEXT(INDEX($K$7:$K$31,SMALL(IF($N$7:$N$31&lt;&gt;"",IF($K$7:$K$31&lt;&gt;"",ROW($K$7:$K$31)-MIN(ROW($K$7:$K$31))+1,""),""),ROW()-ROW(A$33)+1)),"##0"),","),"")</f>
+        <f t="array" ref="K52">IFERROR(CONCATENATE(TEXT(INDEX($K$7:$K$30,SMALL(IF($N$7:$N$30&lt;&gt;"",IF($K$7:$K$30&lt;&gt;"",ROW($K$7:$K$30)-MIN(ROW($K$7:$K$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0"),","),"")</f>
         <v>0</v>
       </c>
       <c r="L52">
-        <f t="array" ref="L52">IFERROR(CONCATENATE((INDEX($N$7:$N$31,SMALL(IF($N$7:$N$31&lt;&gt;"",IF($K$7:$K$31&lt;&gt;"",ROW($K$7:$K$31)-MIN(ROW($K$7:$K$31))+1,""),""),ROW()-ROW(A$33)+1))),","),"")</f>
+        <f t="array" ref="L52">IFERROR(CONCATENATE((INDEX($N$7:$N$30,SMALL(IF($N$7:$N$30&lt;&gt;"",IF($K$7:$K$30&lt;&gt;"",ROW($K$7:$K$30)-MIN(ROW($K$7:$K$30))+1,""),""),ROW()-ROW(A$32)+1))),","),"")</f>
         <v>0</v>
       </c>
       <c r="M52">
-        <f t="array" ref="M52">IFERROR(CONCATENATE((INDEX($A$7:$A$31,SMALL(IF($N$7:$N$31&lt;&gt;"",IF($K$7:$K$31&lt;&gt;"",ROW($K$7:$K$31)-MIN(ROW($K$7:$K$31))+1,""),""),ROW()-ROW(A$33)+1))),),"")</f>
+        <f t="array" ref="M52">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($N$7:$N$30&lt;&gt;"",IF($K$7:$K$30&lt;&gt;"",ROW($K$7:$K$30)-MIN(ROW($K$7:$K$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
         <v>0</v>
       </c>
       <c r="Q52">
-        <f t="array" ref="Q52">IFERROR(CONCATENATE((INDEX($T$7:$T$31,SMALL(IF($T$7:$T$31&lt;&gt;"",IF($Q$7:$Q$31&lt;&gt;"",ROW($Q$7:$Q$31)-MIN(ROW($Q$7:$Q$31))+1,""),""),ROW()-ROW(A$33)+1)))," "),"")</f>
+        <f t="array" ref="Q52">IFERROR(CONCATENATE((INDEX($T$7:$T$30,SMALL(IF($T$7:$T$30&lt;&gt;"",IF($Q$7:$Q$30&lt;&gt;"",ROW($Q$7:$Q$30)-MIN(ROW($Q$7:$Q$30))+1,""),""),ROW()-ROW(A$32)+1)))," "),"")</f>
         <v>0</v>
       </c>
       <c r="R52">
-        <f t="array" ref="R52">IFERROR(CONCATENATE(TEXT(INDEX($Q$7:$Q$31,SMALL(IF($T$7:$T$31&lt;&gt;"",IF($Q$7:$Q$31&lt;&gt;"",ROW($Q$7:$Q$31)-MIN(ROW($Q$7:$Q$31))+1,""),""),ROW()-ROW(A$33)+1)),"##0")," "),"")</f>
+        <f t="array" ref="R52">IFERROR(CONCATENATE(TEXT(INDEX($Q$7:$Q$30,SMALL(IF($T$7:$T$30&lt;&gt;"",IF($Q$7:$Q$30&lt;&gt;"",ROW($Q$7:$Q$30)-MIN(ROW($Q$7:$Q$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0")," "),"")</f>
         <v>0</v>
       </c>
       <c r="S52">
-        <f t="array" ref="S52">IFERROR(CONCATENATE((INDEX($A$7:$A$31,SMALL(IF($T$7:$T$31&lt;&gt;"",IF($Q$7:$Q$31&lt;&gt;"",ROW($Q$7:$Q$31)-MIN(ROW($Q$7:$Q$31))+1,""),""),ROW()-ROW(A$33)+1))),),"")</f>
+        <f t="array" ref="S52">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($T$7:$T$30&lt;&gt;"",IF($Q$7:$Q$30&lt;&gt;"",ROW($Q$7:$Q$30)-MIN(ROW($Q$7:$Q$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
         <v>0</v>
       </c>
       <c r="W52">
-        <f t="array" ref="W52">IFERROR(CONCATENATE((INDEX($Z$7:$Z$31,SMALL(IF($Z$7:$Z$31&lt;&gt;"",IF($W$7:$W$31&lt;&gt;"",ROW($W$7:$W$31)-MIN(ROW($W$7:$W$31))+1,""),""),ROW()-ROW(A$33)+1))),","),"")</f>
+        <f t="array" ref="W52">IFERROR(CONCATENATE((INDEX($Z$7:$Z$30,SMALL(IF($Z$7:$Z$30&lt;&gt;"",IF($W$7:$W$30&lt;&gt;"",ROW($W$7:$W$30)-MIN(ROW($W$7:$W$30))+1,""),""),ROW()-ROW(A$32)+1))),","),"")</f>
         <v>0</v>
       </c>
       <c r="X52">
-        <f t="array" ref="X52">IFERROR(CONCATENATE(TEXT(INDEX($W$7:$W$31,SMALL(IF($Z$7:$Z$31&lt;&gt;"",IF($W$7:$W$31&lt;&gt;"",ROW($W$7:$W$31)-MIN(ROW($W$7:$W$31))+1,""),""),ROW()-ROW(A$33)+1)),"##0"),","),"")</f>
+        <f t="array" ref="X52">IFERROR(CONCATENATE(TEXT(INDEX($W$7:$W$30,SMALL(IF($Z$7:$Z$30&lt;&gt;"",IF($W$7:$W$30&lt;&gt;"",ROW($W$7:$W$30)-MIN(ROW($W$7:$W$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0"),","),"")</f>
         <v>0</v>
       </c>
       <c r="Y52">
-        <f t="array" ref="Y52">IFERROR(CONCATENATE((INDEX($A$7:$A$31,SMALL(IF($Z$7:$Z$31&lt;&gt;"",IF($W$7:$W$31&lt;&gt;"",ROW($W$7:$W$31)-MIN(ROW($W$7:$W$31))+1,""),""),ROW()-ROW(A$33)+1))),),"")</f>
+        <f t="array" ref="Y52">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($Z$7:$Z$30&lt;&gt;"",IF($W$7:$W$30&lt;&gt;"",ROW($W$7:$W$30)-MIN(ROW($W$7:$W$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="53" spans="11:25">
       <c r="K53">
-        <f t="array" ref="K53">IFERROR(CONCATENATE(TEXT(INDEX($K$7:$K$31,SMALL(IF($N$7:$N$31&lt;&gt;"",IF($K$7:$K$31&lt;&gt;"",ROW($K$7:$K$31)-MIN(ROW($K$7:$K$31))+1,""),""),ROW()-ROW(A$33)+1)),"##0"),","),"")</f>
+        <f t="array" ref="K53">IFERROR(CONCATENATE(TEXT(INDEX($K$7:$K$30,SMALL(IF($N$7:$N$30&lt;&gt;"",IF($K$7:$K$30&lt;&gt;"",ROW($K$7:$K$30)-MIN(ROW($K$7:$K$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0"),","),"")</f>
         <v>0</v>
       </c>
       <c r="L53">
-        <f t="array" ref="L53">IFERROR(CONCATENATE((INDEX($N$7:$N$31,SMALL(IF($N$7:$N$31&lt;&gt;"",IF($K$7:$K$31&lt;&gt;"",ROW($K$7:$K$31)-MIN(ROW($K$7:$K$31))+1,""),""),ROW()-ROW(A$33)+1))),","),"")</f>
+        <f t="array" ref="L53">IFERROR(CONCATENATE((INDEX($N$7:$N$30,SMALL(IF($N$7:$N$30&lt;&gt;"",IF($K$7:$K$30&lt;&gt;"",ROW($K$7:$K$30)-MIN(ROW($K$7:$K$30))+1,""),""),ROW()-ROW(A$32)+1))),","),"")</f>
         <v>0</v>
       </c>
       <c r="M53">
-        <f t="array" ref="M53">IFERROR(CONCATENATE((INDEX($A$7:$A$31,SMALL(IF($N$7:$N$31&lt;&gt;"",IF($K$7:$K$31&lt;&gt;"",ROW($K$7:$K$31)-MIN(ROW($K$7:$K$31))+1,""),""),ROW()-ROW(A$33)+1))),),"")</f>
+        <f t="array" ref="M53">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($N$7:$N$30&lt;&gt;"",IF($K$7:$K$30&lt;&gt;"",ROW($K$7:$K$30)-MIN(ROW($K$7:$K$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
         <v>0</v>
       </c>
       <c r="Q53">
-        <f t="array" ref="Q53">IFERROR(CONCATENATE((INDEX($T$7:$T$31,SMALL(IF($T$7:$T$31&lt;&gt;"",IF($Q$7:$Q$31&lt;&gt;"",ROW($Q$7:$Q$31)-MIN(ROW($Q$7:$Q$31))+1,""),""),ROW()-ROW(A$33)+1)))," "),"")</f>
+        <f t="array" ref="Q53">IFERROR(CONCATENATE((INDEX($T$7:$T$30,SMALL(IF($T$7:$T$30&lt;&gt;"",IF($Q$7:$Q$30&lt;&gt;"",ROW($Q$7:$Q$30)-MIN(ROW($Q$7:$Q$30))+1,""),""),ROW()-ROW(A$32)+1)))," "),"")</f>
         <v>0</v>
       </c>
       <c r="R53">
-        <f t="array" ref="R53">IFERROR(CONCATENATE(TEXT(INDEX($Q$7:$Q$31,SMALL(IF($T$7:$T$31&lt;&gt;"",IF($Q$7:$Q$31&lt;&gt;"",ROW($Q$7:$Q$31)-MIN(ROW($Q$7:$Q$31))+1,""),""),ROW()-ROW(A$33)+1)),"##0")," "),"")</f>
+        <f t="array" ref="R53">IFERROR(CONCATENATE(TEXT(INDEX($Q$7:$Q$30,SMALL(IF($T$7:$T$30&lt;&gt;"",IF($Q$7:$Q$30&lt;&gt;"",ROW($Q$7:$Q$30)-MIN(ROW($Q$7:$Q$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0")," "),"")</f>
         <v>0</v>
       </c>
       <c r="S53">
-        <f t="array" ref="S53">IFERROR(CONCATENATE((INDEX($A$7:$A$31,SMALL(IF($T$7:$T$31&lt;&gt;"",IF($Q$7:$Q$31&lt;&gt;"",ROW($Q$7:$Q$31)-MIN(ROW($Q$7:$Q$31))+1,""),""),ROW()-ROW(A$33)+1))),),"")</f>
+        <f t="array" ref="S53">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($T$7:$T$30&lt;&gt;"",IF($Q$7:$Q$30&lt;&gt;"",ROW($Q$7:$Q$30)-MIN(ROW($Q$7:$Q$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
         <v>0</v>
       </c>
       <c r="W53">
-        <f t="array" ref="W53">IFERROR(CONCATENATE((INDEX($Z$7:$Z$31,SMALL(IF($Z$7:$Z$31&lt;&gt;"",IF($W$7:$W$31&lt;&gt;"",ROW($W$7:$W$31)-MIN(ROW($W$7:$W$31))+1,""),""),ROW()-ROW(A$33)+1))),","),"")</f>
+        <f t="array" ref="W53">IFERROR(CONCATENATE((INDEX($Z$7:$Z$30,SMALL(IF($Z$7:$Z$30&lt;&gt;"",IF($W$7:$W$30&lt;&gt;"",ROW($W$7:$W$30)-MIN(ROW($W$7:$W$30))+1,""),""),ROW()-ROW(A$32)+1))),","),"")</f>
         <v>0</v>
       </c>
       <c r="X53">
-        <f t="array" ref="X53">IFERROR(CONCATENATE(TEXT(INDEX($W$7:$W$31,SMALL(IF($Z$7:$Z$31&lt;&gt;"",IF($W$7:$W$31&lt;&gt;"",ROW($W$7:$W$31)-MIN(ROW($W$7:$W$31))+1,""),""),ROW()-ROW(A$33)+1)),"##0"),","),"")</f>
+        <f t="array" ref="X53">IFERROR(CONCATENATE(TEXT(INDEX($W$7:$W$30,SMALL(IF($Z$7:$Z$30&lt;&gt;"",IF($W$7:$W$30&lt;&gt;"",ROW($W$7:$W$30)-MIN(ROW($W$7:$W$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0"),","),"")</f>
         <v>0</v>
       </c>
       <c r="Y53">
-        <f t="array" ref="Y53">IFERROR(CONCATENATE((INDEX($A$7:$A$31,SMALL(IF($Z$7:$Z$31&lt;&gt;"",IF($W$7:$W$31&lt;&gt;"",ROW($W$7:$W$31)-MIN(ROW($W$7:$W$31))+1,""),""),ROW()-ROW(A$33)+1))),),"")</f>
+        <f t="array" ref="Y53">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($Z$7:$Z$30&lt;&gt;"",IF($W$7:$W$30&lt;&gt;"",ROW($W$7:$W$30)-MIN(ROW($W$7:$W$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="54" spans="11:25">
       <c r="K54">
-        <f t="array" ref="K54">IFERROR(CONCATENATE(TEXT(INDEX($K$7:$K$31,SMALL(IF($N$7:$N$31&lt;&gt;"",IF($K$7:$K$31&lt;&gt;"",ROW($K$7:$K$31)-MIN(ROW($K$7:$K$31))+1,""),""),ROW()-ROW(A$33)+1)),"##0"),","),"")</f>
+        <f t="array" ref="K54">IFERROR(CONCATENATE(TEXT(INDEX($K$7:$K$30,SMALL(IF($N$7:$N$30&lt;&gt;"",IF($K$7:$K$30&lt;&gt;"",ROW($K$7:$K$30)-MIN(ROW($K$7:$K$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0"),","),"")</f>
         <v>0</v>
       </c>
       <c r="L54">
-        <f t="array" ref="L54">IFERROR(CONCATENATE((INDEX($N$7:$N$31,SMALL(IF($N$7:$N$31&lt;&gt;"",IF($K$7:$K$31&lt;&gt;"",ROW($K$7:$K$31)-MIN(ROW($K$7:$K$31))+1,""),""),ROW()-ROW(A$33)+1))),","),"")</f>
+        <f t="array" ref="L54">IFERROR(CONCATENATE((INDEX($N$7:$N$30,SMALL(IF($N$7:$N$30&lt;&gt;"",IF($K$7:$K$30&lt;&gt;"",ROW($K$7:$K$30)-MIN(ROW($K$7:$K$30))+1,""),""),ROW()-ROW(A$32)+1))),","),"")</f>
         <v>0</v>
       </c>
       <c r="M54">
-        <f t="array" ref="M54">IFERROR(CONCATENATE((INDEX($A$7:$A$31,SMALL(IF($N$7:$N$31&lt;&gt;"",IF($K$7:$K$31&lt;&gt;"",ROW($K$7:$K$31)-MIN(ROW($K$7:$K$31))+1,""),""),ROW()-ROW(A$33)+1))),),"")</f>
+        <f t="array" ref="M54">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($N$7:$N$30&lt;&gt;"",IF($K$7:$K$30&lt;&gt;"",ROW($K$7:$K$30)-MIN(ROW($K$7:$K$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
         <v>0</v>
       </c>
       <c r="Q54">
-        <f t="array" ref="Q54">IFERROR(CONCATENATE((INDEX($T$7:$T$31,SMALL(IF($T$7:$T$31&lt;&gt;"",IF($Q$7:$Q$31&lt;&gt;"",ROW($Q$7:$Q$31)-MIN(ROW($Q$7:$Q$31))+1,""),""),ROW()-ROW(A$33)+1)))," "),"")</f>
+        <f t="array" ref="Q54">IFERROR(CONCATENATE((INDEX($T$7:$T$30,SMALL(IF($T$7:$T$30&lt;&gt;"",IF($Q$7:$Q$30&lt;&gt;"",ROW($Q$7:$Q$30)-MIN(ROW($Q$7:$Q$30))+1,""),""),ROW()-ROW(A$32)+1)))," "),"")</f>
         <v>0</v>
       </c>
       <c r="R54">
-        <f t="array" ref="R54">IFERROR(CONCATENATE(TEXT(INDEX($Q$7:$Q$31,SMALL(IF($T$7:$T$31&lt;&gt;"",IF($Q$7:$Q$31&lt;&gt;"",ROW($Q$7:$Q$31)-MIN(ROW($Q$7:$Q$31))+1,""),""),ROW()-ROW(A$33)+1)),"##0")," "),"")</f>
+        <f t="array" ref="R54">IFERROR(CONCATENATE(TEXT(INDEX($Q$7:$Q$30,SMALL(IF($T$7:$T$30&lt;&gt;"",IF($Q$7:$Q$30&lt;&gt;"",ROW($Q$7:$Q$30)-MIN(ROW($Q$7:$Q$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0")," "),"")</f>
         <v>0</v>
       </c>
       <c r="S54">
-        <f t="array" ref="S54">IFERROR(CONCATENATE((INDEX($A$7:$A$31,SMALL(IF($T$7:$T$31&lt;&gt;"",IF($Q$7:$Q$31&lt;&gt;"",ROW($Q$7:$Q$31)-MIN(ROW($Q$7:$Q$31))+1,""),""),ROW()-ROW(A$33)+1))),),"")</f>
+        <f t="array" ref="S54">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($T$7:$T$30&lt;&gt;"",IF($Q$7:$Q$30&lt;&gt;"",ROW($Q$7:$Q$30)-MIN(ROW($Q$7:$Q$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
         <v>0</v>
       </c>
       <c r="W54">
-        <f t="array" ref="W54">IFERROR(CONCATENATE((INDEX($Z$7:$Z$31,SMALL(IF($Z$7:$Z$31&lt;&gt;"",IF($W$7:$W$31&lt;&gt;"",ROW($W$7:$W$31)-MIN(ROW($W$7:$W$31))+1,""),""),ROW()-ROW(A$33)+1))),","),"")</f>
+        <f t="array" ref="W54">IFERROR(CONCATENATE((INDEX($Z$7:$Z$30,SMALL(IF($Z$7:$Z$30&lt;&gt;"",IF($W$7:$W$30&lt;&gt;"",ROW($W$7:$W$30)-MIN(ROW($W$7:$W$30))+1,""),""),ROW()-ROW(A$32)+1))),","),"")</f>
         <v>0</v>
       </c>
       <c r="X54">
-        <f t="array" ref="X54">IFERROR(CONCATENATE(TEXT(INDEX($W$7:$W$31,SMALL(IF($Z$7:$Z$31&lt;&gt;"",IF($W$7:$W$31&lt;&gt;"",ROW($W$7:$W$31)-MIN(ROW($W$7:$W$31))+1,""),""),ROW()-ROW(A$33)+1)),"##0"),","),"")</f>
+        <f t="array" ref="X54">IFERROR(CONCATENATE(TEXT(INDEX($W$7:$W$30,SMALL(IF($Z$7:$Z$30&lt;&gt;"",IF($W$7:$W$30&lt;&gt;"",ROW($W$7:$W$30)-MIN(ROW($W$7:$W$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0"),","),"")</f>
         <v>0</v>
       </c>
       <c r="Y54">
-        <f t="array" ref="Y54">IFERROR(CONCATENATE((INDEX($A$7:$A$31,SMALL(IF($Z$7:$Z$31&lt;&gt;"",IF($W$7:$W$31&lt;&gt;"",ROW($W$7:$W$31)-MIN(ROW($W$7:$W$31))+1,""),""),ROW()-ROW(A$33)+1))),),"")</f>
+        <f t="array" ref="Y54">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($Z$7:$Z$30&lt;&gt;"",IF($W$7:$W$30&lt;&gt;"",ROW($W$7:$W$30)-MIN(ROW($W$7:$W$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
         <v>0</v>
       </c>
     </row>
     <row r="55" spans="11:25">
       <c r="K55">
-        <f t="array" ref="K55">IFERROR(CONCATENATE(TEXT(INDEX($K$7:$K$31,SMALL(IF($N$7:$N$31&lt;&gt;"",IF($K$7:$K$31&lt;&gt;"",ROW($K$7:$K$31)-MIN(ROW($K$7:$K$31))+1,""),""),ROW()-ROW(A$33)+1)),"##0"),","),"")</f>
+        <f t="array" ref="K55">IFERROR(CONCATENATE(TEXT(INDEX($K$7:$K$30,SMALL(IF($N$7:$N$30&lt;&gt;"",IF($K$7:$K$30&lt;&gt;"",ROW($K$7:$K$30)-MIN(ROW($K$7:$K$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0"),","),"")</f>
         <v>0</v>
       </c>
       <c r="L55">
-        <f t="array" ref="L55">IFERROR(CONCATENATE((INDEX($N$7:$N$31,SMALL(IF($N$7:$N$31&lt;&gt;"",IF($K$7:$K$31&lt;&gt;"",ROW($K$7:$K$31)-MIN(ROW($K$7:$K$31))+1,""),""),ROW()-ROW(A$33)+1))),","),"")</f>
+        <f t="array" ref="L55">IFERROR(CONCATENATE((INDEX($N$7:$N$30,SMALL(IF($N$7:$N$30&lt;&gt;"",IF($K$7:$K$30&lt;&gt;"",ROW($K$7:$K$30)-MIN(ROW($K$7:$K$30))+1,""),""),ROW()-ROW(A$32)+1))),","),"")</f>
         <v>0</v>
       </c>
       <c r="M55">
-        <f t="array" ref="M55">IFERROR(CONCATENATE((INDEX($A$7:$A$31,SMALL(IF($N$7:$N$31&lt;&gt;"",IF($K$7:$K$31&lt;&gt;"",ROW($K$7:$K$31)-MIN(ROW($K$7:$K$31))+1,""),""),ROW()-ROW(A$33)+1))),),"")</f>
+        <f t="array" ref="M55">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($N$7:$N$30&lt;&gt;"",IF($K$7:$K$30&lt;&gt;"",ROW($K$7:$K$30)-MIN(ROW($K$7:$K$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
         <v>0</v>
       </c>
       <c r="Q55">
-        <f t="array" ref="Q55">IFERROR(CONCATENATE((INDEX($T$7:$T$31,SMALL(IF($T$7:$T$31&lt;&gt;"",IF($Q$7:$Q$31&lt;&gt;"",ROW($Q$7:$Q$31)-MIN(ROW($Q$7:$Q$31))+1,""),""),ROW()-ROW(A$33)+1)))," "),"")</f>
+        <f t="array" ref="Q55">IFERROR(CONCATENATE((INDEX($T$7:$T$30,SMALL(IF($T$7:$T$30&lt;&gt;"",IF($Q$7:$Q$30&lt;&gt;"",ROW($Q$7:$Q$30)-MIN(ROW($Q$7:$Q$30))+1,""),""),ROW()-ROW(A$32)+1)))," "),"")</f>
         <v>0</v>
       </c>
       <c r="R55">
-        <f t="array" ref="R55">IFERROR(CONCATENATE(TEXT(INDEX($Q$7:$Q$31,SMALL(IF($T$7:$T$31&lt;&gt;"",IF($Q$7:$Q$31&lt;&gt;"",ROW($Q$7:$Q$31)-MIN(ROW($Q$7:$Q$31))+1,""),""),ROW()-ROW(A$33)+1)),"##0")," "),"")</f>
+        <f t="array" ref="R55">IFERROR(CONCATENATE(TEXT(INDEX($Q$7:$Q$30,SMALL(IF($T$7:$T$30&lt;&gt;"",IF($Q$7:$Q$30&lt;&gt;"",ROW($Q$7:$Q$30)-MIN(ROW($Q$7:$Q$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0")," "),"")</f>
         <v>0</v>
       </c>
       <c r="S55">
-        <f t="array" ref="S55">IFERROR(CONCATENATE((INDEX($A$7:$A$31,SMALL(IF($T$7:$T$31&lt;&gt;"",IF($Q$7:$Q$31&lt;&gt;"",ROW($Q$7:$Q$31)-MIN(ROW($Q$7:$Q$31))+1,""),""),ROW()-ROW(A$33)+1))),),"")</f>
+        <f t="array" ref="S55">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($T$7:$T$30&lt;&gt;"",IF($Q$7:$Q$30&lt;&gt;"",ROW($Q$7:$Q$30)-MIN(ROW($Q$7:$Q$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
         <v>0</v>
       </c>
       <c r="W55">
-        <f t="array" ref="W55">IFERROR(CONCATENATE((INDEX($Z$7:$Z$31,SMALL(IF($Z$7:$Z$31&lt;&gt;"",IF($W$7:$W$31&lt;&gt;"",ROW($W$7:$W$31)-MIN(ROW($W$7:$W$31))+1,""),""),ROW()-ROW(A$33)+1))),","),"")</f>
+        <f t="array" ref="W55">IFERROR(CONCATENATE((INDEX($Z$7:$Z$30,SMALL(IF($Z$7:$Z$30&lt;&gt;"",IF($W$7:$W$30&lt;&gt;"",ROW($W$7:$W$30)-MIN(ROW($W$7:$W$30))+1,""),""),ROW()-ROW(A$32)+1))),","),"")</f>
         <v>0</v>
       </c>
       <c r="X55">
-        <f t="array" ref="X55">IFERROR(CONCATENATE(TEXT(INDEX($W$7:$W$31,SMALL(IF($Z$7:$Z$31&lt;&gt;"",IF($W$7:$W$31&lt;&gt;"",ROW($W$7:$W$31)-MIN(ROW($W$7:$W$31))+1,""),""),ROW()-ROW(A$33)+1)),"##0"),","),"")</f>
+        <f t="array" ref="X55">IFERROR(CONCATENATE(TEXT(INDEX($W$7:$W$30,SMALL(IF($Z$7:$Z$30&lt;&gt;"",IF($W$7:$W$30&lt;&gt;"",ROW($W$7:$W$30)-MIN(ROW($W$7:$W$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0"),","),"")</f>
         <v>0</v>
       </c>
       <c r="Y55">
-        <f t="array" ref="Y55">IFERROR(CONCATENATE((INDEX($A$7:$A$31,SMALL(IF($Z$7:$Z$31&lt;&gt;"",IF($W$7:$W$31&lt;&gt;"",ROW($W$7:$W$31)-MIN(ROW($W$7:$W$31))+1,""),""),ROW()-ROW(A$33)+1))),),"")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="11:25">
-      <c r="K56">
-        <f t="array" ref="K56">IFERROR(CONCATENATE(TEXT(INDEX($K$7:$K$31,SMALL(IF($N$7:$N$31&lt;&gt;"",IF($K$7:$K$31&lt;&gt;"",ROW($K$7:$K$31)-MIN(ROW($K$7:$K$31))+1,""),""),ROW()-ROW(A$33)+1)),"##0"),","),"")</f>
-        <v>0</v>
-      </c>
-      <c r="L56">
-        <f t="array" ref="L56">IFERROR(CONCATENATE((INDEX($N$7:$N$31,SMALL(IF($N$7:$N$31&lt;&gt;"",IF($K$7:$K$31&lt;&gt;"",ROW($K$7:$K$31)-MIN(ROW($K$7:$K$31))+1,""),""),ROW()-ROW(A$33)+1))),","),"")</f>
-        <v>0</v>
-      </c>
-      <c r="M56">
-        <f t="array" ref="M56">IFERROR(CONCATENATE((INDEX($A$7:$A$31,SMALL(IF($N$7:$N$31&lt;&gt;"",IF($K$7:$K$31&lt;&gt;"",ROW($K$7:$K$31)-MIN(ROW($K$7:$K$31))+1,""),""),ROW()-ROW(A$33)+1))),),"")</f>
-        <v>0</v>
-      </c>
-      <c r="Q56">
-        <f t="array" ref="Q56">IFERROR(CONCATENATE((INDEX($T$7:$T$31,SMALL(IF($T$7:$T$31&lt;&gt;"",IF($Q$7:$Q$31&lt;&gt;"",ROW($Q$7:$Q$31)-MIN(ROW($Q$7:$Q$31))+1,""),""),ROW()-ROW(A$33)+1)))," "),"")</f>
-        <v>0</v>
-      </c>
-      <c r="R56">
-        <f t="array" ref="R56">IFERROR(CONCATENATE(TEXT(INDEX($Q$7:$Q$31,SMALL(IF($T$7:$T$31&lt;&gt;"",IF($Q$7:$Q$31&lt;&gt;"",ROW($Q$7:$Q$31)-MIN(ROW($Q$7:$Q$31))+1,""),""),ROW()-ROW(A$33)+1)),"##0")," "),"")</f>
-        <v>0</v>
-      </c>
-      <c r="S56">
-        <f t="array" ref="S56">IFERROR(CONCATENATE((INDEX($A$7:$A$31,SMALL(IF($T$7:$T$31&lt;&gt;"",IF($Q$7:$Q$31&lt;&gt;"",ROW($Q$7:$Q$31)-MIN(ROW($Q$7:$Q$31))+1,""),""),ROW()-ROW(A$33)+1))),),"")</f>
-        <v>0</v>
-      </c>
-      <c r="W56">
-        <f t="array" ref="W56">IFERROR(CONCATENATE((INDEX($Z$7:$Z$31,SMALL(IF($Z$7:$Z$31&lt;&gt;"",IF($W$7:$W$31&lt;&gt;"",ROW($W$7:$W$31)-MIN(ROW($W$7:$W$31))+1,""),""),ROW()-ROW(A$33)+1))),","),"")</f>
-        <v>0</v>
-      </c>
-      <c r="X56">
-        <f t="array" ref="X56">IFERROR(CONCATENATE(TEXT(INDEX($W$7:$W$31,SMALL(IF($Z$7:$Z$31&lt;&gt;"",IF($W$7:$W$31&lt;&gt;"",ROW($W$7:$W$31)-MIN(ROW($W$7:$W$31))+1,""),""),ROW()-ROW(A$33)+1)),"##0"),","),"")</f>
-        <v>0</v>
-      </c>
-      <c r="Y56">
-        <f t="array" ref="Y56">IFERROR(CONCATENATE((INDEX($A$7:$A$31,SMALL(IF($Z$7:$Z$31&lt;&gt;"",IF($W$7:$W$31&lt;&gt;"",ROW($W$7:$W$31)-MIN(ROW($W$7:$W$31))+1,""),""),ROW()-ROW(A$33)+1))),),"")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="11:25">
-      <c r="K57">
-        <f t="array" ref="K57">IFERROR(CONCATENATE(TEXT(INDEX($K$7:$K$31,SMALL(IF($N$7:$N$31&lt;&gt;"",IF($K$7:$K$31&lt;&gt;"",ROW($K$7:$K$31)-MIN(ROW($K$7:$K$31))+1,""),""),ROW()-ROW(A$33)+1)),"##0"),","),"")</f>
-        <v>0</v>
-      </c>
-      <c r="L57">
-        <f t="array" ref="L57">IFERROR(CONCATENATE((INDEX($N$7:$N$31,SMALL(IF($N$7:$N$31&lt;&gt;"",IF($K$7:$K$31&lt;&gt;"",ROW($K$7:$K$31)-MIN(ROW($K$7:$K$31))+1,""),""),ROW()-ROW(A$33)+1))),","),"")</f>
-        <v>0</v>
-      </c>
-      <c r="M57">
-        <f t="array" ref="M57">IFERROR(CONCATENATE((INDEX($A$7:$A$31,SMALL(IF($N$7:$N$31&lt;&gt;"",IF($K$7:$K$31&lt;&gt;"",ROW($K$7:$K$31)-MIN(ROW($K$7:$K$31))+1,""),""),ROW()-ROW(A$33)+1))),),"")</f>
-        <v>0</v>
-      </c>
-      <c r="Q57">
-        <f t="array" ref="Q57">IFERROR(CONCATENATE((INDEX($T$7:$T$31,SMALL(IF($T$7:$T$31&lt;&gt;"",IF($Q$7:$Q$31&lt;&gt;"",ROW($Q$7:$Q$31)-MIN(ROW($Q$7:$Q$31))+1,""),""),ROW()-ROW(A$33)+1)))," "),"")</f>
-        <v>0</v>
-      </c>
-      <c r="R57">
-        <f t="array" ref="R57">IFERROR(CONCATENATE(TEXT(INDEX($Q$7:$Q$31,SMALL(IF($T$7:$T$31&lt;&gt;"",IF($Q$7:$Q$31&lt;&gt;"",ROW($Q$7:$Q$31)-MIN(ROW($Q$7:$Q$31))+1,""),""),ROW()-ROW(A$33)+1)),"##0")," "),"")</f>
-        <v>0</v>
-      </c>
-      <c r="S57">
-        <f t="array" ref="S57">IFERROR(CONCATENATE((INDEX($A$7:$A$31,SMALL(IF($T$7:$T$31&lt;&gt;"",IF($Q$7:$Q$31&lt;&gt;"",ROW($Q$7:$Q$31)-MIN(ROW($Q$7:$Q$31))+1,""),""),ROW()-ROW(A$33)+1))),),"")</f>
-        <v>0</v>
-      </c>
-      <c r="W57">
-        <f t="array" ref="W57">IFERROR(CONCATENATE((INDEX($Z$7:$Z$31,SMALL(IF($Z$7:$Z$31&lt;&gt;"",IF($W$7:$W$31&lt;&gt;"",ROW($W$7:$W$31)-MIN(ROW($W$7:$W$31))+1,""),""),ROW()-ROW(A$33)+1))),","),"")</f>
-        <v>0</v>
-      </c>
-      <c r="X57">
-        <f t="array" ref="X57">IFERROR(CONCATENATE(TEXT(INDEX($W$7:$W$31,SMALL(IF($Z$7:$Z$31&lt;&gt;"",IF($W$7:$W$31&lt;&gt;"",ROW($W$7:$W$31)-MIN(ROW($W$7:$W$31))+1,""),""),ROW()-ROW(A$33)+1)),"##0"),","),"")</f>
-        <v>0</v>
-      </c>
-      <c r="Y57">
-        <f t="array" ref="Y57">IFERROR(CONCATENATE((INDEX($A$7:$A$31,SMALL(IF($Z$7:$Z$31&lt;&gt;"",IF($W$7:$W$31&lt;&gt;"",ROW($W$7:$W$31)-MIN(ROW($W$7:$W$31))+1,""),""),ROW()-ROW(A$33)+1))),),"")</f>
+        <f t="array" ref="Y55">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($Z$7:$Z$30&lt;&gt;"",IF($W$7:$W$30&lt;&gt;"",ROW($W$7:$W$30)-MIN(ROW($W$7:$W$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
         <v>0</v>
       </c>
     </row>
@@ -2915,53 +3304,251 @@
     <mergeCell ref="P5:U5"/>
     <mergeCell ref="V5:AA5"/>
   </mergeCells>
+  <conditionalFormatting sqref="L10">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThanOrEqual">
+      <formula>H10</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L11">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="lessThanOrEqual">
+      <formula>H11</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L12">
+    <cfRule type="cellIs" dxfId="0" priority="5" operator="lessThanOrEqual">
+      <formula>H12</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L13">
+    <cfRule type="cellIs" dxfId="0" priority="7" operator="lessThanOrEqual">
+      <formula>H13</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L19">
+    <cfRule type="cellIs" dxfId="0" priority="9" operator="lessThanOrEqual">
+      <formula>H19</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="L21">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="0" priority="11" operator="lessThanOrEqual">
       <formula>H21</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="L29">
+    <cfRule type="cellIs" dxfId="0" priority="13" operator="lessThanOrEqual">
+      <formula>H29</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M10">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="lessThanOrEqual">
+      <formula>I10</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M11">
+    <cfRule type="cellIs" dxfId="0" priority="4" operator="lessThanOrEqual">
+      <formula>I11</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M12">
+    <cfRule type="cellIs" dxfId="0" priority="6" operator="lessThanOrEqual">
+      <formula>I12</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M13">
+    <cfRule type="cellIs" dxfId="0" priority="8" operator="lessThanOrEqual">
+      <formula>I13</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M19">
+    <cfRule type="cellIs" dxfId="0" priority="10" operator="lessThanOrEqual">
+      <formula>I19</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="M21">
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="0" priority="12" operator="lessThanOrEqual">
       <formula>I21</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R18">
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="lessThanOrEqual">
-      <formula>H18</formula>
+  <conditionalFormatting sqref="M29">
+    <cfRule type="cellIs" dxfId="0" priority="14" operator="lessThanOrEqual">
+      <formula>I29</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R10">
+    <cfRule type="cellIs" dxfId="0" priority="15" operator="lessThanOrEqual">
+      <formula>H10</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R11">
+    <cfRule type="cellIs" dxfId="0" priority="17" operator="lessThanOrEqual">
+      <formula>H11</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R12">
+    <cfRule type="cellIs" dxfId="0" priority="19" operator="lessThanOrEqual">
+      <formula>H12</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R13">
+    <cfRule type="cellIs" dxfId="0" priority="21" operator="lessThanOrEqual">
+      <formula>H13</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R17">
+    <cfRule type="cellIs" dxfId="0" priority="23" operator="lessThanOrEqual">
+      <formula>H17</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R19">
+    <cfRule type="cellIs" dxfId="0" priority="25" operator="lessThanOrEqual">
+      <formula>H19</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R20">
+    <cfRule type="cellIs" dxfId="0" priority="27" operator="lessThanOrEqual">
+      <formula>H20</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R21">
-    <cfRule type="cellIs" dxfId="0" priority="5" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="0" priority="29" operator="lessThanOrEqual">
       <formula>H21</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S18">
-    <cfRule type="cellIs" dxfId="0" priority="4" operator="lessThanOrEqual">
-      <formula>I18</formula>
+  <conditionalFormatting sqref="R29">
+    <cfRule type="cellIs" dxfId="0" priority="31" operator="lessThanOrEqual">
+      <formula>H29</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S10">
+    <cfRule type="cellIs" dxfId="0" priority="16" operator="lessThanOrEqual">
+      <formula>I10</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S11">
+    <cfRule type="cellIs" dxfId="0" priority="18" operator="lessThanOrEqual">
+      <formula>I11</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S12">
+    <cfRule type="cellIs" dxfId="0" priority="20" operator="lessThanOrEqual">
+      <formula>I12</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S13">
+    <cfRule type="cellIs" dxfId="0" priority="22" operator="lessThanOrEqual">
+      <formula>I13</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S17">
+    <cfRule type="cellIs" dxfId="0" priority="24" operator="lessThanOrEqual">
+      <formula>I17</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S19">
+    <cfRule type="cellIs" dxfId="0" priority="26" operator="lessThanOrEqual">
+      <formula>I19</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S20">
+    <cfRule type="cellIs" dxfId="0" priority="28" operator="lessThanOrEqual">
+      <formula>I20</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S21">
-    <cfRule type="cellIs" dxfId="0" priority="6" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="0" priority="30" operator="lessThanOrEqual">
       <formula>I21</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="S29">
+    <cfRule type="cellIs" dxfId="0" priority="32" operator="lessThanOrEqual">
+      <formula>I29</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="X11">
+    <cfRule type="cellIs" dxfId="0" priority="33" operator="lessThanOrEqual">
+      <formula>H11</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="X12">
+    <cfRule type="cellIs" dxfId="0" priority="35" operator="lessThanOrEqual">
+      <formula>H12</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="X13">
+    <cfRule type="cellIs" dxfId="0" priority="37" operator="lessThanOrEqual">
+      <formula>H13</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="X17">
+    <cfRule type="cellIs" dxfId="0" priority="39" operator="lessThanOrEqual">
+      <formula>H17</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="X19">
+    <cfRule type="cellIs" dxfId="0" priority="41" operator="lessThanOrEqual">
+      <formula>H19</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="X21">
-    <cfRule type="cellIs" dxfId="0" priority="7" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="0" priority="43" operator="lessThanOrEqual">
       <formula>H21</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="Y11">
+    <cfRule type="cellIs" dxfId="0" priority="34" operator="lessThanOrEqual">
+      <formula>I11</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y12">
+    <cfRule type="cellIs" dxfId="0" priority="36" operator="lessThanOrEqual">
+      <formula>I12</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y13">
+    <cfRule type="cellIs" dxfId="0" priority="38" operator="lessThanOrEqual">
+      <formula>I13</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y17">
+    <cfRule type="cellIs" dxfId="0" priority="40" operator="lessThanOrEqual">
+      <formula>I17</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y19">
+    <cfRule type="cellIs" dxfId="0" priority="42" operator="lessThanOrEqual">
+      <formula>I19</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="Y21">
-    <cfRule type="cellIs" dxfId="0" priority="8" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="0" priority="44" operator="lessThanOrEqual">
       <formula>I21</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="U18" r:id="rId1"/>
-    <hyperlink ref="O21" r:id="rId2"/>
-    <hyperlink ref="U21" r:id="rId3"/>
-    <hyperlink ref="AA21" r:id="rId4"/>
+    <hyperlink ref="O10" r:id="rId1"/>
+    <hyperlink ref="U10" r:id="rId2"/>
+    <hyperlink ref="O11" r:id="rId3"/>
+    <hyperlink ref="U11" r:id="rId4"/>
+    <hyperlink ref="AA11" r:id="rId5"/>
+    <hyperlink ref="O12" r:id="rId6"/>
+    <hyperlink ref="U12" r:id="rId7"/>
+    <hyperlink ref="AA12" r:id="rId8"/>
+    <hyperlink ref="O13" r:id="rId9"/>
+    <hyperlink ref="U13" r:id="rId10"/>
+    <hyperlink ref="AA13" r:id="rId11"/>
+    <hyperlink ref="U17" r:id="rId12"/>
+    <hyperlink ref="AA17" r:id="rId13"/>
+    <hyperlink ref="O19" r:id="rId14"/>
+    <hyperlink ref="U19" r:id="rId15"/>
+    <hyperlink ref="AA19" r:id="rId16"/>
+    <hyperlink ref="U20" r:id="rId17"/>
+    <hyperlink ref="O21" r:id="rId18"/>
+    <hyperlink ref="U21" r:id="rId19"/>
+    <hyperlink ref="AA21" r:id="rId20"/>
+    <hyperlink ref="O29" r:id="rId21"/>
+    <hyperlink ref="U29" r:id="rId22"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId5"/>
+  <legacyDrawing r:id="rId23"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed KiCost BOM issue, updated BOM
</commit_message>
<xml_diff>
--- a/kicad/hack.xlsx
+++ b/kicad/hack.xlsx
@@ -13,8 +13,10 @@
     <definedName name="BoardQty">KiCost!$I$1</definedName>
     <definedName name="digikey_part_data">KiCost!$J$5:$O$30</definedName>
     <definedName name="global_part_data">KiCost!$A$5:$I$30</definedName>
+    <definedName name="local_part_data">KiCost!$AB$5:$AG$30</definedName>
     <definedName name="mouser_part_data">KiCost!$P$5:$U$30</definedName>
     <definedName name="newark_part_data">KiCost!$V$5:$AA$30</definedName>
+    <definedName name="seeedstudio_part_data">KiCost!$AH$5:$AM$30</definedName>
     <definedName name="TotalCost">KiCost!$I$2</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -378,12 +380,168 @@
         </r>
       </text>
     </comment>
+    <comment ref="AB6" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Available quantity of each part at the distributor.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AC6" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Purchase quantity of each part from this distributor.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AD6" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Unit price of each part from this distributor.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AE6" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>(Unit Price) x (Purchase Qty) of each part from this distributor.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AF6" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Distributor-assigned part number for each part.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AG6" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Link to distributor webpage for each part.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AH6" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Available quantity of each part at the distributor.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AI6" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Purchase quantity of each part from this distributor.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AJ6" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Unit price of each part from this distributor.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AK6" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>(Unit Price) x (Purchase Qty) of each part from this distributor.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AL6" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Distributor-assigned part number for each part.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AM6" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Link to distributor webpage for each part.</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="134">
   <si>
     <t>Global Part Info</t>
   </si>
@@ -415,6 +573,120 @@
     <t>Desc</t>
   </si>
   <si>
+    <t>C3,C4</t>
+  </si>
+  <si>
+    <t>10uF</t>
+  </si>
+  <si>
+    <t>hack-footprints:c_elec_3x5.3</t>
+  </si>
+  <si>
+    <t>UWX1C100MCL2GB</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>RED</t>
+  </si>
+  <si>
+    <t>hack-footprints:LED_0603_HandSoldering</t>
+  </si>
+  <si>
+    <t>304090042</t>
+  </si>
+  <si>
+    <t>U2</t>
+  </si>
+  <si>
+    <t>STF202</t>
+  </si>
+  <si>
+    <t>hack-footprints:TSOP-6</t>
+  </si>
+  <si>
+    <t>STF202-22T1G</t>
+  </si>
+  <si>
+    <t>C5</t>
+  </si>
+  <si>
+    <t>4.7nF</t>
+  </si>
+  <si>
+    <t>hack-footprints:C_0603_HandSoldering</t>
+  </si>
+  <si>
+    <t>302010144</t>
+  </si>
+  <si>
+    <t>L2</t>
+  </si>
+  <si>
+    <t>10uH</t>
+  </si>
+  <si>
+    <t>hack-footprints:ELLVFG</t>
+  </si>
+  <si>
+    <t>ELL-VFG100MC</t>
+  </si>
+  <si>
+    <t>JP1</t>
+  </si>
+  <si>
+    <t>Jumper_NO_Small</t>
+  </si>
+  <si>
+    <t>hack-footprints:SMD_Jumper</t>
+  </si>
+  <si>
+    <t>U3</t>
+  </si>
+  <si>
+    <t>ATSAMD21E</t>
+  </si>
+  <si>
+    <t>hack-footprints:QFN-32-1EP_5x5mm_Pitch0.5mm</t>
+  </si>
+  <si>
+    <t>ATSAMD21E18A-MU</t>
+  </si>
+  <si>
+    <t>L1</t>
+  </si>
+  <si>
+    <t>BLM18EG221</t>
+  </si>
+  <si>
+    <t>hack-footprints:L_0603_HandSoldering</t>
+  </si>
+  <si>
+    <t>BLM18EG221SN1D</t>
+  </si>
+  <si>
+    <t>R3</t>
+  </si>
+  <si>
+    <t>10k</t>
+  </si>
+  <si>
+    <t>hack-footprints:R_0603_HandSoldering</t>
+  </si>
+  <si>
+    <t>301010299</t>
+  </si>
+  <si>
+    <t>FID1-FID3</t>
+  </si>
+  <si>
+    <t>FIDUCIAL</t>
+  </si>
+  <si>
+    <t>hack-footprints:FIDUCIAL</t>
+  </si>
+  <si>
     <t>S1</t>
   </si>
   <si>
@@ -427,16 +699,88 @@
     <t>311020045</t>
   </si>
   <si>
-    <t>C5</t>
-  </si>
-  <si>
-    <t>4.7nF</t>
-  </si>
-  <si>
-    <t>hack:C_0603_HandSoldering</t>
-  </si>
-  <si>
-    <t>302010144</t>
+    <t>LOGO3</t>
+  </si>
+  <si>
+    <t>HACK</t>
+  </si>
+  <si>
+    <t>hack-footprints:HACK-LOGO</t>
+  </si>
+  <si>
+    <t>P4</t>
+  </si>
+  <si>
+    <t>CONN_01X01</t>
+  </si>
+  <si>
+    <t>hack-footprints:Pin_Castellated_1x01</t>
+  </si>
+  <si>
+    <t>P1</t>
+  </si>
+  <si>
+    <t>USB_micro</t>
+  </si>
+  <si>
+    <t>hack-footprints:ST-USB-001G</t>
+  </si>
+  <si>
+    <t>320010000</t>
+  </si>
+  <si>
+    <t>X1</t>
+  </si>
+  <si>
+    <t>ABS07</t>
+  </si>
+  <si>
+    <t>hack-footprints:xtal_3.2x1.5mm</t>
+  </si>
+  <si>
+    <t>306010055</t>
+  </si>
+  <si>
+    <t>C1,C2</t>
+  </si>
+  <si>
+    <t>2.2uF</t>
+  </si>
+  <si>
+    <t>CC0603MRX5R5BB225</t>
+  </si>
+  <si>
+    <t>U1</t>
+  </si>
+  <si>
+    <t>MIC5528</t>
+  </si>
+  <si>
+    <t>hack-footprints:DFN-6-1EP_1.2x1.2mm_Pitch0.4mm</t>
+  </si>
+  <si>
+    <t>MIC5528-3.3YMT-TR</t>
+  </si>
+  <si>
+    <t>LOGO2</t>
+  </si>
+  <si>
+    <t>HACKADAY</t>
+  </si>
+  <si>
+    <t>hack-footprints:HACKADAY-LOGO</t>
+  </si>
+  <si>
+    <t>mfr_pn</t>
+  </si>
+  <si>
+    <t>C8-C11</t>
+  </si>
+  <si>
+    <t>100nF</t>
+  </si>
+  <si>
+    <t>302010138</t>
   </si>
   <si>
     <t>R1</t>
@@ -445,70 +789,37 @@
     <t>1M</t>
   </si>
   <si>
-    <t>hack:R_0603_HandSoldering</t>
-  </si>
-  <si>
     <t>301010151</t>
   </si>
   <si>
-    <t>U1</t>
-  </si>
-  <si>
-    <t>MIC5528</t>
-  </si>
-  <si>
-    <t>hack:DFN-6-1EP_1.2x1.2mm_Pitch0.4mm</t>
-  </si>
-  <si>
-    <t>MIC5528-3.3YMT-TR</t>
-  </si>
-  <si>
-    <t>L1</t>
-  </si>
-  <si>
-    <t>BLM18EG221</t>
-  </si>
-  <si>
-    <t>hack:L_0603_HandSoldering</t>
-  </si>
-  <si>
-    <t>BLM18EG221SN1D</t>
-  </si>
-  <si>
-    <t>U2</t>
-  </si>
-  <si>
-    <t>STF202</t>
-  </si>
-  <si>
-    <t>hack:TSOP-6</t>
-  </si>
-  <si>
-    <t>STF202-22T1G</t>
-  </si>
-  <si>
-    <t>L2</t>
-  </si>
-  <si>
-    <t>10uH</t>
-  </si>
-  <si>
-    <t>hack:ELLVFG</t>
-  </si>
-  <si>
-    <t>ELL-VFG100MC</t>
-  </si>
-  <si>
     <t>LOGO1</t>
   </si>
   <si>
     <t>OSHW</t>
   </si>
   <si>
-    <t>hack:OSHW-LOGO</t>
-  </si>
-  <si>
-    <t>mfr_pn</t>
+    <t>hack-footprints:OSHW-LOGO</t>
+  </si>
+  <si>
+    <t>P2,P3</t>
+  </si>
+  <si>
+    <t>CONN_01X13</t>
+  </si>
+  <si>
+    <t>hack-footprints:Pin_Castellated_1x13</t>
+  </si>
+  <si>
+    <t>320020128</t>
+  </si>
+  <si>
+    <t>R2,R4</t>
+  </si>
+  <si>
+    <t>330</t>
+  </si>
+  <si>
+    <t>301010300</t>
   </si>
   <si>
     <t>C6,C7</t>
@@ -520,150 +831,6 @@
     <t>302010097</t>
   </si>
   <si>
-    <t>X1</t>
-  </si>
-  <si>
-    <t>ABS07</t>
-  </si>
-  <si>
-    <t>306010055</t>
-  </si>
-  <si>
-    <t>R2,R4</t>
-  </si>
-  <si>
-    <t>330</t>
-  </si>
-  <si>
-    <t>301010300</t>
-  </si>
-  <si>
-    <t>FID1-FID3</t>
-  </si>
-  <si>
-    <t>FIDUCIAL</t>
-  </si>
-  <si>
-    <t>hack:FIDUCIAL</t>
-  </si>
-  <si>
-    <t>C3,C4</t>
-  </si>
-  <si>
-    <t>10uF</t>
-  </si>
-  <si>
-    <t>hack:c_elec_3x5.3</t>
-  </si>
-  <si>
-    <t>UWX1C100MCL2GB</t>
-  </si>
-  <si>
-    <t>LOGO3</t>
-  </si>
-  <si>
-    <t>HACK</t>
-  </si>
-  <si>
-    <t>U3</t>
-  </si>
-  <si>
-    <t>ATSAMD21E</t>
-  </si>
-  <si>
-    <t>hack:QFN-32-1EP_5x5mm_Pitch0.5mm</t>
-  </si>
-  <si>
-    <t>ATSAMD21E18A-MU</t>
-  </si>
-  <si>
-    <t>D1</t>
-  </si>
-  <si>
-    <t>RED</t>
-  </si>
-  <si>
-    <t>hack:LED_0603_HandSoldering</t>
-  </si>
-  <si>
-    <t>304090042</t>
-  </si>
-  <si>
-    <t>R3</t>
-  </si>
-  <si>
-    <t>10k</t>
-  </si>
-  <si>
-    <t>301010299</t>
-  </si>
-  <si>
-    <t>P2,P3</t>
-  </si>
-  <si>
-    <t>CONN_01X13</t>
-  </si>
-  <si>
-    <t>hack-footprints:Pin_Castellated_1x13</t>
-  </si>
-  <si>
-    <t>JP1</t>
-  </si>
-  <si>
-    <t>Jumper_NO_Small</t>
-  </si>
-  <si>
-    <t>hack:SMD_Jumper</t>
-  </si>
-  <si>
-    <t>LOGO2</t>
-  </si>
-  <si>
-    <t>HACKADAY</t>
-  </si>
-  <si>
-    <t>hack:HACKADAY-LOGO</t>
-  </si>
-  <si>
-    <t>C8-C11</t>
-  </si>
-  <si>
-    <t>100nF</t>
-  </si>
-  <si>
-    <t>302010138</t>
-  </si>
-  <si>
-    <t>P4</t>
-  </si>
-  <si>
-    <t>CONN_01X01</t>
-  </si>
-  <si>
-    <t>hack-footprints:Pin_Castellated_1x01</t>
-  </si>
-  <si>
-    <t>P1</t>
-  </si>
-  <si>
-    <t>USB_micro</t>
-  </si>
-  <si>
-    <t>hack:47346-0001</t>
-  </si>
-  <si>
-    <t>320010000</t>
-  </si>
-  <si>
-    <t>C1,C2</t>
-  </si>
-  <si>
-    <t>2.2uF</t>
-  </si>
-  <si>
-    <t>302010054</t>
-  </si>
-  <si>
     <t>Board Qty:</t>
   </si>
   <si>
@@ -688,79 +855,94 @@
     <t>Cat#</t>
   </si>
   <si>
+    <t>493-2099-1-ND</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>STF202-22T1GOSCT-ND</t>
+  </si>
+  <si>
+    <t>PCD2293CT-ND</t>
+  </si>
+  <si>
+    <t>ATSAMD21E18A-MU-ND</t>
+  </si>
+  <si>
+    <t>490-3992-1-ND</t>
+  </si>
+  <si>
+    <t>13410-63200100000-ND</t>
+  </si>
+  <si>
+    <t>311-1814-1-ND</t>
+  </si>
+  <si>
     <t>576-4766-1-ND</t>
   </si>
   <si>
-    <t>Link</t>
-  </si>
-  <si>
-    <t>490-3992-1-ND</t>
-  </si>
-  <si>
-    <t>STF202-22T1GOSCT-ND</t>
-  </si>
-  <si>
-    <t>PCD2293CT-ND</t>
-  </si>
-  <si>
-    <t>493-2099-1-ND</t>
-  </si>
-  <si>
-    <t>ATSAMD21E18A-MU-ND</t>
-  </si>
-  <si>
-    <t>13410-63200100000-ND</t>
-  </si>
-  <si>
     <t>Mouser</t>
   </si>
   <si>
+    <t>647-UWX1C100MCL2</t>
+  </si>
+  <si>
+    <t>863-STF202-22T1G</t>
+  </si>
+  <si>
+    <t>667-ELL-VFG100MC</t>
+  </si>
+  <si>
+    <t>556-ATSAMD21E18A-MU</t>
+  </si>
+  <si>
+    <t>81-BLM18EG221SN1D</t>
+  </si>
+  <si>
+    <t>653-VAL</t>
+  </si>
+  <si>
+    <t>972-XLH3200100004X</t>
+  </si>
+  <si>
+    <t>603-CC603MRX5R5BB225</t>
+  </si>
+  <si>
     <t>998-MIC5528-3.3YMTTR</t>
   </si>
   <si>
-    <t>81-BLM18EG221SN1D</t>
-  </si>
-  <si>
-    <t>863-STF202-22T1G</t>
-  </si>
-  <si>
-    <t>667-ELL-VFG100MC</t>
-  </si>
-  <si>
     <t>575-3301010300240000</t>
   </si>
   <si>
-    <t>647-UWX1C100MCL2</t>
-  </si>
-  <si>
-    <t>653-VAL</t>
-  </si>
-  <si>
-    <t>556-ATSAMD21E18A-MU</t>
-  </si>
-  <si>
-    <t>972-XLH3200100004X</t>
-  </si>
-  <si>
     <t>Newark</t>
   </si>
   <si>
+    <t>58R3619</t>
+  </si>
+  <si>
+    <t>45J2271</t>
+  </si>
+  <si>
+    <t>15R1033</t>
+  </si>
+  <si>
+    <t>45X9914</t>
+  </si>
+  <si>
     <t>73M9090</t>
   </si>
   <si>
-    <t>45J2271</t>
-  </si>
-  <si>
-    <t>15R1033</t>
+    <t>90R7669</t>
   </si>
   <si>
     <t>76T1133</t>
   </si>
   <si>
-    <t>58R3619</t>
-  </si>
-  <si>
-    <t>45X9914</t>
+    <t>Local</t>
+  </si>
+  <si>
+    <t>Seeedstudio</t>
   </si>
 </sst>
 </file>
@@ -772,7 +954,7 @@
     <numFmt numFmtId="164" formatCode="$#,##0.00"/>
     <numFmt numFmtId="164" formatCode="$#,##0.00"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -820,6 +1002,14 @@
     </font>
     <font>
       <b/>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -827,7 +1017,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -858,6 +1048,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC0C0C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF909090"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -871,7 +1073,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -898,7 +1100,13 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1207,7 +1415,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AA55"/>
+  <dimension ref="A1:AM55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="9" ySplit="6" topLeftCell="J7" activePane="bottomRight" state="frozen"/>
@@ -1245,19 +1453,31 @@
     <col min="25" max="25" width="15.7109375" customWidth="1"/>
     <col min="26" max="26" width="9.140625" outlineLevel="2"/>
     <col min="27" max="27" width="9.140625" outlineLevel="2"/>
+    <col min="28" max="28" width="9.140625" outlineLevel="1"/>
+    <col min="29" max="29" width="9.140625" outlineLevel="2"/>
+    <col min="30" max="30" width="9.140625" outlineLevel="2"/>
+    <col min="31" max="31" width="15.7109375" customWidth="1"/>
+    <col min="32" max="32" width="9.140625" outlineLevel="2"/>
+    <col min="33" max="33" width="9.140625" outlineLevel="2"/>
+    <col min="34" max="34" width="9.140625" outlineLevel="1"/>
+    <col min="35" max="35" width="9.140625" outlineLevel="2"/>
+    <col min="36" max="36" width="9.140625" outlineLevel="2"/>
+    <col min="37" max="37" width="15.7109375" customWidth="1"/>
+    <col min="38" max="38" width="9.140625" outlineLevel="2"/>
+    <col min="39" max="39" width="9.140625" outlineLevel="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27">
+    <row r="1" spans="1:39">
       <c r="H1" s="2" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="I1" s="2">
         <v>100</v>
       </c>
     </row>
-    <row r="2" spans="1:27">
+    <row r="2" spans="1:39">
       <c r="H2" s="3" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="I2" s="4">
         <f>sum(I7:I30)</f>
@@ -1275,17 +1495,25 @@
         <f>sum(Y7:Y30)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:27">
+      <c r="AE2" s="4">
+        <f>sum(AE7:AE30)</f>
+        <v>0</v>
+      </c>
+      <c r="AK2" s="4">
+        <f>sum(AK7:AK30)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:39">
       <c r="H3" s="3" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="I3" s="5">
         <f>TotalCost/BoardQty</f>
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:27">
+    <row r="5" spans="1:39">
       <c r="A5" s="6" t="s">
         <v>0</v>
       </c>
@@ -1298,7 +1526,7 @@
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
       <c r="J5" s="7" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="K5" s="7"/>
       <c r="L5" s="7"/>
@@ -1306,7 +1534,7 @@
       <c r="N5" s="7"/>
       <c r="O5" s="7"/>
       <c r="P5" s="8" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="Q5" s="8"/>
       <c r="R5" s="8"/>
@@ -1314,98 +1542,150 @@
       <c r="T5" s="8"/>
       <c r="U5" s="8"/>
       <c r="V5" s="9" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="W5" s="9"/>
       <c r="X5" s="9"/>
       <c r="Y5" s="9"/>
       <c r="Z5" s="9"/>
       <c r="AA5" s="9"/>
-    </row>
-    <row r="6" spans="1:27">
-      <c r="A6" s="10" t="s">
+      <c r="AB5" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="AC5" s="10"/>
+      <c r="AD5" s="10"/>
+      <c r="AE5" s="10"/>
+      <c r="AF5" s="10"/>
+      <c r="AG5" s="10"/>
+      <c r="AH5" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="AI5" s="11"/>
+      <c r="AJ5" s="11"/>
+      <c r="AK5" s="11"/>
+      <c r="AL5" s="11"/>
+      <c r="AM5" s="11"/>
+    </row>
+    <row r="6" spans="1:39">
+      <c r="A6" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="10" t="s">
+      <c r="F6" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="G6" s="10" t="s">
+      <c r="G6" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="H6" s="10" t="s">
+      <c r="H6" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="I6" s="10" t="s">
+      <c r="I6" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="J6" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="K6" s="10" t="s">
-        <v>99</v>
-      </c>
-      <c r="L6" s="10" t="s">
+      <c r="J6" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="K6" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="L6" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="M6" s="10" t="s">
+      <c r="M6" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="N6" s="10" t="s">
+      <c r="N6" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="O6" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="O6" s="10" t="s">
-        <v>97</v>
-      </c>
-      <c r="P6" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="Q6" s="10" t="s">
-        <v>99</v>
-      </c>
-      <c r="R6" s="10" t="s">
+      <c r="P6" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="Q6" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="R6" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="S6" s="10" t="s">
+      <c r="S6" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="T6" s="10" t="s">
+      <c r="T6" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="U6" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="U6" s="10" t="s">
-        <v>97</v>
-      </c>
-      <c r="V6" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="W6" s="10" t="s">
-        <v>99</v>
-      </c>
-      <c r="X6" s="10" t="s">
+      <c r="V6" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="W6" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="X6" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="Y6" s="10" t="s">
+      <c r="Y6" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="Z6" s="10" t="s">
+      <c r="Z6" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="AA6" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="AA6" s="10" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="7" spans="1:27">
+      <c r="AB6" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="AC6" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="AD6" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="AE6" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="AF6" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="AG6" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="AH6" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="AI6" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="AJ6" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="AK6" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="AL6" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="AM6" s="12" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:39">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -1419,19 +1699,70 @@
         <v>13</v>
       </c>
       <c r="G7">
-        <f>BoardQty*1</f>
-        <v>0</v>
-      </c>
-      <c r="H7" s="11">
-        <f>MINA(INDIRECT(ADDRESS(ROW(),COLUMN(newark_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(digikey_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(mouser_part_data)+2)))</f>
-        <v>0</v>
-      </c>
-      <c r="I7" s="11">
+        <f>BoardQty*2</f>
+        <v>0</v>
+      </c>
+      <c r="H7" s="13">
+        <f>MINA(INDIRECT(ADDRESS(ROW(),COLUMN(newark_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(digikey_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(seeedstudio_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(local_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(mouser_part_data)+2)))</f>
+        <v>0</v>
+      </c>
+      <c r="I7" s="13">
         <f>iferror(G7*H7,"")</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:27">
+      <c r="J7">
+        <v>147965</v>
+      </c>
+      <c r="L7" s="13">
+        <f>iferror(lookup(if(K7="",G7,K7),{0,1,10,25,50,100,250,500,1000,2000,4000,10000,14000,50000,100000},{0.0,0.28,0.237,0.1628,0.1332,0.1184,0.0888,0.07844,0.06956,0.0592,0.05476,0.0518,0.04914,0.0444,0.03922}),"")</f>
+        <v>0</v>
+      </c>
+      <c r="M7" s="13">
+        <f>iferror(if(K7="",G7,K7)*L7,"")</f>
+        <v>0</v>
+      </c>
+      <c r="N7" t="s">
+        <v>104</v>
+      </c>
+      <c r="O7" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="P7">
+        <v>23290</v>
+      </c>
+      <c r="R7" s="13">
+        <f>iferror(lookup(if(Q7="",G7,Q7),{0,1,10,100,1000,2000,10000,24000,50000,100000},{0.0,0.279,0.134,0.078,0.07,0.055,0.05,0.048,0.045,0.04}),"")</f>
+        <v>0</v>
+      </c>
+      <c r="S7" s="13">
+        <f>iferror(if(Q7="",G7,Q7)*R7,"")</f>
+        <v>0</v>
+      </c>
+      <c r="T7" t="s">
+        <v>114</v>
+      </c>
+      <c r="U7" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="V7">
+        <v>1079</v>
+      </c>
+      <c r="X7" s="13">
+        <f>iferror(lookup(if(W7="",G7,W7),{0,1,10,25,50,100,250,500,1000},{0.0,0.318,0.296,0.195,0.162,0.138,0.111,0.098,0.087}),"")</f>
+        <v>0</v>
+      </c>
+      <c r="Y7" s="13">
+        <f>iferror(if(W7="",G7,W7)*X7,"")</f>
+        <v>0</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>125</v>
+      </c>
+      <c r="AA7" s="14" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="8" spans="1:39">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -1448,16 +1779,27 @@
         <f>BoardQty*1</f>
         <v>0</v>
       </c>
-      <c r="H8" s="11">
-        <f>MINA(INDIRECT(ADDRESS(ROW(),COLUMN(newark_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(digikey_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(mouser_part_data)+2)))</f>
-        <v>0</v>
-      </c>
-      <c r="I8" s="11">
+      <c r="H8" s="13">
+        <f>MINA(INDIRECT(ADDRESS(ROW(),COLUMN(newark_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(digikey_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(seeedstudio_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(local_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(mouser_part_data)+2)))</f>
+        <v>0</v>
+      </c>
+      <c r="I8" s="13">
         <f>iferror(G8*H8,"")</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:27">
+      <c r="AD8" s="13">
+        <f>iferror(lookup(if(AC8="",G8,AC8),{0,1},{0.0,0.03}),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AE8" s="13">
+        <f>iferror(if(AC8="",G8,AC8)*AD8,"")</f>
+        <v>0</v>
+      </c>
+      <c r="AF8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:39">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -1474,16 +1816,67 @@
         <f>BoardQty*1</f>
         <v>0</v>
       </c>
-      <c r="H9" s="11">
-        <f>MINA(INDIRECT(ADDRESS(ROW(),COLUMN(newark_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(digikey_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(mouser_part_data)+2)))</f>
-        <v>0</v>
-      </c>
-      <c r="I9" s="11">
+      <c r="H9" s="13">
+        <f>MINA(INDIRECT(ADDRESS(ROW(),COLUMN(newark_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(digikey_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(seeedstudio_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(local_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(mouser_part_data)+2)))</f>
+        <v>0</v>
+      </c>
+      <c r="I9" s="13">
         <f>iferror(G9*H9,"")</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:27">
+      <c r="J9">
+        <v>10898</v>
+      </c>
+      <c r="L9" s="13">
+        <f>iferror(lookup(if(K9="",G9,K9),{0,1,10,25,100,250,500,1000,3000,6000,15000,30000,75000,150000},{0.0,0.67,0.569,0.498,0.4264,0.36984,0.31326,0.2415,0.2139,0.2001,0.1863,0.17664,0.1725,0.1656}),"")</f>
+        <v>0</v>
+      </c>
+      <c r="M9" s="13">
+        <f>iferror(if(K9="",G9,K9)*L9,"")</f>
+        <v>0</v>
+      </c>
+      <c r="N9" t="s">
+        <v>106</v>
+      </c>
+      <c r="O9" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="P9">
+        <v>13023</v>
+      </c>
+      <c r="R9" s="13">
+        <f>iferror(lookup(if(Q9="",G9,Q9),{0,1,10,100,1000,3000,9000,24000},{0.0,0.651,0.492,0.308,0.232,0.197,0.183,0.18}),"")</f>
+        <v>0</v>
+      </c>
+      <c r="S9" s="13">
+        <f>iferror(if(Q9="",G9,Q9)*R9,"")</f>
+        <v>0</v>
+      </c>
+      <c r="T9" t="s">
+        <v>115</v>
+      </c>
+      <c r="U9" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="V9">
+        <v>7937</v>
+      </c>
+      <c r="X9" s="13">
+        <f>iferror(lookup(if(W9="",G9,W9),{0,1,25,100,250,500,1000,3000,9000},{0.0,0.66,0.483,0.304,0.294,0.286,0.235,0.201,0.187}),"")</f>
+        <v>0</v>
+      </c>
+      <c r="Y9" s="13">
+        <f>iferror(if(W9="",G9,W9)*X9,"")</f>
+        <v>0</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>126</v>
+      </c>
+      <c r="AA9" s="14" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="10" spans="1:39">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -1500,50 +1893,27 @@
         <f>BoardQty*1</f>
         <v>0</v>
       </c>
-      <c r="H10" s="11">
-        <f>MINA(INDIRECT(ADDRESS(ROW(),COLUMN(newark_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(digikey_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(mouser_part_data)+2)))</f>
-        <v>0</v>
-      </c>
-      <c r="I10" s="11">
+      <c r="H10" s="13">
+        <f>MINA(INDIRECT(ADDRESS(ROW(),COLUMN(newark_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(digikey_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(seeedstudio_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(local_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(mouser_part_data)+2)))</f>
+        <v>0</v>
+      </c>
+      <c r="I10" s="13">
         <f>iferror(G10*H10,"")</f>
         <v>0</v>
       </c>
-      <c r="J10">
-        <v>5000</v>
-      </c>
-      <c r="L10" s="11">
-        <f>iferror(lookup(if(K10="",G10,K10),{0,1,25,100,4500,5000},{0.0,0.19,0.16,0.14,0.24,0.14}),"")</f>
-        <v>0</v>
-      </c>
-      <c r="M10" s="11">
-        <f>iferror(if(K10="",G10,K10)*L10,"")</f>
-        <v>0</v>
-      </c>
-      <c r="N10" t="s">
-        <v>101</v>
-      </c>
-      <c r="O10" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="P10">
-        <v>4797</v>
-      </c>
-      <c r="R10" s="11">
-        <f>iferror(lookup(if(Q10="",G10,Q10),{0,1,10,25,100,5000},{0.0,0.197,0.187,0.158,0.138,0.138}),"")</f>
-        <v>0</v>
-      </c>
-      <c r="S10" s="11">
-        <f>iferror(if(Q10="",G10,Q10)*R10,"")</f>
-        <v>0</v>
-      </c>
-      <c r="T10" t="s">
-        <v>110</v>
-      </c>
-      <c r="U10" s="12" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="11" spans="1:27">
+      <c r="AD10" s="13">
+        <f>iferror(lookup(if(AC10="",G10,AC10),{0,1},{0.0,0.01}),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AE10" s="13">
+        <f>iferror(if(AC10="",G10,AC10)*AD10,"")</f>
+        <v>0</v>
+      </c>
+      <c r="AF10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:39">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -1560,67 +1930,67 @@
         <f>BoardQty*1</f>
         <v>0</v>
       </c>
-      <c r="H11" s="11">
-        <f>MINA(INDIRECT(ADDRESS(ROW(),COLUMN(newark_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(digikey_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(mouser_part_data)+2)))</f>
-        <v>0</v>
-      </c>
-      <c r="I11" s="11">
+      <c r="H11" s="13">
+        <f>MINA(INDIRECT(ADDRESS(ROW(),COLUMN(newark_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(digikey_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(seeedstudio_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(local_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(mouser_part_data)+2)))</f>
+        <v>0</v>
+      </c>
+      <c r="I11" s="13">
         <f>iferror(G11*H11,"")</f>
         <v>0</v>
       </c>
       <c r="J11">
-        <v>317364</v>
-      </c>
-      <c r="L11" s="11">
-        <f>iferror(lookup(if(K11="",G11,K11),{0,1,10,50,100,250,500,1000,4000,8000,12000},{0.0,0.23,0.175,0.1252,0.1126,0.09508,0.08508,0.07257,0.0637,0.05847,0.05688}),"")</f>
-        <v>0</v>
-      </c>
-      <c r="M11" s="11">
+        <v>2526</v>
+      </c>
+      <c r="L11" s="13">
+        <f>iferror(lookup(if(K11="",G11,K11),{0,1,10,50,100,500,2000,4000,6000,10000,20000},{0.0,0.54,0.51,0.4786,0.4466,0.3509,0.1914,0.18502,0.17864,0.17226,0.16397}),"")</f>
+        <v>0</v>
+      </c>
+      <c r="M11" s="13">
         <f>iferror(if(K11="",G11,K11)*L11,"")</f>
         <v>0</v>
       </c>
       <c r="N11" t="s">
-        <v>103</v>
-      </c>
-      <c r="O11" s="12" t="s">
-        <v>102</v>
+        <v>107</v>
+      </c>
+      <c r="O11" s="14" t="s">
+        <v>105</v>
       </c>
       <c r="P11">
-        <v>82768</v>
-      </c>
-      <c r="R11" s="11">
-        <f>iferror(lookup(if(Q11="",G11,Q11),{0,1,10,100,500,1000,4000,8000},{0.0,0.227,0.124,0.095,0.085,0.072,0.063,0.06}),"")</f>
-        <v>0</v>
-      </c>
-      <c r="S11" s="11">
+        <v>1767</v>
+      </c>
+      <c r="R11" s="13">
+        <f>iferror(lookup(if(Q11="",G11,Q11),{0,1,10,100,1000,2000,10000,24000,50000},{0.0,0.533,0.472,0.347,0.283,0.182,0.177,0.17,0.167}),"")</f>
+        <v>0</v>
+      </c>
+      <c r="S11" s="13">
         <f>iferror(if(Q11="",G11,Q11)*R11,"")</f>
         <v>0</v>
       </c>
       <c r="T11" t="s">
-        <v>111</v>
-      </c>
-      <c r="U11" s="12" t="s">
-        <v>102</v>
+        <v>116</v>
+      </c>
+      <c r="U11" s="14" t="s">
+        <v>105</v>
       </c>
       <c r="V11">
-        <v>6460</v>
-      </c>
-      <c r="X11" s="11">
-        <f>iferror(lookup(if(W11="",G11,W11),{0,1,50,100,500,1000,2500,5000,10000},{0.0,0.103,0.093,0.075,0.067,0.061,0.056,0.053,0.05}),"")</f>
-        <v>0</v>
-      </c>
-      <c r="Y11" s="11">
+        <v>0</v>
+      </c>
+      <c r="X11" s="13">
+        <f>iferror(lookup(if(W11="",G11,W11),{0,1,2000,4000,10000,20000,40000},{0.0,0.212,0.212,0.203,0.191,0.179,0.166}),"")</f>
+        <v>0</v>
+      </c>
+      <c r="Y11" s="13">
         <f>iferror(if(W11="",G11,W11)*X11,"")</f>
         <v>0</v>
       </c>
       <c r="Z11" t="s">
-        <v>120</v>
-      </c>
-      <c r="AA11" s="12" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="12" spans="1:27">
+        <v>127</v>
+      </c>
+      <c r="AA11" s="14" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="12" spans="1:39">
       <c r="A12" t="s">
         <v>30</v>
       </c>
@@ -1630,226 +2000,234 @@
       <c r="D12" t="s">
         <v>32</v>
       </c>
-      <c r="F12" t="s">
-        <v>33</v>
-      </c>
       <c r="G12">
         <f>BoardQty*1</f>
         <v>0</v>
       </c>
-      <c r="H12" s="11">
-        <f>MINA(INDIRECT(ADDRESS(ROW(),COLUMN(newark_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(digikey_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(mouser_part_data)+2)))</f>
-        <v>0</v>
-      </c>
-      <c r="I12" s="11">
+      <c r="H12" s="13">
+        <f>MINA(INDIRECT(ADDRESS(ROW(),COLUMN(newark_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(digikey_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(seeedstudio_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(local_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(mouser_part_data)+2)))</f>
+        <v>0</v>
+      </c>
+      <c r="I12" s="13">
         <f>iferror(G12*H12,"")</f>
         <v>0</v>
       </c>
-      <c r="J12">
-        <v>11398</v>
-      </c>
-      <c r="L12" s="11">
-        <f>iferror(lookup(if(K12="",G12,K12),{0,1,10,25,100,250,500,1000,3000,6000,15000,30000,75000,150000},{0.0,0.67,0.569,0.498,0.4264,0.36984,0.31326,0.2415,0.2139,0.2001,0.1863,0.17664,0.1725,0.1656}),"")</f>
-        <v>0</v>
-      </c>
-      <c r="M12" s="11">
-        <f>iferror(if(K12="",G12,K12)*L12,"")</f>
-        <v>0</v>
-      </c>
-      <c r="N12" t="s">
-        <v>104</v>
-      </c>
-      <c r="O12" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="P12">
-        <v>13023</v>
-      </c>
-      <c r="R12" s="11">
-        <f>iferror(lookup(if(Q12="",G12,Q12),{0,1,10,100,1000,3000,9000,24000},{0.0,0.651,0.492,0.308,0.232,0.197,0.183,0.18}),"")</f>
-        <v>0</v>
-      </c>
-      <c r="S12" s="11">
-        <f>iferror(if(Q12="",G12,Q12)*R12,"")</f>
-        <v>0</v>
-      </c>
-      <c r="T12" t="s">
-        <v>112</v>
-      </c>
-      <c r="U12" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="V12">
-        <v>7937</v>
-      </c>
-      <c r="X12" s="11">
-        <f>iferror(lookup(if(W12="",G12,W12),{0,1,25,100,250,500,1000,3000,9000},{0.0,0.66,0.483,0.304,0.294,0.286,0.235,0.201,0.187}),"")</f>
-        <v>0</v>
-      </c>
-      <c r="Y12" s="11">
-        <f>iferror(if(W12="",G12,W12)*X12,"")</f>
-        <v>0</v>
-      </c>
-      <c r="Z12" t="s">
-        <v>121</v>
-      </c>
-      <c r="AA12" s="12" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="13" spans="1:27">
+    </row>
+    <row r="13" spans="1:39">
       <c r="A13" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" t="s">
         <v>34</v>
       </c>
-      <c r="B13" t="s">
+      <c r="D13" t="s">
         <v>35</v>
       </c>
-      <c r="D13" t="s">
+      <c r="F13" t="s">
         <v>36</v>
-      </c>
-      <c r="F13" t="s">
-        <v>37</v>
       </c>
       <c r="G13">
         <f>BoardQty*1</f>
         <v>0</v>
       </c>
-      <c r="H13" s="11">
-        <f>MINA(INDIRECT(ADDRESS(ROW(),COLUMN(newark_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(digikey_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(mouser_part_data)+2)))</f>
-        <v>0</v>
-      </c>
-      <c r="I13" s="11">
+      <c r="H13" s="13">
+        <f>MINA(INDIRECT(ADDRESS(ROW(),COLUMN(newark_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(digikey_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(seeedstudio_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(local_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(mouser_part_data)+2)))</f>
+        <v>0</v>
+      </c>
+      <c r="I13" s="13">
         <f>iferror(G13*H13,"")</f>
         <v>0</v>
       </c>
       <c r="J13">
-        <v>2526</v>
-      </c>
-      <c r="L13" s="11">
-        <f>iferror(lookup(if(K13="",G13,K13),{0,1,10,50,100,500,2000,4000,6000,10000,20000},{0.0,0.54,0.51,0.4786,0.4466,0.3509,0.1914,0.18502,0.17864,0.17226,0.16397}),"")</f>
-        <v>0</v>
-      </c>
-      <c r="M13" s="11">
+        <v>956</v>
+      </c>
+      <c r="L13" s="13">
+        <f>iferror(lookup(if(K13="",G13,K13),{0,1,10,100,250,500,1000},{0.0,5.03,4.493,3.6845,3.325,2.98352,2.51622}),"")</f>
+        <v>0</v>
+      </c>
+      <c r="M13" s="13">
         <f>iferror(if(K13="",G13,K13)*L13,"")</f>
         <v>0</v>
       </c>
       <c r="N13" t="s">
+        <v>108</v>
+      </c>
+      <c r="O13" s="14" t="s">
         <v>105</v>
       </c>
-      <c r="O13" s="12" t="s">
-        <v>102</v>
-      </c>
       <c r="P13">
-        <v>1767</v>
-      </c>
-      <c r="R13" s="11">
-        <f>iferror(lookup(if(Q13="",G13,Q13),{0,1,10,100,1000,2000,10000,24000,50000},{0.0,0.533,0.472,0.347,0.283,0.182,0.177,0.17,0.167}),"")</f>
-        <v>0</v>
-      </c>
-      <c r="S13" s="11">
+        <v>328</v>
+      </c>
+      <c r="R13" s="13">
+        <f>iferror(lookup(if(Q13="",G13,Q13),{0,1,10,25,50,100,250,500,1000},{0.0,4.96,4.43,3.99,3.74,3.63,3.27,2.92,2.61}),"")</f>
+        <v>0</v>
+      </c>
+      <c r="S13" s="13">
         <f>iferror(if(Q13="",G13,Q13)*R13,"")</f>
         <v>0</v>
       </c>
       <c r="T13" t="s">
-        <v>113</v>
-      </c>
-      <c r="U13" s="12" t="s">
-        <v>102</v>
+        <v>117</v>
+      </c>
+      <c r="U13" s="14" t="s">
+        <v>105</v>
       </c>
       <c r="V13">
         <v>0</v>
       </c>
-      <c r="X13" s="11">
-        <f>iferror(lookup(if(W13="",G13,W13),{0,1,2000,4000,10000,20000,40000},{0.0,0.212,0.212,0.203,0.191,0.179,0.166}),"")</f>
-        <v>0</v>
-      </c>
-      <c r="Y13" s="11">
+      <c r="X13" s="13">
+        <f>iferror(lookup(if(W13="",G13,W13),{0,1,500,1000},{0.0,3.04,3.04,2.68}),"")</f>
+        <v>0</v>
+      </c>
+      <c r="Y13" s="13">
         <f>iferror(if(W13="",G13,W13)*X13,"")</f>
         <v>0</v>
       </c>
       <c r="Z13" t="s">
-        <v>122</v>
-      </c>
-      <c r="AA13" s="12" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="14" spans="1:27">
+        <v>128</v>
+      </c>
+      <c r="AA13" s="14" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="14" spans="1:39">
       <c r="A14" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" t="s">
         <v>38</v>
       </c>
-      <c r="B14" t="s">
+      <c r="D14" t="s">
         <v>39</v>
       </c>
-      <c r="D14" t="s">
+      <c r="F14" t="s">
         <v>40</v>
-      </c>
-      <c r="F14" t="s">
-        <v>41</v>
       </c>
       <c r="G14">
         <f>BoardQty*1</f>
         <v>0</v>
       </c>
-      <c r="H14" s="11">
-        <f>MINA(INDIRECT(ADDRESS(ROW(),COLUMN(newark_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(digikey_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(mouser_part_data)+2)))</f>
-        <v>0</v>
-      </c>
-      <c r="I14" s="11">
+      <c r="H14" s="13">
+        <f>MINA(INDIRECT(ADDRESS(ROW(),COLUMN(newark_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(digikey_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(seeedstudio_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(local_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(mouser_part_data)+2)))</f>
+        <v>0</v>
+      </c>
+      <c r="I14" s="13">
         <f>iferror(G14*H14,"")</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:27">
+      <c r="J14">
+        <v>317304</v>
+      </c>
+      <c r="L14" s="13">
+        <f>iferror(lookup(if(K14="",G14,K14),{0,1,10,50,100,250,500,1000,4000,8000,12000},{0.0,0.23,0.175,0.1252,0.1126,0.09508,0.08508,0.07257,0.0637,0.05847,0.05688}),"")</f>
+        <v>0</v>
+      </c>
+      <c r="M14" s="13">
+        <f>iferror(if(K14="",G14,K14)*L14,"")</f>
+        <v>0</v>
+      </c>
+      <c r="N14" t="s">
+        <v>109</v>
+      </c>
+      <c r="O14" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="P14">
+        <v>82768</v>
+      </c>
+      <c r="R14" s="13">
+        <f>iferror(lookup(if(Q14="",G14,Q14),{0,1,10,100,500,1000,4000,8000},{0.0,0.227,0.124,0.095,0.085,0.072,0.063,0.06}),"")</f>
+        <v>0</v>
+      </c>
+      <c r="S14" s="13">
+        <f>iferror(if(Q14="",G14,Q14)*R14,"")</f>
+        <v>0</v>
+      </c>
+      <c r="T14" t="s">
+        <v>118</v>
+      </c>
+      <c r="U14" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="V14">
+        <v>6460</v>
+      </c>
+      <c r="X14" s="13">
+        <f>iferror(lookup(if(W14="",G14,W14),{0,1,50,100,500,1000,2500,5000,10000},{0.0,0.103,0.093,0.075,0.067,0.061,0.056,0.053,0.05}),"")</f>
+        <v>0</v>
+      </c>
+      <c r="Y14" s="13">
+        <f>iferror(if(W14="",G14,W14)*X14,"")</f>
+        <v>0</v>
+      </c>
+      <c r="Z14" t="s">
+        <v>129</v>
+      </c>
+      <c r="AA14" s="14" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="15" spans="1:39">
       <c r="A15" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" t="s">
         <v>42</v>
       </c>
-      <c r="B15" t="s">
+      <c r="D15" t="s">
         <v>43</v>
-      </c>
-      <c r="D15" t="s">
-        <v>16</v>
       </c>
       <c r="F15" t="s">
         <v>44</v>
       </c>
       <c r="G15">
-        <f>BoardQty*2</f>
-        <v>0</v>
-      </c>
-      <c r="H15" s="11">
-        <f>MINA(INDIRECT(ADDRESS(ROW(),COLUMN(newark_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(digikey_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(mouser_part_data)+2)))</f>
-        <v>0</v>
-      </c>
-      <c r="I15" s="11">
+        <f>BoardQty*1</f>
+        <v>0</v>
+      </c>
+      <c r="H15" s="13">
+        <f>MINA(INDIRECT(ADDRESS(ROW(),COLUMN(newark_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(digikey_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(seeedstudio_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(local_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(mouser_part_data)+2)))</f>
+        <v>0</v>
+      </c>
+      <c r="I15" s="13">
         <f>iferror(G15*H15,"")</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:27">
+      <c r="AD15" s="13">
+        <f>iferror(lookup(if(AC15="",G15,AC15),{0,1},{0.0,0.01}),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AE15" s="13">
+        <f>iferror(if(AC15="",G15,AC15)*AD15,"")</f>
+        <v>0</v>
+      </c>
+      <c r="AF15" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:39">
       <c r="A16" t="s">
         <v>45</v>
       </c>
       <c r="B16" t="s">
         <v>46</v>
       </c>
-      <c r="F16" t="s">
+      <c r="D16" t="s">
         <v>47</v>
       </c>
       <c r="G16">
-        <f>BoardQty*1</f>
-        <v>0</v>
-      </c>
-      <c r="H16" s="11">
-        <f>MINA(INDIRECT(ADDRESS(ROW(),COLUMN(newark_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(digikey_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(mouser_part_data)+2)))</f>
-        <v>0</v>
-      </c>
-      <c r="I16" s="11">
+        <f>BoardQty*3</f>
+        <v>0</v>
+      </c>
+      <c r="H16" s="13">
+        <f>MINA(INDIRECT(ADDRESS(ROW(),COLUMN(newark_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(digikey_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(seeedstudio_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(local_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(mouser_part_data)+2)))</f>
+        <v>0</v>
+      </c>
+      <c r="I16" s="13">
         <f>iferror(G16*H16,"")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:27">
+    <row r="17" spans="1:38">
       <c r="A17" t="s">
         <v>48</v>
       </c>
@@ -1857,535 +2235,629 @@
         <v>49</v>
       </c>
       <c r="D17" t="s">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="F17" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="G17">
-        <f>BoardQty*2</f>
-        <v>0</v>
-      </c>
-      <c r="H17" s="11">
-        <f>MINA(INDIRECT(ADDRESS(ROW(),COLUMN(newark_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(digikey_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(mouser_part_data)+2)))</f>
-        <v>0</v>
-      </c>
-      <c r="I17" s="11">
+        <f>BoardQty*1</f>
+        <v>0</v>
+      </c>
+      <c r="H17" s="13">
+        <f>MINA(INDIRECT(ADDRESS(ROW(),COLUMN(newark_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(digikey_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(seeedstudio_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(local_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(mouser_part_data)+2)))</f>
+        <v>0</v>
+      </c>
+      <c r="I17" s="13">
         <f>iferror(G17*H17,"")</f>
         <v>0</v>
       </c>
-      <c r="P17">
-        <v>0</v>
-      </c>
-      <c r="R17" s="11">
-        <f>iferror(lookup(if(Q17="",G17,Q17),{0,1,10,25,50,100,250},{0.0,18.29,15.4,14.21,12.43,11.71,9.76}),"")</f>
-        <v>0</v>
-      </c>
-      <c r="S17" s="11">
-        <f>iferror(if(Q17="",G17,Q17)*R17,"")</f>
-        <v>0</v>
-      </c>
-      <c r="T17" t="s">
-        <v>114</v>
-      </c>
-      <c r="U17" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="V17">
-        <v>6</v>
-      </c>
-      <c r="X17" s="11">
-        <f>iferror(lookup(if(W17="",G17,W17),{0,1,25,50,100,250},{0.0,85.14,81.25,79.09,76.5,73.91}),"")</f>
-        <v>0</v>
-      </c>
-      <c r="Y17" s="11">
-        <f>iferror(if(W17="",G17,W17)*X17,"")</f>
-        <v>0</v>
-      </c>
-      <c r="Z17" t="s">
-        <v>123</v>
-      </c>
-      <c r="AA17" s="12" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="18" spans="1:27">
+      <c r="AD17" s="13">
+        <f>iferror(lookup(if(AC17="",G17,AC17),{0,1},{0.0,0.2036}),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AE17" s="13">
+        <f>iferror(if(AC17="",G17,AC17)*AD17,"")</f>
+        <v>0</v>
+      </c>
+      <c r="AF17" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="1:38">
       <c r="A18" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B18" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D18" t="s">
-        <v>53</v>
+        <v>54</v>
+      </c>
+      <c r="F18" t="s">
+        <v>8</v>
       </c>
       <c r="G18">
-        <f>BoardQty*3</f>
-        <v>0</v>
-      </c>
-      <c r="H18" s="11">
-        <f>MINA(INDIRECT(ADDRESS(ROW(),COLUMN(newark_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(digikey_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(mouser_part_data)+2)))</f>
-        <v>0</v>
-      </c>
-      <c r="I18" s="11">
+        <f>BoardQty*1</f>
+        <v>0</v>
+      </c>
+      <c r="H18" s="13">
+        <f>MINA(INDIRECT(ADDRESS(ROW(),COLUMN(newark_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(digikey_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(seeedstudio_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(local_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(mouser_part_data)+2)))</f>
+        <v>0</v>
+      </c>
+      <c r="I18" s="13">
         <f>iferror(G18*H18,"")</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:27">
+      <c r="P18">
+        <v>149</v>
+      </c>
+      <c r="R18" s="13">
+        <f>iferror(lookup(if(Q18="",G18,Q18),{0,1,25,50,100,200,500},{0.0,1.1,1.02,0.937,0.859,0.799,0.749}),"")</f>
+        <v>0</v>
+      </c>
+      <c r="S18" s="13">
+        <f>iferror(if(Q18="",G18,Q18)*R18,"")</f>
+        <v>0</v>
+      </c>
+      <c r="T18" t="s">
+        <v>119</v>
+      </c>
+      <c r="U18" s="14" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="19" spans="1:38">
       <c r="A19" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B19" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D19" t="s">
-        <v>56</v>
-      </c>
-      <c r="F19" t="s">
         <v>57</v>
       </c>
       <c r="G19">
-        <f>BoardQty*2</f>
-        <v>0</v>
-      </c>
-      <c r="H19" s="11">
-        <f>MINA(INDIRECT(ADDRESS(ROW(),COLUMN(newark_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(digikey_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(mouser_part_data)+2)))</f>
-        <v>0</v>
-      </c>
-      <c r="I19" s="11">
+        <f>BoardQty*1</f>
+        <v>0</v>
+      </c>
+      <c r="H19" s="13">
+        <f>MINA(INDIRECT(ADDRESS(ROW(),COLUMN(newark_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(digikey_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(seeedstudio_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(local_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(mouser_part_data)+2)))</f>
+        <v>0</v>
+      </c>
+      <c r="I19" s="13">
         <f>iferror(G19*H19,"")</f>
         <v>0</v>
       </c>
-      <c r="J19">
-        <v>147965</v>
-      </c>
-      <c r="L19" s="11">
-        <f>iferror(lookup(if(K19="",G19,K19),{0,1,10,25,50,100,250,500,1000,2000,4000,10000,14000,50000,100000},{0.0,0.28,0.237,0.1628,0.1332,0.1184,0.0888,0.07844,0.06956,0.0592,0.05476,0.0518,0.04914,0.0444,0.03922}),"")</f>
-        <v>0</v>
-      </c>
-      <c r="M19" s="11">
-        <f>iferror(if(K19="",G19,K19)*L19,"")</f>
-        <v>0</v>
-      </c>
-      <c r="N19" t="s">
-        <v>106</v>
-      </c>
-      <c r="O19" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="P19">
-        <v>23340</v>
-      </c>
-      <c r="R19" s="11">
-        <f>iferror(lookup(if(Q19="",G19,Q19),{0,1,10,100,1000,2000,10000,24000,50000,100000},{0.0,0.279,0.134,0.078,0.07,0.055,0.05,0.048,0.045,0.04}),"")</f>
-        <v>0</v>
-      </c>
-      <c r="S19" s="11">
-        <f>iferror(if(Q19="",G19,Q19)*R19,"")</f>
-        <v>0</v>
-      </c>
-      <c r="T19" t="s">
-        <v>115</v>
-      </c>
-      <c r="U19" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="V19">
-        <v>1079</v>
-      </c>
-      <c r="X19" s="11">
-        <f>iferror(lookup(if(W19="",G19,W19),{0,1,10,25,50,100,250,500,1000},{0.0,0.318,0.296,0.195,0.162,0.138,0.111,0.098,0.087}),"")</f>
-        <v>0</v>
-      </c>
-      <c r="Y19" s="11">
-        <f>iferror(if(W19="",G19,W19)*X19,"")</f>
-        <v>0</v>
-      </c>
-      <c r="Z19" t="s">
-        <v>124</v>
-      </c>
-      <c r="AA19" s="12" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="20" spans="1:27">
+    </row>
+    <row r="20" spans="1:38">
       <c r="A20" t="s">
         <v>58</v>
       </c>
       <c r="B20" t="s">
         <v>59</v>
       </c>
+      <c r="D20" t="s">
+        <v>60</v>
+      </c>
       <c r="F20" t="s">
-        <v>8</v>
+        <v>61</v>
       </c>
       <c r="G20">
         <f>BoardQty*1</f>
         <v>0</v>
       </c>
-      <c r="H20" s="11">
-        <f>MINA(INDIRECT(ADDRESS(ROW(),COLUMN(newark_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(digikey_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(mouser_part_data)+2)))</f>
-        <v>0</v>
-      </c>
-      <c r="I20" s="11">
+      <c r="H20" s="13">
+        <f>MINA(INDIRECT(ADDRESS(ROW(),COLUMN(newark_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(digikey_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(seeedstudio_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(local_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(mouser_part_data)+2)))</f>
+        <v>0</v>
+      </c>
+      <c r="I20" s="13">
         <f>iferror(G20*H20,"")</f>
         <v>0</v>
       </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+      <c r="L20" s="13">
+        <f>iferror(lookup(if(K20="",G20,K20),{0,1,60,120,300},{0.0,22.5085,22.5085,16.58542,12.8061}),"")</f>
+        <v>0</v>
+      </c>
+      <c r="M20" s="13">
+        <f>iferror(if(K20="",G20,K20)*L20,"")</f>
+        <v>0</v>
+      </c>
+      <c r="N20" t="s">
+        <v>110</v>
+      </c>
+      <c r="O20" s="14" t="s">
+        <v>105</v>
+      </c>
       <c r="P20">
-        <v>149</v>
-      </c>
-      <c r="R20" s="11">
-        <f>iferror(lookup(if(Q20="",G20,Q20),{0,1,25,50,100,200,500},{0.0,1.1,1.02,0.937,0.859,0.799,0.749}),"")</f>
-        <v>0</v>
-      </c>
-      <c r="S20" s="11">
+        <v>0</v>
+      </c>
+      <c r="R20" s="13">
+        <f>iferror(lookup(if(Q20="",G20,Q20),{0,1,100,200,500,1000,2000,5000},{0.0,1.93,1.93,1.83,1.69,1.4,1.3,1.29}),"")</f>
+        <v>0</v>
+      </c>
+      <c r="S20" s="13">
         <f>iferror(if(Q20="",G20,Q20)*R20,"")</f>
         <v>0</v>
       </c>
       <c r="T20" t="s">
-        <v>116</v>
-      </c>
-      <c r="U20" s="12" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="21" spans="1:27">
+        <v>120</v>
+      </c>
+      <c r="U20" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="AD20" s="13">
+        <f>iferror(lookup(if(AC20="",G20,AC20),{0,1},{0.0,0.3}),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AE20" s="13">
+        <f>iferror(if(AC20="",G20,AC20)*AD20,"")</f>
+        <v>0</v>
+      </c>
+      <c r="AF20" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="21" spans="1:38">
       <c r="A21" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B21" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D21" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="F21" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="G21">
         <f>BoardQty*1</f>
         <v>0</v>
       </c>
-      <c r="H21" s="11">
-        <f>MINA(INDIRECT(ADDRESS(ROW(),COLUMN(newark_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(digikey_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(mouser_part_data)+2)))</f>
-        <v>0</v>
-      </c>
-      <c r="I21" s="11">
+      <c r="H21" s="13">
+        <f>MINA(INDIRECT(ADDRESS(ROW(),COLUMN(newark_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(digikey_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(seeedstudio_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(local_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(mouser_part_data)+2)))</f>
+        <v>0</v>
+      </c>
+      <c r="I21" s="13">
         <f>iferror(G21*H21,"")</f>
         <v>0</v>
       </c>
-      <c r="J21">
-        <v>956</v>
-      </c>
-      <c r="L21" s="11">
-        <f>iferror(lookup(if(K21="",G21,K21),{0,1,10,100,250,500,1000},{0.0,5.03,4.493,3.6845,3.325,2.98352,2.51622}),"")</f>
-        <v>0</v>
-      </c>
-      <c r="M21" s="11">
-        <f>iferror(if(K21="",G21,K21)*L21,"")</f>
-        <v>0</v>
-      </c>
-      <c r="N21" t="s">
-        <v>107</v>
-      </c>
-      <c r="O21" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="P21">
-        <v>328</v>
-      </c>
-      <c r="R21" s="11">
-        <f>iferror(lookup(if(Q21="",G21,Q21),{0,1,10,25,50,100,250,500,1000},{0.0,4.96,4.43,3.99,3.74,3.63,3.27,2.92,2.61}),"")</f>
-        <v>0</v>
-      </c>
-      <c r="S21" s="11">
-        <f>iferror(if(Q21="",G21,Q21)*R21,"")</f>
-        <v>0</v>
-      </c>
-      <c r="T21" t="s">
-        <v>117</v>
-      </c>
-      <c r="U21" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="V21">
-        <v>0</v>
-      </c>
-      <c r="X21" s="11">
-        <f>iferror(lookup(if(W21="",G21,W21),{0,1,500,1000},{0.0,3.04,3.04,2.68}),"")</f>
-        <v>0</v>
-      </c>
-      <c r="Y21" s="11">
-        <f>iferror(if(W21="",G21,W21)*X21,"")</f>
-        <v>0</v>
-      </c>
-      <c r="Z21" t="s">
-        <v>125</v>
-      </c>
-      <c r="AA21" s="12" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="22" spans="1:27">
+      <c r="AD21" s="13">
+        <f>iferror(lookup(if(AC21="",G21,AC21),{0,1},{0.0,0.35}),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AE21" s="13">
+        <f>iferror(if(AC21="",G21,AC21)*AD21,"")</f>
+        <v>0</v>
+      </c>
+      <c r="AF21" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="22" spans="1:38">
       <c r="A22" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B22" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D22" t="s">
-        <v>66</v>
+        <v>24</v>
       </c>
       <c r="F22" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="G22">
-        <f>BoardQty*1</f>
-        <v>0</v>
-      </c>
-      <c r="H22" s="11">
-        <f>MINA(INDIRECT(ADDRESS(ROW(),COLUMN(newark_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(digikey_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(mouser_part_data)+2)))</f>
-        <v>0</v>
-      </c>
-      <c r="I22" s="11">
+        <f>BoardQty*2</f>
+        <v>0</v>
+      </c>
+      <c r="H22" s="13">
+        <f>MINA(INDIRECT(ADDRESS(ROW(),COLUMN(newark_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(digikey_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(seeedstudio_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(local_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(mouser_part_data)+2)))</f>
+        <v>0</v>
+      </c>
+      <c r="I22" s="13">
         <f>iferror(G22*H22,"")</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:27">
+      <c r="J22">
+        <v>6174</v>
+      </c>
+      <c r="L22" s="13">
+        <f>iferror(lookup(if(K22="",G22,K22),{0,1,10,25,100,250,500,1000,4000,8000,12000,28000,100000},{0.0,0.1,0.072,0.0508,0.0329,0.02692,0.02302,0.01794,0.01376,0.01256,0.01196,0.01136,0.00822}),"")</f>
+        <v>0</v>
+      </c>
+      <c r="M22" s="13">
+        <f>iferror(if(K22="",G22,K22)*L22,"")</f>
+        <v>0</v>
+      </c>
+      <c r="N22" t="s">
+        <v>111</v>
+      </c>
+      <c r="O22" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="P22">
+        <v>4215</v>
+      </c>
+      <c r="R22" s="13">
+        <f>iferror(lookup(if(Q22="",G22,Q22),{0,1,10,100,1000,4000,24000,48000,100000},{0.0,0.099,0.052,0.024,0.019,0.013,0.012,0.011,0.009}),"")</f>
+        <v>0</v>
+      </c>
+      <c r="S22" s="13">
+        <f>iferror(if(Q22="",G22,Q22)*R22,"")</f>
+        <v>0</v>
+      </c>
+      <c r="T22" t="s">
+        <v>121</v>
+      </c>
+      <c r="U22" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="V22">
+        <v>3335</v>
+      </c>
+      <c r="X22" s="13">
+        <f>iferror(lookup(if(W22="",G22,W22),{0,1,10,100,250,500,1000},{0.0,0.16,0.11,0.053,0.044,0.037,0.03}),"")</f>
+        <v>0</v>
+      </c>
+      <c r="Y22" s="13">
+        <f>iferror(if(W22="",G22,W22)*X22,"")</f>
+        <v>0</v>
+      </c>
+      <c r="Z22" t="s">
+        <v>130</v>
+      </c>
+      <c r="AA22" s="14" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="23" spans="1:38">
       <c r="A23" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B23" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D23" t="s">
-        <v>20</v>
+        <v>71</v>
       </c>
       <c r="F23" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="G23">
         <f>BoardQty*1</f>
         <v>0</v>
       </c>
-      <c r="H23" s="11">
-        <f>MINA(INDIRECT(ADDRESS(ROW(),COLUMN(newark_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(digikey_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(mouser_part_data)+2)))</f>
-        <v>0</v>
-      </c>
-      <c r="I23" s="11">
+      <c r="H23" s="13">
+        <f>MINA(INDIRECT(ADDRESS(ROW(),COLUMN(newark_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(digikey_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(seeedstudio_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(local_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(mouser_part_data)+2)))</f>
+        <v>0</v>
+      </c>
+      <c r="I23" s="13">
         <f>iferror(G23*H23,"")</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:27">
+      <c r="J23">
+        <v>5000</v>
+      </c>
+      <c r="L23" s="13">
+        <f>iferror(lookup(if(K23="",G23,K23),{0,1,25,100,4500,5000},{0.0,0.19,0.16,0.14,0.24,0.14}),"")</f>
+        <v>0</v>
+      </c>
+      <c r="M23" s="13">
+        <f>iferror(if(K23="",G23,K23)*L23,"")</f>
+        <v>0</v>
+      </c>
+      <c r="N23" t="s">
+        <v>112</v>
+      </c>
+      <c r="O23" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="P23">
+        <v>4797</v>
+      </c>
+      <c r="R23" s="13">
+        <f>iferror(lookup(if(Q23="",G23,Q23),{0,1,10,25,100,5000},{0.0,0.197,0.187,0.158,0.138,0.138}),"")</f>
+        <v>0</v>
+      </c>
+      <c r="S23" s="13">
+        <f>iferror(if(Q23="",G23,Q23)*R23,"")</f>
+        <v>0</v>
+      </c>
+      <c r="T23" t="s">
+        <v>122</v>
+      </c>
+      <c r="U23" s="14" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="24" spans="1:38">
       <c r="A24" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B24" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D24" t="s">
-        <v>73</v>
+        <v>75</v>
+      </c>
+      <c r="F24" t="s">
+        <v>76</v>
       </c>
       <c r="G24">
-        <f>BoardQty*2</f>
-        <v>0</v>
-      </c>
-      <c r="H24" s="11">
-        <f>MINA(INDIRECT(ADDRESS(ROW(),COLUMN(newark_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(digikey_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(mouser_part_data)+2)))</f>
-        <v>0</v>
-      </c>
-      <c r="I24" s="11">
+        <f>BoardQty*1</f>
+        <v>0</v>
+      </c>
+      <c r="H24" s="13">
+        <f>MINA(INDIRECT(ADDRESS(ROW(),COLUMN(newark_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(digikey_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(seeedstudio_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(local_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(mouser_part_data)+2)))</f>
+        <v>0</v>
+      </c>
+      <c r="I24" s="13">
         <f>iferror(G24*H24,"")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:27">
+    <row r="25" spans="1:38">
       <c r="A25" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="B25" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="D25" t="s">
-        <v>76</v>
+        <v>24</v>
+      </c>
+      <c r="F25" t="s">
+        <v>79</v>
       </c>
       <c r="G25">
-        <f>BoardQty*1</f>
-        <v>0</v>
-      </c>
-      <c r="H25" s="11">
-        <f>MINA(INDIRECT(ADDRESS(ROW(),COLUMN(newark_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(digikey_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(mouser_part_data)+2)))</f>
-        <v>0</v>
-      </c>
-      <c r="I25" s="11">
+        <f>BoardQty*4</f>
+        <v>0</v>
+      </c>
+      <c r="H25" s="13">
+        <f>MINA(INDIRECT(ADDRESS(ROW(),COLUMN(newark_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(digikey_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(seeedstudio_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(local_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(mouser_part_data)+2)))</f>
+        <v>0</v>
+      </c>
+      <c r="I25" s="13">
         <f>iferror(G25*H25,"")</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:27">
+      <c r="AD25" s="13">
+        <f>iferror(lookup(if(AC25="",G25,AC25),{0,1},{0.0,0.02}),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AE25" s="13">
+        <f>iferror(if(AC25="",G25,AC25)*AD25,"")</f>
+        <v>0</v>
+      </c>
+      <c r="AF25" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="26" spans="1:38">
       <c r="A26" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B26" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="D26" t="s">
-        <v>79</v>
+        <v>43</v>
       </c>
       <c r="F26" t="s">
-        <v>41</v>
+        <v>82</v>
       </c>
       <c r="G26">
         <f>BoardQty*1</f>
         <v>0</v>
       </c>
-      <c r="H26" s="11">
-        <f>MINA(INDIRECT(ADDRESS(ROW(),COLUMN(newark_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(digikey_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(mouser_part_data)+2)))</f>
-        <v>0</v>
-      </c>
-      <c r="I26" s="11">
+      <c r="H26" s="13">
+        <f>MINA(INDIRECT(ADDRESS(ROW(),COLUMN(newark_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(digikey_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(seeedstudio_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(local_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(mouser_part_data)+2)))</f>
+        <v>0</v>
+      </c>
+      <c r="I26" s="13">
         <f>iferror(G26*H26,"")</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:27">
+      <c r="AD26" s="13">
+        <f>iferror(lookup(if(AC26="",G26,AC26),{0,1},{0.0,0.01}),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AE26" s="13">
+        <f>iferror(if(AC26="",G26,AC26)*AD26,"")</f>
+        <v>0</v>
+      </c>
+      <c r="AF26" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="27" spans="1:38">
       <c r="A27" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B27" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="D27" t="s">
-        <v>16</v>
+        <v>85</v>
       </c>
       <c r="F27" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="G27">
-        <f>BoardQty*4</f>
-        <v>0</v>
-      </c>
-      <c r="H27" s="11">
-        <f>MINA(INDIRECT(ADDRESS(ROW(),COLUMN(newark_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(digikey_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(mouser_part_data)+2)))</f>
-        <v>0</v>
-      </c>
-      <c r="I27" s="11">
+        <f>BoardQty*1</f>
+        <v>0</v>
+      </c>
+      <c r="H27" s="13">
+        <f>MINA(INDIRECT(ADDRESS(ROW(),COLUMN(newark_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(digikey_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(seeedstudio_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(local_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(mouser_part_data)+2)))</f>
+        <v>0</v>
+      </c>
+      <c r="I27" s="13">
         <f>iferror(G27*H27,"")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:27">
+    <row r="28" spans="1:38">
       <c r="A28" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B28" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="D28" t="s">
-        <v>85</v>
+        <v>88</v>
+      </c>
+      <c r="F28" t="s">
+        <v>89</v>
       </c>
       <c r="G28">
-        <f>BoardQty*1</f>
-        <v>0</v>
-      </c>
-      <c r="H28" s="11">
-        <f>MINA(INDIRECT(ADDRESS(ROW(),COLUMN(newark_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(digikey_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(mouser_part_data)+2)))</f>
-        <v>0</v>
-      </c>
-      <c r="I28" s="11">
+        <f>BoardQty*2</f>
+        <v>0</v>
+      </c>
+      <c r="H28" s="13">
+        <f>MINA(INDIRECT(ADDRESS(ROW(),COLUMN(newark_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(digikey_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(seeedstudio_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(local_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(mouser_part_data)+2)))</f>
+        <v>0</v>
+      </c>
+      <c r="I28" s="13">
         <f>iferror(G28*H28,"")</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:27">
+      <c r="AD28" s="13">
+        <f>iferror(lookup(if(AC28="",G28,AC28),{0,1},{0.0,0.08}),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AE28" s="13">
+        <f>iferror(if(AC28="",G28,AC28)*AD28,"")</f>
+        <v>0</v>
+      </c>
+      <c r="AF28" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="29" spans="1:38">
       <c r="A29" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="B29" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="D29" t="s">
-        <v>88</v>
+        <v>43</v>
       </c>
       <c r="F29" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="G29">
-        <f>BoardQty*1</f>
-        <v>0</v>
-      </c>
-      <c r="H29" s="11">
-        <f>MINA(INDIRECT(ADDRESS(ROW(),COLUMN(newark_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(digikey_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(mouser_part_data)+2)))</f>
-        <v>0</v>
-      </c>
-      <c r="I29" s="11">
+        <f>BoardQty*2</f>
+        <v>0</v>
+      </c>
+      <c r="H29" s="13">
+        <f>MINA(INDIRECT(ADDRESS(ROW(),COLUMN(newark_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(digikey_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(seeedstudio_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(local_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(mouser_part_data)+2)))</f>
+        <v>0</v>
+      </c>
+      <c r="I29" s="13">
         <f>iferror(G29*H29,"")</f>
         <v>0</v>
       </c>
-      <c r="J29">
-        <v>0</v>
-      </c>
-      <c r="L29" s="11">
-        <f>iferror(lookup(if(K29="",G29,K29),{0,1,60,120,300},{0.0,22.5085,22.5085,16.58542,12.8061}),"")</f>
-        <v>0</v>
-      </c>
-      <c r="M29" s="11">
-        <f>iferror(if(K29="",G29,K29)*L29,"")</f>
-        <v>0</v>
-      </c>
-      <c r="N29" t="s">
-        <v>108</v>
-      </c>
-      <c r="O29" s="12" t="s">
-        <v>102</v>
-      </c>
       <c r="P29">
         <v>0</v>
       </c>
-      <c r="R29" s="11">
-        <f>iferror(lookup(if(Q29="",G29,Q29),{0,1,100,200,500,1000,2000,5000},{0.0,1.93,1.93,1.83,1.69,1.4,1.3,1.29}),"")</f>
-        <v>0</v>
-      </c>
-      <c r="S29" s="11">
+      <c r="R29" s="13">
+        <f>iferror(lookup(if(Q29="",G29,Q29),{0,1,10,25,50,100,250},{0.0,18.29,15.4,14.21,12.43,11.71,9.76}),"")</f>
+        <v>0</v>
+      </c>
+      <c r="S29" s="13">
         <f>iferror(if(Q29="",G29,Q29)*R29,"")</f>
         <v>0</v>
       </c>
       <c r="T29" t="s">
-        <v>118</v>
-      </c>
-      <c r="U29" s="12" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="30" spans="1:27">
+        <v>123</v>
+      </c>
+      <c r="U29" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="V29">
+        <v>6</v>
+      </c>
+      <c r="X29" s="13">
+        <f>iferror(lookup(if(W29="",G29,W29),{0,1,25,50,100,250},{0.0,85.14,81.25,79.09,76.5,73.91}),"")</f>
+        <v>0</v>
+      </c>
+      <c r="Y29" s="13">
+        <f>iferror(if(W29="",G29,W29)*X29,"")</f>
+        <v>0</v>
+      </c>
+      <c r="Z29" t="s">
+        <v>131</v>
+      </c>
+      <c r="AA29" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="AD29" s="13">
+        <f>iferror(lookup(if(AC29="",G29,AC29),{0,1},{0.0,0.01}),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AE29" s="13">
+        <f>iferror(if(AC29="",G29,AC29)*AD29,"")</f>
+        <v>0</v>
+      </c>
+      <c r="AF29" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="30" spans="1:38">
       <c r="A30" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="B30" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="D30" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="F30" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="G30">
         <f>BoardQty*2</f>
         <v>0</v>
       </c>
-      <c r="H30" s="11">
-        <f>MINA(INDIRECT(ADDRESS(ROW(),COLUMN(newark_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(digikey_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(mouser_part_data)+2)))</f>
-        <v>0</v>
-      </c>
-      <c r="I30" s="11">
+      <c r="H30" s="13">
+        <f>MINA(INDIRECT(ADDRESS(ROW(),COLUMN(newark_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(digikey_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(seeedstudio_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(local_part_data)+2)),INDIRECT(ADDRESS(ROW(),COLUMN(mouser_part_data)+2)))</f>
+        <v>0</v>
+      </c>
+      <c r="I30" s="13">
         <f>iferror(G30*H30,"")</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:27">
+      <c r="AD30" s="13">
+        <f>iferror(lookup(if(AC30="",G30,AC30),{0,1},{0.0,0.01}),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AE30" s="13">
+        <f>iferror(if(AC30="",G30,AC30)*AD30,"")</f>
+        <v>0</v>
+      </c>
+      <c r="AF30" t="s">
+        <v>95</v>
+      </c>
+      <c r="AJ30" s="13">
+        <f>iferror(lookup(if(AI30="",G30,AI30),{0,1,100},{0.0,1.0,1.0}),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AK30" s="13">
+        <f>iferror(if(AI30="",G30,AI30)*AJ30,"")</f>
+        <v>0</v>
+      </c>
+      <c r="AL30" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="32" spans="1:38">
       <c r="K32">
         <f t="array" ref="K32">IFERROR(CONCATENATE(TEXT(INDEX($K$7:$K$30,SMALL(IF($N$7:$N$30&lt;&gt;"",IF($K$7:$K$30&lt;&gt;"",ROW($K$7:$K$30)-MIN(ROW($K$7:$K$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0"),","),"")</f>
         <v>0</v>
@@ -2422,8 +2894,32 @@
         <f t="array" ref="Y32">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($Z$7:$Z$30&lt;&gt;"",IF($W$7:$W$30&lt;&gt;"",ROW($W$7:$W$30)-MIN(ROW($W$7:$W$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="11:25">
+      <c r="AC32">
+        <f t="array" ref="AC32">IFERROR(CONCATENATE(TEXT(INDEX($AC$7:$AC$30,SMALL(IF($AF$7:$AF$30&lt;&gt;"",IF($AC$7:$AC$30&lt;&gt;"",ROW($AC$7:$AC$30)-MIN(ROW($AC$7:$AC$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0"),),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AD32">
+        <f t="array" ref="AD32">IFERROR(CONCATENATE((INDEX($AF$7:$AF$30,SMALL(IF($AF$7:$AF$30&lt;&gt;"",IF($AC$7:$AC$30&lt;&gt;"",ROW($AC$7:$AC$30)-MIN(ROW($AC$7:$AC$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AE32">
+        <f t="array" ref="AE32">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($AF$7:$AF$30&lt;&gt;"",IF($AC$7:$AC$30&lt;&gt;"",ROW($AC$7:$AC$30)-MIN(ROW($AC$7:$AC$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AI32">
+        <f t="array" ref="AI32">IFERROR(CONCATENATE(TEXT(INDEX($AI$7:$AI$30,SMALL(IF($AL$7:$AL$30&lt;&gt;"",IF($AI$7:$AI$30&lt;&gt;"",ROW($AI$7:$AI$30)-MIN(ROW($AI$7:$AI$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0"),),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AJ32">
+        <f t="array" ref="AJ32">IFERROR(CONCATENATE((INDEX($AL$7:$AL$30,SMALL(IF($AL$7:$AL$30&lt;&gt;"",IF($AI$7:$AI$30&lt;&gt;"",ROW($AI$7:$AI$30)-MIN(ROW($AI$7:$AI$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AK32">
+        <f t="array" ref="AK32">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($AL$7:$AL$30&lt;&gt;"",IF($AI$7:$AI$30&lt;&gt;"",ROW($AI$7:$AI$30)-MIN(ROW($AI$7:$AI$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="11:37">
       <c r="K33">
         <f t="array" ref="K33">IFERROR(CONCATENATE(TEXT(INDEX($K$7:$K$30,SMALL(IF($N$7:$N$30&lt;&gt;"",IF($K$7:$K$30&lt;&gt;"",ROW($K$7:$K$30)-MIN(ROW($K$7:$K$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0"),","),"")</f>
         <v>0</v>
@@ -2460,8 +2956,32 @@
         <f t="array" ref="Y33">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($Z$7:$Z$30&lt;&gt;"",IF($W$7:$W$30&lt;&gt;"",ROW($W$7:$W$30)-MIN(ROW($W$7:$W$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="11:25">
+      <c r="AC33">
+        <f t="array" ref="AC33">IFERROR(CONCATENATE(TEXT(INDEX($AC$7:$AC$30,SMALL(IF($AF$7:$AF$30&lt;&gt;"",IF($AC$7:$AC$30&lt;&gt;"",ROW($AC$7:$AC$30)-MIN(ROW($AC$7:$AC$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0"),),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AD33">
+        <f t="array" ref="AD33">IFERROR(CONCATENATE((INDEX($AF$7:$AF$30,SMALL(IF($AF$7:$AF$30&lt;&gt;"",IF($AC$7:$AC$30&lt;&gt;"",ROW($AC$7:$AC$30)-MIN(ROW($AC$7:$AC$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AE33">
+        <f t="array" ref="AE33">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($AF$7:$AF$30&lt;&gt;"",IF($AC$7:$AC$30&lt;&gt;"",ROW($AC$7:$AC$30)-MIN(ROW($AC$7:$AC$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AI33">
+        <f t="array" ref="AI33">IFERROR(CONCATENATE(TEXT(INDEX($AI$7:$AI$30,SMALL(IF($AL$7:$AL$30&lt;&gt;"",IF($AI$7:$AI$30&lt;&gt;"",ROW($AI$7:$AI$30)-MIN(ROW($AI$7:$AI$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0"),),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AJ33">
+        <f t="array" ref="AJ33">IFERROR(CONCATENATE((INDEX($AL$7:$AL$30,SMALL(IF($AL$7:$AL$30&lt;&gt;"",IF($AI$7:$AI$30&lt;&gt;"",ROW($AI$7:$AI$30)-MIN(ROW($AI$7:$AI$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AK33">
+        <f t="array" ref="AK33">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($AL$7:$AL$30&lt;&gt;"",IF($AI$7:$AI$30&lt;&gt;"",ROW($AI$7:$AI$30)-MIN(ROW($AI$7:$AI$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="11:37">
       <c r="K34">
         <f t="array" ref="K34">IFERROR(CONCATENATE(TEXT(INDEX($K$7:$K$30,SMALL(IF($N$7:$N$30&lt;&gt;"",IF($K$7:$K$30&lt;&gt;"",ROW($K$7:$K$30)-MIN(ROW($K$7:$K$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0"),","),"")</f>
         <v>0</v>
@@ -2498,8 +3018,32 @@
         <f t="array" ref="Y34">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($Z$7:$Z$30&lt;&gt;"",IF($W$7:$W$30&lt;&gt;"",ROW($W$7:$W$30)-MIN(ROW($W$7:$W$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="11:25">
+      <c r="AC34">
+        <f t="array" ref="AC34">IFERROR(CONCATENATE(TEXT(INDEX($AC$7:$AC$30,SMALL(IF($AF$7:$AF$30&lt;&gt;"",IF($AC$7:$AC$30&lt;&gt;"",ROW($AC$7:$AC$30)-MIN(ROW($AC$7:$AC$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0"),),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AD34">
+        <f t="array" ref="AD34">IFERROR(CONCATENATE((INDEX($AF$7:$AF$30,SMALL(IF($AF$7:$AF$30&lt;&gt;"",IF($AC$7:$AC$30&lt;&gt;"",ROW($AC$7:$AC$30)-MIN(ROW($AC$7:$AC$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AE34">
+        <f t="array" ref="AE34">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($AF$7:$AF$30&lt;&gt;"",IF($AC$7:$AC$30&lt;&gt;"",ROW($AC$7:$AC$30)-MIN(ROW($AC$7:$AC$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AI34">
+        <f t="array" ref="AI34">IFERROR(CONCATENATE(TEXT(INDEX($AI$7:$AI$30,SMALL(IF($AL$7:$AL$30&lt;&gt;"",IF($AI$7:$AI$30&lt;&gt;"",ROW($AI$7:$AI$30)-MIN(ROW($AI$7:$AI$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0"),),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AJ34">
+        <f t="array" ref="AJ34">IFERROR(CONCATENATE((INDEX($AL$7:$AL$30,SMALL(IF($AL$7:$AL$30&lt;&gt;"",IF($AI$7:$AI$30&lt;&gt;"",ROW($AI$7:$AI$30)-MIN(ROW($AI$7:$AI$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AK34">
+        <f t="array" ref="AK34">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($AL$7:$AL$30&lt;&gt;"",IF($AI$7:$AI$30&lt;&gt;"",ROW($AI$7:$AI$30)-MIN(ROW($AI$7:$AI$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="11:37">
       <c r="K35">
         <f t="array" ref="K35">IFERROR(CONCATENATE(TEXT(INDEX($K$7:$K$30,SMALL(IF($N$7:$N$30&lt;&gt;"",IF($K$7:$K$30&lt;&gt;"",ROW($K$7:$K$30)-MIN(ROW($K$7:$K$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0"),","),"")</f>
         <v>0</v>
@@ -2536,8 +3080,32 @@
         <f t="array" ref="Y35">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($Z$7:$Z$30&lt;&gt;"",IF($W$7:$W$30&lt;&gt;"",ROW($W$7:$W$30)-MIN(ROW($W$7:$W$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="11:25">
+      <c r="AC35">
+        <f t="array" ref="AC35">IFERROR(CONCATENATE(TEXT(INDEX($AC$7:$AC$30,SMALL(IF($AF$7:$AF$30&lt;&gt;"",IF($AC$7:$AC$30&lt;&gt;"",ROW($AC$7:$AC$30)-MIN(ROW($AC$7:$AC$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0"),),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AD35">
+        <f t="array" ref="AD35">IFERROR(CONCATENATE((INDEX($AF$7:$AF$30,SMALL(IF($AF$7:$AF$30&lt;&gt;"",IF($AC$7:$AC$30&lt;&gt;"",ROW($AC$7:$AC$30)-MIN(ROW($AC$7:$AC$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AE35">
+        <f t="array" ref="AE35">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($AF$7:$AF$30&lt;&gt;"",IF($AC$7:$AC$30&lt;&gt;"",ROW($AC$7:$AC$30)-MIN(ROW($AC$7:$AC$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AI35">
+        <f t="array" ref="AI35">IFERROR(CONCATENATE(TEXT(INDEX($AI$7:$AI$30,SMALL(IF($AL$7:$AL$30&lt;&gt;"",IF($AI$7:$AI$30&lt;&gt;"",ROW($AI$7:$AI$30)-MIN(ROW($AI$7:$AI$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0"),),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AJ35">
+        <f t="array" ref="AJ35">IFERROR(CONCATENATE((INDEX($AL$7:$AL$30,SMALL(IF($AL$7:$AL$30&lt;&gt;"",IF($AI$7:$AI$30&lt;&gt;"",ROW($AI$7:$AI$30)-MIN(ROW($AI$7:$AI$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AK35">
+        <f t="array" ref="AK35">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($AL$7:$AL$30&lt;&gt;"",IF($AI$7:$AI$30&lt;&gt;"",ROW($AI$7:$AI$30)-MIN(ROW($AI$7:$AI$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="11:37">
       <c r="K36">
         <f t="array" ref="K36">IFERROR(CONCATENATE(TEXT(INDEX($K$7:$K$30,SMALL(IF($N$7:$N$30&lt;&gt;"",IF($K$7:$K$30&lt;&gt;"",ROW($K$7:$K$30)-MIN(ROW($K$7:$K$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0"),","),"")</f>
         <v>0</v>
@@ -2574,8 +3142,32 @@
         <f t="array" ref="Y36">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($Z$7:$Z$30&lt;&gt;"",IF($W$7:$W$30&lt;&gt;"",ROW($W$7:$W$30)-MIN(ROW($W$7:$W$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="11:25">
+      <c r="AC36">
+        <f t="array" ref="AC36">IFERROR(CONCATENATE(TEXT(INDEX($AC$7:$AC$30,SMALL(IF($AF$7:$AF$30&lt;&gt;"",IF($AC$7:$AC$30&lt;&gt;"",ROW($AC$7:$AC$30)-MIN(ROW($AC$7:$AC$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0"),),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AD36">
+        <f t="array" ref="AD36">IFERROR(CONCATENATE((INDEX($AF$7:$AF$30,SMALL(IF($AF$7:$AF$30&lt;&gt;"",IF($AC$7:$AC$30&lt;&gt;"",ROW($AC$7:$AC$30)-MIN(ROW($AC$7:$AC$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AE36">
+        <f t="array" ref="AE36">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($AF$7:$AF$30&lt;&gt;"",IF($AC$7:$AC$30&lt;&gt;"",ROW($AC$7:$AC$30)-MIN(ROW($AC$7:$AC$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AI36">
+        <f t="array" ref="AI36">IFERROR(CONCATENATE(TEXT(INDEX($AI$7:$AI$30,SMALL(IF($AL$7:$AL$30&lt;&gt;"",IF($AI$7:$AI$30&lt;&gt;"",ROW($AI$7:$AI$30)-MIN(ROW($AI$7:$AI$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0"),),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AJ36">
+        <f t="array" ref="AJ36">IFERROR(CONCATENATE((INDEX($AL$7:$AL$30,SMALL(IF($AL$7:$AL$30&lt;&gt;"",IF($AI$7:$AI$30&lt;&gt;"",ROW($AI$7:$AI$30)-MIN(ROW($AI$7:$AI$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AK36">
+        <f t="array" ref="AK36">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($AL$7:$AL$30&lt;&gt;"",IF($AI$7:$AI$30&lt;&gt;"",ROW($AI$7:$AI$30)-MIN(ROW($AI$7:$AI$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="11:37">
       <c r="K37">
         <f t="array" ref="K37">IFERROR(CONCATENATE(TEXT(INDEX($K$7:$K$30,SMALL(IF($N$7:$N$30&lt;&gt;"",IF($K$7:$K$30&lt;&gt;"",ROW($K$7:$K$30)-MIN(ROW($K$7:$K$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0"),","),"")</f>
         <v>0</v>
@@ -2612,8 +3204,32 @@
         <f t="array" ref="Y37">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($Z$7:$Z$30&lt;&gt;"",IF($W$7:$W$30&lt;&gt;"",ROW($W$7:$W$30)-MIN(ROW($W$7:$W$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="11:25">
+      <c r="AC37">
+        <f t="array" ref="AC37">IFERROR(CONCATENATE(TEXT(INDEX($AC$7:$AC$30,SMALL(IF($AF$7:$AF$30&lt;&gt;"",IF($AC$7:$AC$30&lt;&gt;"",ROW($AC$7:$AC$30)-MIN(ROW($AC$7:$AC$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0"),),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AD37">
+        <f t="array" ref="AD37">IFERROR(CONCATENATE((INDEX($AF$7:$AF$30,SMALL(IF($AF$7:$AF$30&lt;&gt;"",IF($AC$7:$AC$30&lt;&gt;"",ROW($AC$7:$AC$30)-MIN(ROW($AC$7:$AC$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AE37">
+        <f t="array" ref="AE37">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($AF$7:$AF$30&lt;&gt;"",IF($AC$7:$AC$30&lt;&gt;"",ROW($AC$7:$AC$30)-MIN(ROW($AC$7:$AC$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AI37">
+        <f t="array" ref="AI37">IFERROR(CONCATENATE(TEXT(INDEX($AI$7:$AI$30,SMALL(IF($AL$7:$AL$30&lt;&gt;"",IF($AI$7:$AI$30&lt;&gt;"",ROW($AI$7:$AI$30)-MIN(ROW($AI$7:$AI$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0"),),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AJ37">
+        <f t="array" ref="AJ37">IFERROR(CONCATENATE((INDEX($AL$7:$AL$30,SMALL(IF($AL$7:$AL$30&lt;&gt;"",IF($AI$7:$AI$30&lt;&gt;"",ROW($AI$7:$AI$30)-MIN(ROW($AI$7:$AI$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AK37">
+        <f t="array" ref="AK37">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($AL$7:$AL$30&lt;&gt;"",IF($AI$7:$AI$30&lt;&gt;"",ROW($AI$7:$AI$30)-MIN(ROW($AI$7:$AI$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="11:37">
       <c r="K38">
         <f t="array" ref="K38">IFERROR(CONCATENATE(TEXT(INDEX($K$7:$K$30,SMALL(IF($N$7:$N$30&lt;&gt;"",IF($K$7:$K$30&lt;&gt;"",ROW($K$7:$K$30)-MIN(ROW($K$7:$K$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0"),","),"")</f>
         <v>0</v>
@@ -2650,8 +3266,32 @@
         <f t="array" ref="Y38">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($Z$7:$Z$30&lt;&gt;"",IF($W$7:$W$30&lt;&gt;"",ROW($W$7:$W$30)-MIN(ROW($W$7:$W$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="11:25">
+      <c r="AC38">
+        <f t="array" ref="AC38">IFERROR(CONCATENATE(TEXT(INDEX($AC$7:$AC$30,SMALL(IF($AF$7:$AF$30&lt;&gt;"",IF($AC$7:$AC$30&lt;&gt;"",ROW($AC$7:$AC$30)-MIN(ROW($AC$7:$AC$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0"),),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AD38">
+        <f t="array" ref="AD38">IFERROR(CONCATENATE((INDEX($AF$7:$AF$30,SMALL(IF($AF$7:$AF$30&lt;&gt;"",IF($AC$7:$AC$30&lt;&gt;"",ROW($AC$7:$AC$30)-MIN(ROW($AC$7:$AC$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AE38">
+        <f t="array" ref="AE38">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($AF$7:$AF$30&lt;&gt;"",IF($AC$7:$AC$30&lt;&gt;"",ROW($AC$7:$AC$30)-MIN(ROW($AC$7:$AC$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AI38">
+        <f t="array" ref="AI38">IFERROR(CONCATENATE(TEXT(INDEX($AI$7:$AI$30,SMALL(IF($AL$7:$AL$30&lt;&gt;"",IF($AI$7:$AI$30&lt;&gt;"",ROW($AI$7:$AI$30)-MIN(ROW($AI$7:$AI$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0"),),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AJ38">
+        <f t="array" ref="AJ38">IFERROR(CONCATENATE((INDEX($AL$7:$AL$30,SMALL(IF($AL$7:$AL$30&lt;&gt;"",IF($AI$7:$AI$30&lt;&gt;"",ROW($AI$7:$AI$30)-MIN(ROW($AI$7:$AI$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AK38">
+        <f t="array" ref="AK38">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($AL$7:$AL$30&lt;&gt;"",IF($AI$7:$AI$30&lt;&gt;"",ROW($AI$7:$AI$30)-MIN(ROW($AI$7:$AI$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="11:37">
       <c r="K39">
         <f t="array" ref="K39">IFERROR(CONCATENATE(TEXT(INDEX($K$7:$K$30,SMALL(IF($N$7:$N$30&lt;&gt;"",IF($K$7:$K$30&lt;&gt;"",ROW($K$7:$K$30)-MIN(ROW($K$7:$K$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0"),","),"")</f>
         <v>0</v>
@@ -2688,8 +3328,32 @@
         <f t="array" ref="Y39">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($Z$7:$Z$30&lt;&gt;"",IF($W$7:$W$30&lt;&gt;"",ROW($W$7:$W$30)-MIN(ROW($W$7:$W$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="11:25">
+      <c r="AC39">
+        <f t="array" ref="AC39">IFERROR(CONCATENATE(TEXT(INDEX($AC$7:$AC$30,SMALL(IF($AF$7:$AF$30&lt;&gt;"",IF($AC$7:$AC$30&lt;&gt;"",ROW($AC$7:$AC$30)-MIN(ROW($AC$7:$AC$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0"),),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AD39">
+        <f t="array" ref="AD39">IFERROR(CONCATENATE((INDEX($AF$7:$AF$30,SMALL(IF($AF$7:$AF$30&lt;&gt;"",IF($AC$7:$AC$30&lt;&gt;"",ROW($AC$7:$AC$30)-MIN(ROW($AC$7:$AC$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AE39">
+        <f t="array" ref="AE39">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($AF$7:$AF$30&lt;&gt;"",IF($AC$7:$AC$30&lt;&gt;"",ROW($AC$7:$AC$30)-MIN(ROW($AC$7:$AC$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AI39">
+        <f t="array" ref="AI39">IFERROR(CONCATENATE(TEXT(INDEX($AI$7:$AI$30,SMALL(IF($AL$7:$AL$30&lt;&gt;"",IF($AI$7:$AI$30&lt;&gt;"",ROW($AI$7:$AI$30)-MIN(ROW($AI$7:$AI$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0"),),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AJ39">
+        <f t="array" ref="AJ39">IFERROR(CONCATENATE((INDEX($AL$7:$AL$30,SMALL(IF($AL$7:$AL$30&lt;&gt;"",IF($AI$7:$AI$30&lt;&gt;"",ROW($AI$7:$AI$30)-MIN(ROW($AI$7:$AI$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AK39">
+        <f t="array" ref="AK39">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($AL$7:$AL$30&lt;&gt;"",IF($AI$7:$AI$30&lt;&gt;"",ROW($AI$7:$AI$30)-MIN(ROW($AI$7:$AI$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="11:37">
       <c r="K40">
         <f t="array" ref="K40">IFERROR(CONCATENATE(TEXT(INDEX($K$7:$K$30,SMALL(IF($N$7:$N$30&lt;&gt;"",IF($K$7:$K$30&lt;&gt;"",ROW($K$7:$K$30)-MIN(ROW($K$7:$K$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0"),","),"")</f>
         <v>0</v>
@@ -2726,8 +3390,32 @@
         <f t="array" ref="Y40">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($Z$7:$Z$30&lt;&gt;"",IF($W$7:$W$30&lt;&gt;"",ROW($W$7:$W$30)-MIN(ROW($W$7:$W$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="11:25">
+      <c r="AC40">
+        <f t="array" ref="AC40">IFERROR(CONCATENATE(TEXT(INDEX($AC$7:$AC$30,SMALL(IF($AF$7:$AF$30&lt;&gt;"",IF($AC$7:$AC$30&lt;&gt;"",ROW($AC$7:$AC$30)-MIN(ROW($AC$7:$AC$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0"),),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AD40">
+        <f t="array" ref="AD40">IFERROR(CONCATENATE((INDEX($AF$7:$AF$30,SMALL(IF($AF$7:$AF$30&lt;&gt;"",IF($AC$7:$AC$30&lt;&gt;"",ROW($AC$7:$AC$30)-MIN(ROW($AC$7:$AC$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AE40">
+        <f t="array" ref="AE40">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($AF$7:$AF$30&lt;&gt;"",IF($AC$7:$AC$30&lt;&gt;"",ROW($AC$7:$AC$30)-MIN(ROW($AC$7:$AC$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AI40">
+        <f t="array" ref="AI40">IFERROR(CONCATENATE(TEXT(INDEX($AI$7:$AI$30,SMALL(IF($AL$7:$AL$30&lt;&gt;"",IF($AI$7:$AI$30&lt;&gt;"",ROW($AI$7:$AI$30)-MIN(ROW($AI$7:$AI$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0"),),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AJ40">
+        <f t="array" ref="AJ40">IFERROR(CONCATENATE((INDEX($AL$7:$AL$30,SMALL(IF($AL$7:$AL$30&lt;&gt;"",IF($AI$7:$AI$30&lt;&gt;"",ROW($AI$7:$AI$30)-MIN(ROW($AI$7:$AI$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AK40">
+        <f t="array" ref="AK40">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($AL$7:$AL$30&lt;&gt;"",IF($AI$7:$AI$30&lt;&gt;"",ROW($AI$7:$AI$30)-MIN(ROW($AI$7:$AI$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="11:37">
       <c r="K41">
         <f t="array" ref="K41">IFERROR(CONCATENATE(TEXT(INDEX($K$7:$K$30,SMALL(IF($N$7:$N$30&lt;&gt;"",IF($K$7:$K$30&lt;&gt;"",ROW($K$7:$K$30)-MIN(ROW($K$7:$K$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0"),","),"")</f>
         <v>0</v>
@@ -2764,8 +3452,32 @@
         <f t="array" ref="Y41">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($Z$7:$Z$30&lt;&gt;"",IF($W$7:$W$30&lt;&gt;"",ROW($W$7:$W$30)-MIN(ROW($W$7:$W$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="11:25">
+      <c r="AC41">
+        <f t="array" ref="AC41">IFERROR(CONCATENATE(TEXT(INDEX($AC$7:$AC$30,SMALL(IF($AF$7:$AF$30&lt;&gt;"",IF($AC$7:$AC$30&lt;&gt;"",ROW($AC$7:$AC$30)-MIN(ROW($AC$7:$AC$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0"),),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AD41">
+        <f t="array" ref="AD41">IFERROR(CONCATENATE((INDEX($AF$7:$AF$30,SMALL(IF($AF$7:$AF$30&lt;&gt;"",IF($AC$7:$AC$30&lt;&gt;"",ROW($AC$7:$AC$30)-MIN(ROW($AC$7:$AC$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AE41">
+        <f t="array" ref="AE41">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($AF$7:$AF$30&lt;&gt;"",IF($AC$7:$AC$30&lt;&gt;"",ROW($AC$7:$AC$30)-MIN(ROW($AC$7:$AC$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AI41">
+        <f t="array" ref="AI41">IFERROR(CONCATENATE(TEXT(INDEX($AI$7:$AI$30,SMALL(IF($AL$7:$AL$30&lt;&gt;"",IF($AI$7:$AI$30&lt;&gt;"",ROW($AI$7:$AI$30)-MIN(ROW($AI$7:$AI$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0"),),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AJ41">
+        <f t="array" ref="AJ41">IFERROR(CONCATENATE((INDEX($AL$7:$AL$30,SMALL(IF($AL$7:$AL$30&lt;&gt;"",IF($AI$7:$AI$30&lt;&gt;"",ROW($AI$7:$AI$30)-MIN(ROW($AI$7:$AI$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AK41">
+        <f t="array" ref="AK41">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($AL$7:$AL$30&lt;&gt;"",IF($AI$7:$AI$30&lt;&gt;"",ROW($AI$7:$AI$30)-MIN(ROW($AI$7:$AI$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="11:37">
       <c r="K42">
         <f t="array" ref="K42">IFERROR(CONCATENATE(TEXT(INDEX($K$7:$K$30,SMALL(IF($N$7:$N$30&lt;&gt;"",IF($K$7:$K$30&lt;&gt;"",ROW($K$7:$K$30)-MIN(ROW($K$7:$K$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0"),","),"")</f>
         <v>0</v>
@@ -2802,8 +3514,32 @@
         <f t="array" ref="Y42">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($Z$7:$Z$30&lt;&gt;"",IF($W$7:$W$30&lt;&gt;"",ROW($W$7:$W$30)-MIN(ROW($W$7:$W$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="11:25">
+      <c r="AC42">
+        <f t="array" ref="AC42">IFERROR(CONCATENATE(TEXT(INDEX($AC$7:$AC$30,SMALL(IF($AF$7:$AF$30&lt;&gt;"",IF($AC$7:$AC$30&lt;&gt;"",ROW($AC$7:$AC$30)-MIN(ROW($AC$7:$AC$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0"),),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AD42">
+        <f t="array" ref="AD42">IFERROR(CONCATENATE((INDEX($AF$7:$AF$30,SMALL(IF($AF$7:$AF$30&lt;&gt;"",IF($AC$7:$AC$30&lt;&gt;"",ROW($AC$7:$AC$30)-MIN(ROW($AC$7:$AC$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AE42">
+        <f t="array" ref="AE42">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($AF$7:$AF$30&lt;&gt;"",IF($AC$7:$AC$30&lt;&gt;"",ROW($AC$7:$AC$30)-MIN(ROW($AC$7:$AC$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AI42">
+        <f t="array" ref="AI42">IFERROR(CONCATENATE(TEXT(INDEX($AI$7:$AI$30,SMALL(IF($AL$7:$AL$30&lt;&gt;"",IF($AI$7:$AI$30&lt;&gt;"",ROW($AI$7:$AI$30)-MIN(ROW($AI$7:$AI$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0"),),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AJ42">
+        <f t="array" ref="AJ42">IFERROR(CONCATENATE((INDEX($AL$7:$AL$30,SMALL(IF($AL$7:$AL$30&lt;&gt;"",IF($AI$7:$AI$30&lt;&gt;"",ROW($AI$7:$AI$30)-MIN(ROW($AI$7:$AI$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AK42">
+        <f t="array" ref="AK42">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($AL$7:$AL$30&lt;&gt;"",IF($AI$7:$AI$30&lt;&gt;"",ROW($AI$7:$AI$30)-MIN(ROW($AI$7:$AI$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="11:37">
       <c r="K43">
         <f t="array" ref="K43">IFERROR(CONCATENATE(TEXT(INDEX($K$7:$K$30,SMALL(IF($N$7:$N$30&lt;&gt;"",IF($K$7:$K$30&lt;&gt;"",ROW($K$7:$K$30)-MIN(ROW($K$7:$K$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0"),","),"")</f>
         <v>0</v>
@@ -2840,8 +3576,32 @@
         <f t="array" ref="Y43">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($Z$7:$Z$30&lt;&gt;"",IF($W$7:$W$30&lt;&gt;"",ROW($W$7:$W$30)-MIN(ROW($W$7:$W$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="11:25">
+      <c r="AC43">
+        <f t="array" ref="AC43">IFERROR(CONCATENATE(TEXT(INDEX($AC$7:$AC$30,SMALL(IF($AF$7:$AF$30&lt;&gt;"",IF($AC$7:$AC$30&lt;&gt;"",ROW($AC$7:$AC$30)-MIN(ROW($AC$7:$AC$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0"),),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AD43">
+        <f t="array" ref="AD43">IFERROR(CONCATENATE((INDEX($AF$7:$AF$30,SMALL(IF($AF$7:$AF$30&lt;&gt;"",IF($AC$7:$AC$30&lt;&gt;"",ROW($AC$7:$AC$30)-MIN(ROW($AC$7:$AC$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AE43">
+        <f t="array" ref="AE43">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($AF$7:$AF$30&lt;&gt;"",IF($AC$7:$AC$30&lt;&gt;"",ROW($AC$7:$AC$30)-MIN(ROW($AC$7:$AC$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AI43">
+        <f t="array" ref="AI43">IFERROR(CONCATENATE(TEXT(INDEX($AI$7:$AI$30,SMALL(IF($AL$7:$AL$30&lt;&gt;"",IF($AI$7:$AI$30&lt;&gt;"",ROW($AI$7:$AI$30)-MIN(ROW($AI$7:$AI$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0"),),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AJ43">
+        <f t="array" ref="AJ43">IFERROR(CONCATENATE((INDEX($AL$7:$AL$30,SMALL(IF($AL$7:$AL$30&lt;&gt;"",IF($AI$7:$AI$30&lt;&gt;"",ROW($AI$7:$AI$30)-MIN(ROW($AI$7:$AI$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AK43">
+        <f t="array" ref="AK43">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($AL$7:$AL$30&lt;&gt;"",IF($AI$7:$AI$30&lt;&gt;"",ROW($AI$7:$AI$30)-MIN(ROW($AI$7:$AI$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="11:37">
       <c r="K44">
         <f t="array" ref="K44">IFERROR(CONCATENATE(TEXT(INDEX($K$7:$K$30,SMALL(IF($N$7:$N$30&lt;&gt;"",IF($K$7:$K$30&lt;&gt;"",ROW($K$7:$K$30)-MIN(ROW($K$7:$K$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0"),","),"")</f>
         <v>0</v>
@@ -2878,8 +3638,32 @@
         <f t="array" ref="Y44">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($Z$7:$Z$30&lt;&gt;"",IF($W$7:$W$30&lt;&gt;"",ROW($W$7:$W$30)-MIN(ROW($W$7:$W$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="11:25">
+      <c r="AC44">
+        <f t="array" ref="AC44">IFERROR(CONCATENATE(TEXT(INDEX($AC$7:$AC$30,SMALL(IF($AF$7:$AF$30&lt;&gt;"",IF($AC$7:$AC$30&lt;&gt;"",ROW($AC$7:$AC$30)-MIN(ROW($AC$7:$AC$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0"),),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AD44">
+        <f t="array" ref="AD44">IFERROR(CONCATENATE((INDEX($AF$7:$AF$30,SMALL(IF($AF$7:$AF$30&lt;&gt;"",IF($AC$7:$AC$30&lt;&gt;"",ROW($AC$7:$AC$30)-MIN(ROW($AC$7:$AC$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AE44">
+        <f t="array" ref="AE44">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($AF$7:$AF$30&lt;&gt;"",IF($AC$7:$AC$30&lt;&gt;"",ROW($AC$7:$AC$30)-MIN(ROW($AC$7:$AC$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AI44">
+        <f t="array" ref="AI44">IFERROR(CONCATENATE(TEXT(INDEX($AI$7:$AI$30,SMALL(IF($AL$7:$AL$30&lt;&gt;"",IF($AI$7:$AI$30&lt;&gt;"",ROW($AI$7:$AI$30)-MIN(ROW($AI$7:$AI$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0"),),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AJ44">
+        <f t="array" ref="AJ44">IFERROR(CONCATENATE((INDEX($AL$7:$AL$30,SMALL(IF($AL$7:$AL$30&lt;&gt;"",IF($AI$7:$AI$30&lt;&gt;"",ROW($AI$7:$AI$30)-MIN(ROW($AI$7:$AI$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AK44">
+        <f t="array" ref="AK44">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($AL$7:$AL$30&lt;&gt;"",IF($AI$7:$AI$30&lt;&gt;"",ROW($AI$7:$AI$30)-MIN(ROW($AI$7:$AI$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="11:37">
       <c r="K45">
         <f t="array" ref="K45">IFERROR(CONCATENATE(TEXT(INDEX($K$7:$K$30,SMALL(IF($N$7:$N$30&lt;&gt;"",IF($K$7:$K$30&lt;&gt;"",ROW($K$7:$K$30)-MIN(ROW($K$7:$K$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0"),","),"")</f>
         <v>0</v>
@@ -2916,8 +3700,32 @@
         <f t="array" ref="Y45">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($Z$7:$Z$30&lt;&gt;"",IF($W$7:$W$30&lt;&gt;"",ROW($W$7:$W$30)-MIN(ROW($W$7:$W$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="11:25">
+      <c r="AC45">
+        <f t="array" ref="AC45">IFERROR(CONCATENATE(TEXT(INDEX($AC$7:$AC$30,SMALL(IF($AF$7:$AF$30&lt;&gt;"",IF($AC$7:$AC$30&lt;&gt;"",ROW($AC$7:$AC$30)-MIN(ROW($AC$7:$AC$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0"),),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AD45">
+        <f t="array" ref="AD45">IFERROR(CONCATENATE((INDEX($AF$7:$AF$30,SMALL(IF($AF$7:$AF$30&lt;&gt;"",IF($AC$7:$AC$30&lt;&gt;"",ROW($AC$7:$AC$30)-MIN(ROW($AC$7:$AC$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AE45">
+        <f t="array" ref="AE45">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($AF$7:$AF$30&lt;&gt;"",IF($AC$7:$AC$30&lt;&gt;"",ROW($AC$7:$AC$30)-MIN(ROW($AC$7:$AC$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AI45">
+        <f t="array" ref="AI45">IFERROR(CONCATENATE(TEXT(INDEX($AI$7:$AI$30,SMALL(IF($AL$7:$AL$30&lt;&gt;"",IF($AI$7:$AI$30&lt;&gt;"",ROW($AI$7:$AI$30)-MIN(ROW($AI$7:$AI$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0"),),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AJ45">
+        <f t="array" ref="AJ45">IFERROR(CONCATENATE((INDEX($AL$7:$AL$30,SMALL(IF($AL$7:$AL$30&lt;&gt;"",IF($AI$7:$AI$30&lt;&gt;"",ROW($AI$7:$AI$30)-MIN(ROW($AI$7:$AI$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AK45">
+        <f t="array" ref="AK45">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($AL$7:$AL$30&lt;&gt;"",IF($AI$7:$AI$30&lt;&gt;"",ROW($AI$7:$AI$30)-MIN(ROW($AI$7:$AI$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="11:37">
       <c r="K46">
         <f t="array" ref="K46">IFERROR(CONCATENATE(TEXT(INDEX($K$7:$K$30,SMALL(IF($N$7:$N$30&lt;&gt;"",IF($K$7:$K$30&lt;&gt;"",ROW($K$7:$K$30)-MIN(ROW($K$7:$K$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0"),","),"")</f>
         <v>0</v>
@@ -2954,8 +3762,32 @@
         <f t="array" ref="Y46">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($Z$7:$Z$30&lt;&gt;"",IF($W$7:$W$30&lt;&gt;"",ROW($W$7:$W$30)-MIN(ROW($W$7:$W$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="11:25">
+      <c r="AC46">
+        <f t="array" ref="AC46">IFERROR(CONCATENATE(TEXT(INDEX($AC$7:$AC$30,SMALL(IF($AF$7:$AF$30&lt;&gt;"",IF($AC$7:$AC$30&lt;&gt;"",ROW($AC$7:$AC$30)-MIN(ROW($AC$7:$AC$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0"),),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AD46">
+        <f t="array" ref="AD46">IFERROR(CONCATENATE((INDEX($AF$7:$AF$30,SMALL(IF($AF$7:$AF$30&lt;&gt;"",IF($AC$7:$AC$30&lt;&gt;"",ROW($AC$7:$AC$30)-MIN(ROW($AC$7:$AC$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AE46">
+        <f t="array" ref="AE46">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($AF$7:$AF$30&lt;&gt;"",IF($AC$7:$AC$30&lt;&gt;"",ROW($AC$7:$AC$30)-MIN(ROW($AC$7:$AC$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AI46">
+        <f t="array" ref="AI46">IFERROR(CONCATENATE(TEXT(INDEX($AI$7:$AI$30,SMALL(IF($AL$7:$AL$30&lt;&gt;"",IF($AI$7:$AI$30&lt;&gt;"",ROW($AI$7:$AI$30)-MIN(ROW($AI$7:$AI$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0"),),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AJ46">
+        <f t="array" ref="AJ46">IFERROR(CONCATENATE((INDEX($AL$7:$AL$30,SMALL(IF($AL$7:$AL$30&lt;&gt;"",IF($AI$7:$AI$30&lt;&gt;"",ROW($AI$7:$AI$30)-MIN(ROW($AI$7:$AI$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AK46">
+        <f t="array" ref="AK46">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($AL$7:$AL$30&lt;&gt;"",IF($AI$7:$AI$30&lt;&gt;"",ROW($AI$7:$AI$30)-MIN(ROW($AI$7:$AI$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="11:37">
       <c r="K47">
         <f t="array" ref="K47">IFERROR(CONCATENATE(TEXT(INDEX($K$7:$K$30,SMALL(IF($N$7:$N$30&lt;&gt;"",IF($K$7:$K$30&lt;&gt;"",ROW($K$7:$K$30)-MIN(ROW($K$7:$K$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0"),","),"")</f>
         <v>0</v>
@@ -2992,8 +3824,32 @@
         <f t="array" ref="Y47">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($Z$7:$Z$30&lt;&gt;"",IF($W$7:$W$30&lt;&gt;"",ROW($W$7:$W$30)-MIN(ROW($W$7:$W$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="11:25">
+      <c r="AC47">
+        <f t="array" ref="AC47">IFERROR(CONCATENATE(TEXT(INDEX($AC$7:$AC$30,SMALL(IF($AF$7:$AF$30&lt;&gt;"",IF($AC$7:$AC$30&lt;&gt;"",ROW($AC$7:$AC$30)-MIN(ROW($AC$7:$AC$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0"),),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AD47">
+        <f t="array" ref="AD47">IFERROR(CONCATENATE((INDEX($AF$7:$AF$30,SMALL(IF($AF$7:$AF$30&lt;&gt;"",IF($AC$7:$AC$30&lt;&gt;"",ROW($AC$7:$AC$30)-MIN(ROW($AC$7:$AC$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AE47">
+        <f t="array" ref="AE47">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($AF$7:$AF$30&lt;&gt;"",IF($AC$7:$AC$30&lt;&gt;"",ROW($AC$7:$AC$30)-MIN(ROW($AC$7:$AC$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AI47">
+        <f t="array" ref="AI47">IFERROR(CONCATENATE(TEXT(INDEX($AI$7:$AI$30,SMALL(IF($AL$7:$AL$30&lt;&gt;"",IF($AI$7:$AI$30&lt;&gt;"",ROW($AI$7:$AI$30)-MIN(ROW($AI$7:$AI$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0"),),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AJ47">
+        <f t="array" ref="AJ47">IFERROR(CONCATENATE((INDEX($AL$7:$AL$30,SMALL(IF($AL$7:$AL$30&lt;&gt;"",IF($AI$7:$AI$30&lt;&gt;"",ROW($AI$7:$AI$30)-MIN(ROW($AI$7:$AI$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AK47">
+        <f t="array" ref="AK47">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($AL$7:$AL$30&lt;&gt;"",IF($AI$7:$AI$30&lt;&gt;"",ROW($AI$7:$AI$30)-MIN(ROW($AI$7:$AI$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="11:37">
       <c r="K48">
         <f t="array" ref="K48">IFERROR(CONCATENATE(TEXT(INDEX($K$7:$K$30,SMALL(IF($N$7:$N$30&lt;&gt;"",IF($K$7:$K$30&lt;&gt;"",ROW($K$7:$K$30)-MIN(ROW($K$7:$K$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0"),","),"")</f>
         <v>0</v>
@@ -3030,8 +3886,32 @@
         <f t="array" ref="Y48">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($Z$7:$Z$30&lt;&gt;"",IF($W$7:$W$30&lt;&gt;"",ROW($W$7:$W$30)-MIN(ROW($W$7:$W$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="11:25">
+      <c r="AC48">
+        <f t="array" ref="AC48">IFERROR(CONCATENATE(TEXT(INDEX($AC$7:$AC$30,SMALL(IF($AF$7:$AF$30&lt;&gt;"",IF($AC$7:$AC$30&lt;&gt;"",ROW($AC$7:$AC$30)-MIN(ROW($AC$7:$AC$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0"),),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AD48">
+        <f t="array" ref="AD48">IFERROR(CONCATENATE((INDEX($AF$7:$AF$30,SMALL(IF($AF$7:$AF$30&lt;&gt;"",IF($AC$7:$AC$30&lt;&gt;"",ROW($AC$7:$AC$30)-MIN(ROW($AC$7:$AC$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AE48">
+        <f t="array" ref="AE48">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($AF$7:$AF$30&lt;&gt;"",IF($AC$7:$AC$30&lt;&gt;"",ROW($AC$7:$AC$30)-MIN(ROW($AC$7:$AC$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AI48">
+        <f t="array" ref="AI48">IFERROR(CONCATENATE(TEXT(INDEX($AI$7:$AI$30,SMALL(IF($AL$7:$AL$30&lt;&gt;"",IF($AI$7:$AI$30&lt;&gt;"",ROW($AI$7:$AI$30)-MIN(ROW($AI$7:$AI$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0"),),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AJ48">
+        <f t="array" ref="AJ48">IFERROR(CONCATENATE((INDEX($AL$7:$AL$30,SMALL(IF($AL$7:$AL$30&lt;&gt;"",IF($AI$7:$AI$30&lt;&gt;"",ROW($AI$7:$AI$30)-MIN(ROW($AI$7:$AI$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AK48">
+        <f t="array" ref="AK48">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($AL$7:$AL$30&lt;&gt;"",IF($AI$7:$AI$30&lt;&gt;"",ROW($AI$7:$AI$30)-MIN(ROW($AI$7:$AI$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="11:37">
       <c r="K49">
         <f t="array" ref="K49">IFERROR(CONCATENATE(TEXT(INDEX($K$7:$K$30,SMALL(IF($N$7:$N$30&lt;&gt;"",IF($K$7:$K$30&lt;&gt;"",ROW($K$7:$K$30)-MIN(ROW($K$7:$K$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0"),","),"")</f>
         <v>0</v>
@@ -3068,8 +3948,32 @@
         <f t="array" ref="Y49">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($Z$7:$Z$30&lt;&gt;"",IF($W$7:$W$30&lt;&gt;"",ROW($W$7:$W$30)-MIN(ROW($W$7:$W$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="11:25">
+      <c r="AC49">
+        <f t="array" ref="AC49">IFERROR(CONCATENATE(TEXT(INDEX($AC$7:$AC$30,SMALL(IF($AF$7:$AF$30&lt;&gt;"",IF($AC$7:$AC$30&lt;&gt;"",ROW($AC$7:$AC$30)-MIN(ROW($AC$7:$AC$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0"),),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AD49">
+        <f t="array" ref="AD49">IFERROR(CONCATENATE((INDEX($AF$7:$AF$30,SMALL(IF($AF$7:$AF$30&lt;&gt;"",IF($AC$7:$AC$30&lt;&gt;"",ROW($AC$7:$AC$30)-MIN(ROW($AC$7:$AC$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AE49">
+        <f t="array" ref="AE49">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($AF$7:$AF$30&lt;&gt;"",IF($AC$7:$AC$30&lt;&gt;"",ROW($AC$7:$AC$30)-MIN(ROW($AC$7:$AC$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AI49">
+        <f t="array" ref="AI49">IFERROR(CONCATENATE(TEXT(INDEX($AI$7:$AI$30,SMALL(IF($AL$7:$AL$30&lt;&gt;"",IF($AI$7:$AI$30&lt;&gt;"",ROW($AI$7:$AI$30)-MIN(ROW($AI$7:$AI$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0"),),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AJ49">
+        <f t="array" ref="AJ49">IFERROR(CONCATENATE((INDEX($AL$7:$AL$30,SMALL(IF($AL$7:$AL$30&lt;&gt;"",IF($AI$7:$AI$30&lt;&gt;"",ROW($AI$7:$AI$30)-MIN(ROW($AI$7:$AI$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AK49">
+        <f t="array" ref="AK49">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($AL$7:$AL$30&lt;&gt;"",IF($AI$7:$AI$30&lt;&gt;"",ROW($AI$7:$AI$30)-MIN(ROW($AI$7:$AI$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="11:37">
       <c r="K50">
         <f t="array" ref="K50">IFERROR(CONCATENATE(TEXT(INDEX($K$7:$K$30,SMALL(IF($N$7:$N$30&lt;&gt;"",IF($K$7:$K$30&lt;&gt;"",ROW($K$7:$K$30)-MIN(ROW($K$7:$K$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0"),","),"")</f>
         <v>0</v>
@@ -3106,8 +4010,32 @@
         <f t="array" ref="Y50">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($Z$7:$Z$30&lt;&gt;"",IF($W$7:$W$30&lt;&gt;"",ROW($W$7:$W$30)-MIN(ROW($W$7:$W$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="11:25">
+      <c r="AC50">
+        <f t="array" ref="AC50">IFERROR(CONCATENATE(TEXT(INDEX($AC$7:$AC$30,SMALL(IF($AF$7:$AF$30&lt;&gt;"",IF($AC$7:$AC$30&lt;&gt;"",ROW($AC$7:$AC$30)-MIN(ROW($AC$7:$AC$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0"),),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AD50">
+        <f t="array" ref="AD50">IFERROR(CONCATENATE((INDEX($AF$7:$AF$30,SMALL(IF($AF$7:$AF$30&lt;&gt;"",IF($AC$7:$AC$30&lt;&gt;"",ROW($AC$7:$AC$30)-MIN(ROW($AC$7:$AC$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AE50">
+        <f t="array" ref="AE50">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($AF$7:$AF$30&lt;&gt;"",IF($AC$7:$AC$30&lt;&gt;"",ROW($AC$7:$AC$30)-MIN(ROW($AC$7:$AC$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AI50">
+        <f t="array" ref="AI50">IFERROR(CONCATENATE(TEXT(INDEX($AI$7:$AI$30,SMALL(IF($AL$7:$AL$30&lt;&gt;"",IF($AI$7:$AI$30&lt;&gt;"",ROW($AI$7:$AI$30)-MIN(ROW($AI$7:$AI$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0"),),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AJ50">
+        <f t="array" ref="AJ50">IFERROR(CONCATENATE((INDEX($AL$7:$AL$30,SMALL(IF($AL$7:$AL$30&lt;&gt;"",IF($AI$7:$AI$30&lt;&gt;"",ROW($AI$7:$AI$30)-MIN(ROW($AI$7:$AI$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AK50">
+        <f t="array" ref="AK50">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($AL$7:$AL$30&lt;&gt;"",IF($AI$7:$AI$30&lt;&gt;"",ROW($AI$7:$AI$30)-MIN(ROW($AI$7:$AI$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="11:37">
       <c r="K51">
         <f t="array" ref="K51">IFERROR(CONCATENATE(TEXT(INDEX($K$7:$K$30,SMALL(IF($N$7:$N$30&lt;&gt;"",IF($K$7:$K$30&lt;&gt;"",ROW($K$7:$K$30)-MIN(ROW($K$7:$K$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0"),","),"")</f>
         <v>0</v>
@@ -3144,8 +4072,32 @@
         <f t="array" ref="Y51">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($Z$7:$Z$30&lt;&gt;"",IF($W$7:$W$30&lt;&gt;"",ROW($W$7:$W$30)-MIN(ROW($W$7:$W$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="11:25">
+      <c r="AC51">
+        <f t="array" ref="AC51">IFERROR(CONCATENATE(TEXT(INDEX($AC$7:$AC$30,SMALL(IF($AF$7:$AF$30&lt;&gt;"",IF($AC$7:$AC$30&lt;&gt;"",ROW($AC$7:$AC$30)-MIN(ROW($AC$7:$AC$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0"),),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AD51">
+        <f t="array" ref="AD51">IFERROR(CONCATENATE((INDEX($AF$7:$AF$30,SMALL(IF($AF$7:$AF$30&lt;&gt;"",IF($AC$7:$AC$30&lt;&gt;"",ROW($AC$7:$AC$30)-MIN(ROW($AC$7:$AC$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AE51">
+        <f t="array" ref="AE51">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($AF$7:$AF$30&lt;&gt;"",IF($AC$7:$AC$30&lt;&gt;"",ROW($AC$7:$AC$30)-MIN(ROW($AC$7:$AC$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AI51">
+        <f t="array" ref="AI51">IFERROR(CONCATENATE(TEXT(INDEX($AI$7:$AI$30,SMALL(IF($AL$7:$AL$30&lt;&gt;"",IF($AI$7:$AI$30&lt;&gt;"",ROW($AI$7:$AI$30)-MIN(ROW($AI$7:$AI$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0"),),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AJ51">
+        <f t="array" ref="AJ51">IFERROR(CONCATENATE((INDEX($AL$7:$AL$30,SMALL(IF($AL$7:$AL$30&lt;&gt;"",IF($AI$7:$AI$30&lt;&gt;"",ROW($AI$7:$AI$30)-MIN(ROW($AI$7:$AI$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AK51">
+        <f t="array" ref="AK51">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($AL$7:$AL$30&lt;&gt;"",IF($AI$7:$AI$30&lt;&gt;"",ROW($AI$7:$AI$30)-MIN(ROW($AI$7:$AI$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="11:37">
       <c r="K52">
         <f t="array" ref="K52">IFERROR(CONCATENATE(TEXT(INDEX($K$7:$K$30,SMALL(IF($N$7:$N$30&lt;&gt;"",IF($K$7:$K$30&lt;&gt;"",ROW($K$7:$K$30)-MIN(ROW($K$7:$K$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0"),","),"")</f>
         <v>0</v>
@@ -3182,8 +4134,32 @@
         <f t="array" ref="Y52">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($Z$7:$Z$30&lt;&gt;"",IF($W$7:$W$30&lt;&gt;"",ROW($W$7:$W$30)-MIN(ROW($W$7:$W$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="11:25">
+      <c r="AC52">
+        <f t="array" ref="AC52">IFERROR(CONCATENATE(TEXT(INDEX($AC$7:$AC$30,SMALL(IF($AF$7:$AF$30&lt;&gt;"",IF($AC$7:$AC$30&lt;&gt;"",ROW($AC$7:$AC$30)-MIN(ROW($AC$7:$AC$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0"),),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AD52">
+        <f t="array" ref="AD52">IFERROR(CONCATENATE((INDEX($AF$7:$AF$30,SMALL(IF($AF$7:$AF$30&lt;&gt;"",IF($AC$7:$AC$30&lt;&gt;"",ROW($AC$7:$AC$30)-MIN(ROW($AC$7:$AC$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AE52">
+        <f t="array" ref="AE52">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($AF$7:$AF$30&lt;&gt;"",IF($AC$7:$AC$30&lt;&gt;"",ROW($AC$7:$AC$30)-MIN(ROW($AC$7:$AC$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AI52">
+        <f t="array" ref="AI52">IFERROR(CONCATENATE(TEXT(INDEX($AI$7:$AI$30,SMALL(IF($AL$7:$AL$30&lt;&gt;"",IF($AI$7:$AI$30&lt;&gt;"",ROW($AI$7:$AI$30)-MIN(ROW($AI$7:$AI$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0"),),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AJ52">
+        <f t="array" ref="AJ52">IFERROR(CONCATENATE((INDEX($AL$7:$AL$30,SMALL(IF($AL$7:$AL$30&lt;&gt;"",IF($AI$7:$AI$30&lt;&gt;"",ROW($AI$7:$AI$30)-MIN(ROW($AI$7:$AI$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AK52">
+        <f t="array" ref="AK52">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($AL$7:$AL$30&lt;&gt;"",IF($AI$7:$AI$30&lt;&gt;"",ROW($AI$7:$AI$30)-MIN(ROW($AI$7:$AI$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="11:37">
       <c r="K53">
         <f t="array" ref="K53">IFERROR(CONCATENATE(TEXT(INDEX($K$7:$K$30,SMALL(IF($N$7:$N$30&lt;&gt;"",IF($K$7:$K$30&lt;&gt;"",ROW($K$7:$K$30)-MIN(ROW($K$7:$K$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0"),","),"")</f>
         <v>0</v>
@@ -3220,8 +4196,32 @@
         <f t="array" ref="Y53">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($Z$7:$Z$30&lt;&gt;"",IF($W$7:$W$30&lt;&gt;"",ROW($W$7:$W$30)-MIN(ROW($W$7:$W$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="11:25">
+      <c r="AC53">
+        <f t="array" ref="AC53">IFERROR(CONCATENATE(TEXT(INDEX($AC$7:$AC$30,SMALL(IF($AF$7:$AF$30&lt;&gt;"",IF($AC$7:$AC$30&lt;&gt;"",ROW($AC$7:$AC$30)-MIN(ROW($AC$7:$AC$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0"),),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AD53">
+        <f t="array" ref="AD53">IFERROR(CONCATENATE((INDEX($AF$7:$AF$30,SMALL(IF($AF$7:$AF$30&lt;&gt;"",IF($AC$7:$AC$30&lt;&gt;"",ROW($AC$7:$AC$30)-MIN(ROW($AC$7:$AC$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AE53">
+        <f t="array" ref="AE53">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($AF$7:$AF$30&lt;&gt;"",IF($AC$7:$AC$30&lt;&gt;"",ROW($AC$7:$AC$30)-MIN(ROW($AC$7:$AC$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AI53">
+        <f t="array" ref="AI53">IFERROR(CONCATENATE(TEXT(INDEX($AI$7:$AI$30,SMALL(IF($AL$7:$AL$30&lt;&gt;"",IF($AI$7:$AI$30&lt;&gt;"",ROW($AI$7:$AI$30)-MIN(ROW($AI$7:$AI$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0"),),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AJ53">
+        <f t="array" ref="AJ53">IFERROR(CONCATENATE((INDEX($AL$7:$AL$30,SMALL(IF($AL$7:$AL$30&lt;&gt;"",IF($AI$7:$AI$30&lt;&gt;"",ROW($AI$7:$AI$30)-MIN(ROW($AI$7:$AI$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AK53">
+        <f t="array" ref="AK53">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($AL$7:$AL$30&lt;&gt;"",IF($AI$7:$AI$30&lt;&gt;"",ROW($AI$7:$AI$30)-MIN(ROW($AI$7:$AI$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="11:37">
       <c r="K54">
         <f t="array" ref="K54">IFERROR(CONCATENATE(TEXT(INDEX($K$7:$K$30,SMALL(IF($N$7:$N$30&lt;&gt;"",IF($K$7:$K$30&lt;&gt;"",ROW($K$7:$K$30)-MIN(ROW($K$7:$K$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0"),","),"")</f>
         <v>0</v>
@@ -3258,8 +4258,32 @@
         <f t="array" ref="Y54">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($Z$7:$Z$30&lt;&gt;"",IF($W$7:$W$30&lt;&gt;"",ROW($W$7:$W$30)-MIN(ROW($W$7:$W$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="11:25">
+      <c r="AC54">
+        <f t="array" ref="AC54">IFERROR(CONCATENATE(TEXT(INDEX($AC$7:$AC$30,SMALL(IF($AF$7:$AF$30&lt;&gt;"",IF($AC$7:$AC$30&lt;&gt;"",ROW($AC$7:$AC$30)-MIN(ROW($AC$7:$AC$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0"),),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AD54">
+        <f t="array" ref="AD54">IFERROR(CONCATENATE((INDEX($AF$7:$AF$30,SMALL(IF($AF$7:$AF$30&lt;&gt;"",IF($AC$7:$AC$30&lt;&gt;"",ROW($AC$7:$AC$30)-MIN(ROW($AC$7:$AC$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AE54">
+        <f t="array" ref="AE54">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($AF$7:$AF$30&lt;&gt;"",IF($AC$7:$AC$30&lt;&gt;"",ROW($AC$7:$AC$30)-MIN(ROW($AC$7:$AC$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AI54">
+        <f t="array" ref="AI54">IFERROR(CONCATENATE(TEXT(INDEX($AI$7:$AI$30,SMALL(IF($AL$7:$AL$30&lt;&gt;"",IF($AI$7:$AI$30&lt;&gt;"",ROW($AI$7:$AI$30)-MIN(ROW($AI$7:$AI$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0"),),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AJ54">
+        <f t="array" ref="AJ54">IFERROR(CONCATENATE((INDEX($AL$7:$AL$30,SMALL(IF($AL$7:$AL$30&lt;&gt;"",IF($AI$7:$AI$30&lt;&gt;"",ROW($AI$7:$AI$30)-MIN(ROW($AI$7:$AI$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AK54">
+        <f t="array" ref="AK54">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($AL$7:$AL$30&lt;&gt;"",IF($AI$7:$AI$30&lt;&gt;"",ROW($AI$7:$AI$30)-MIN(ROW($AI$7:$AI$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="11:37">
       <c r="K55">
         <f t="array" ref="K55">IFERROR(CONCATENATE(TEXT(INDEX($K$7:$K$30,SMALL(IF($N$7:$N$30&lt;&gt;"",IF($K$7:$K$30&lt;&gt;"",ROW($K$7:$K$30)-MIN(ROW($K$7:$K$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0"),","),"")</f>
         <v>0</v>
@@ -3296,27 +4320,163 @@
         <f t="array" ref="Y55">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($Z$7:$Z$30&lt;&gt;"",IF($W$7:$W$30&lt;&gt;"",ROW($W$7:$W$30)-MIN(ROW($W$7:$W$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
         <v>0</v>
       </c>
+      <c r="AC55">
+        <f t="array" ref="AC55">IFERROR(CONCATENATE(TEXT(INDEX($AC$7:$AC$30,SMALL(IF($AF$7:$AF$30&lt;&gt;"",IF($AC$7:$AC$30&lt;&gt;"",ROW($AC$7:$AC$30)-MIN(ROW($AC$7:$AC$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0"),),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AD55">
+        <f t="array" ref="AD55">IFERROR(CONCATENATE((INDEX($AF$7:$AF$30,SMALL(IF($AF$7:$AF$30&lt;&gt;"",IF($AC$7:$AC$30&lt;&gt;"",ROW($AC$7:$AC$30)-MIN(ROW($AC$7:$AC$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AE55">
+        <f t="array" ref="AE55">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($AF$7:$AF$30&lt;&gt;"",IF($AC$7:$AC$30&lt;&gt;"",ROW($AC$7:$AC$30)-MIN(ROW($AC$7:$AC$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AI55">
+        <f t="array" ref="AI55">IFERROR(CONCATENATE(TEXT(INDEX($AI$7:$AI$30,SMALL(IF($AL$7:$AL$30&lt;&gt;"",IF($AI$7:$AI$30&lt;&gt;"",ROW($AI$7:$AI$30)-MIN(ROW($AI$7:$AI$30))+1,""),""),ROW()-ROW(A$32)+1)),"##0"),),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AJ55">
+        <f t="array" ref="AJ55">IFERROR(CONCATENATE((INDEX($AL$7:$AL$30,SMALL(IF($AL$7:$AL$30&lt;&gt;"",IF($AI$7:$AI$30&lt;&gt;"",ROW($AI$7:$AI$30)-MIN(ROW($AI$7:$AI$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
+        <v>0</v>
+      </c>
+      <c r="AK55">
+        <f t="array" ref="AK55">IFERROR(CONCATENATE((INDEX($A$7:$A$30,SMALL(IF($AL$7:$AL$30&lt;&gt;"",IF($AI$7:$AI$30&lt;&gt;"",ROW($AI$7:$AI$30)-MIN(ROW($AI$7:$AI$30))+1,""),""),ROW()-ROW(A$32)+1))),),"")</f>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="6">
     <mergeCell ref="A5:I5"/>
     <mergeCell ref="J5:O5"/>
     <mergeCell ref="P5:U5"/>
     <mergeCell ref="V5:AA5"/>
+    <mergeCell ref="AB5:AG5"/>
+    <mergeCell ref="AH5:AM5"/>
   </mergeCells>
-  <conditionalFormatting sqref="L10">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThanOrEqual">
+  <conditionalFormatting sqref="AD10">
+    <cfRule type="cellIs" dxfId="0" priority="53" operator="lessThanOrEqual">
       <formula>H10</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="AD15">
+    <cfRule type="cellIs" dxfId="0" priority="55" operator="lessThanOrEqual">
+      <formula>H15</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD17">
+    <cfRule type="cellIs" dxfId="0" priority="57" operator="lessThanOrEqual">
+      <formula>H17</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD20">
+    <cfRule type="cellIs" dxfId="0" priority="59" operator="lessThanOrEqual">
+      <formula>H20</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD21">
+    <cfRule type="cellIs" dxfId="0" priority="61" operator="lessThanOrEqual">
+      <formula>H21</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD25">
+    <cfRule type="cellIs" dxfId="0" priority="63" operator="lessThanOrEqual">
+      <formula>H25</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD26">
+    <cfRule type="cellIs" dxfId="0" priority="65" operator="lessThanOrEqual">
+      <formula>H26</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD28">
+    <cfRule type="cellIs" dxfId="0" priority="67" operator="lessThanOrEqual">
+      <formula>H28</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD29">
+    <cfRule type="cellIs" dxfId="0" priority="69" operator="lessThanOrEqual">
+      <formula>H29</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD30">
+    <cfRule type="cellIs" dxfId="0" priority="71" operator="lessThanOrEqual">
+      <formula>H30</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD8">
+    <cfRule type="cellIs" dxfId="0" priority="51" operator="lessThanOrEqual">
+      <formula>H8</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE10">
+    <cfRule type="cellIs" dxfId="0" priority="54" operator="lessThanOrEqual">
+      <formula>I10</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE15">
+    <cfRule type="cellIs" dxfId="0" priority="56" operator="lessThanOrEqual">
+      <formula>I15</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE17">
+    <cfRule type="cellIs" dxfId="0" priority="58" operator="lessThanOrEqual">
+      <formula>I17</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE20">
+    <cfRule type="cellIs" dxfId="0" priority="60" operator="lessThanOrEqual">
+      <formula>I20</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE21">
+    <cfRule type="cellIs" dxfId="0" priority="62" operator="lessThanOrEqual">
+      <formula>I21</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE25">
+    <cfRule type="cellIs" dxfId="0" priority="64" operator="lessThanOrEqual">
+      <formula>I25</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE26">
+    <cfRule type="cellIs" dxfId="0" priority="66" operator="lessThanOrEqual">
+      <formula>I26</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE28">
+    <cfRule type="cellIs" dxfId="0" priority="68" operator="lessThanOrEqual">
+      <formula>I28</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE29">
+    <cfRule type="cellIs" dxfId="0" priority="70" operator="lessThanOrEqual">
+      <formula>I29</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE30">
+    <cfRule type="cellIs" dxfId="0" priority="72" operator="lessThanOrEqual">
+      <formula>I30</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE8">
+    <cfRule type="cellIs" dxfId="0" priority="52" operator="lessThanOrEqual">
+      <formula>I8</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AJ30">
+    <cfRule type="cellIs" dxfId="0" priority="73" operator="lessThanOrEqual">
+      <formula>H30</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AK30">
+    <cfRule type="cellIs" dxfId="0" priority="74" operator="lessThanOrEqual">
+      <formula>I30</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="L11">
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="0" priority="5" operator="lessThanOrEqual">
       <formula>H11</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L12">
-    <cfRule type="cellIs" dxfId="0" priority="5" operator="lessThanOrEqual">
-      <formula>H12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L13">
@@ -3324,34 +4484,39 @@
       <formula>H13</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L19">
+  <conditionalFormatting sqref="L14">
     <cfRule type="cellIs" dxfId="0" priority="9" operator="lessThanOrEqual">
-      <formula>H19</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L21">
+      <formula>H14</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L20">
     <cfRule type="cellIs" dxfId="0" priority="11" operator="lessThanOrEqual">
-      <formula>H21</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L29">
+      <formula>H20</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L22">
     <cfRule type="cellIs" dxfId="0" priority="13" operator="lessThanOrEqual">
-      <formula>H29</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M10">
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="lessThanOrEqual">
-      <formula>I10</formula>
+      <formula>H22</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L23">
+    <cfRule type="cellIs" dxfId="0" priority="15" operator="lessThanOrEqual">
+      <formula>H23</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L7">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThanOrEqual">
+      <formula>H7</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L9">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="lessThanOrEqual">
+      <formula>H9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M11">
-    <cfRule type="cellIs" dxfId="0" priority="4" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="0" priority="6" operator="lessThanOrEqual">
       <formula>I11</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M12">
-    <cfRule type="cellIs" dxfId="0" priority="6" operator="lessThanOrEqual">
-      <formula>I12</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M13">
@@ -3359,196 +4524,234 @@
       <formula>I13</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M19">
+  <conditionalFormatting sqref="M14">
     <cfRule type="cellIs" dxfId="0" priority="10" operator="lessThanOrEqual">
-      <formula>I19</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M21">
+      <formula>I14</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M20">
     <cfRule type="cellIs" dxfId="0" priority="12" operator="lessThanOrEqual">
-      <formula>I21</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M29">
+      <formula>I20</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M22">
     <cfRule type="cellIs" dxfId="0" priority="14" operator="lessThanOrEqual">
+      <formula>I22</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M23">
+    <cfRule type="cellIs" dxfId="0" priority="16" operator="lessThanOrEqual">
+      <formula>I23</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M7">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="lessThanOrEqual">
+      <formula>I7</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M9">
+    <cfRule type="cellIs" dxfId="0" priority="4" operator="lessThanOrEqual">
+      <formula>I9</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R11">
+    <cfRule type="cellIs" dxfId="0" priority="21" operator="lessThanOrEqual">
+      <formula>H11</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R13">
+    <cfRule type="cellIs" dxfId="0" priority="23" operator="lessThanOrEqual">
+      <formula>H13</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R14">
+    <cfRule type="cellIs" dxfId="0" priority="25" operator="lessThanOrEqual">
+      <formula>H14</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R18">
+    <cfRule type="cellIs" dxfId="0" priority="27" operator="lessThanOrEqual">
+      <formula>H18</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R20">
+    <cfRule type="cellIs" dxfId="0" priority="29" operator="lessThanOrEqual">
+      <formula>H20</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R22">
+    <cfRule type="cellIs" dxfId="0" priority="31" operator="lessThanOrEqual">
+      <formula>H22</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R23">
+    <cfRule type="cellIs" dxfId="0" priority="33" operator="lessThanOrEqual">
+      <formula>H23</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R29">
+    <cfRule type="cellIs" dxfId="0" priority="35" operator="lessThanOrEqual">
+      <formula>H29</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R7">
+    <cfRule type="cellIs" dxfId="0" priority="17" operator="lessThanOrEqual">
+      <formula>H7</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R9">
+    <cfRule type="cellIs" dxfId="0" priority="19" operator="lessThanOrEqual">
+      <formula>H9</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S11">
+    <cfRule type="cellIs" dxfId="0" priority="22" operator="lessThanOrEqual">
+      <formula>I11</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S13">
+    <cfRule type="cellIs" dxfId="0" priority="24" operator="lessThanOrEqual">
+      <formula>I13</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S14">
+    <cfRule type="cellIs" dxfId="0" priority="26" operator="lessThanOrEqual">
+      <formula>I14</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S18">
+    <cfRule type="cellIs" dxfId="0" priority="28" operator="lessThanOrEqual">
+      <formula>I18</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S20">
+    <cfRule type="cellIs" dxfId="0" priority="30" operator="lessThanOrEqual">
+      <formula>I20</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S22">
+    <cfRule type="cellIs" dxfId="0" priority="32" operator="lessThanOrEqual">
+      <formula>I22</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S23">
+    <cfRule type="cellIs" dxfId="0" priority="34" operator="lessThanOrEqual">
+      <formula>I23</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S29">
+    <cfRule type="cellIs" dxfId="0" priority="36" operator="lessThanOrEqual">
       <formula>I29</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R10">
-    <cfRule type="cellIs" dxfId="0" priority="15" operator="lessThanOrEqual">
-      <formula>H10</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="R11">
-    <cfRule type="cellIs" dxfId="0" priority="17" operator="lessThanOrEqual">
+  <conditionalFormatting sqref="S7">
+    <cfRule type="cellIs" dxfId="0" priority="18" operator="lessThanOrEqual">
+      <formula>I7</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S9">
+    <cfRule type="cellIs" dxfId="0" priority="20" operator="lessThanOrEqual">
+      <formula>I9</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="X11">
+    <cfRule type="cellIs" dxfId="0" priority="41" operator="lessThanOrEqual">
       <formula>H11</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R12">
-    <cfRule type="cellIs" dxfId="0" priority="19" operator="lessThanOrEqual">
-      <formula>H12</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="R13">
-    <cfRule type="cellIs" dxfId="0" priority="21" operator="lessThanOrEqual">
+  <conditionalFormatting sqref="X13">
+    <cfRule type="cellIs" dxfId="0" priority="43" operator="lessThanOrEqual">
       <formula>H13</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R17">
-    <cfRule type="cellIs" dxfId="0" priority="23" operator="lessThanOrEqual">
-      <formula>H17</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="R19">
-    <cfRule type="cellIs" dxfId="0" priority="25" operator="lessThanOrEqual">
-      <formula>H19</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="R20">
-    <cfRule type="cellIs" dxfId="0" priority="27" operator="lessThanOrEqual">
-      <formula>H20</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="R21">
-    <cfRule type="cellIs" dxfId="0" priority="29" operator="lessThanOrEqual">
-      <formula>H21</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="R29">
-    <cfRule type="cellIs" dxfId="0" priority="31" operator="lessThanOrEqual">
+  <conditionalFormatting sqref="X14">
+    <cfRule type="cellIs" dxfId="0" priority="45" operator="lessThanOrEqual">
+      <formula>H14</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="X22">
+    <cfRule type="cellIs" dxfId="0" priority="47" operator="lessThanOrEqual">
+      <formula>H22</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="X29">
+    <cfRule type="cellIs" dxfId="0" priority="49" operator="lessThanOrEqual">
       <formula>H29</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S10">
-    <cfRule type="cellIs" dxfId="0" priority="16" operator="lessThanOrEqual">
-      <formula>I10</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S11">
-    <cfRule type="cellIs" dxfId="0" priority="18" operator="lessThanOrEqual">
+  <conditionalFormatting sqref="X7">
+    <cfRule type="cellIs" dxfId="0" priority="37" operator="lessThanOrEqual">
+      <formula>H7</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="X9">
+    <cfRule type="cellIs" dxfId="0" priority="39" operator="lessThanOrEqual">
+      <formula>H9</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y11">
+    <cfRule type="cellIs" dxfId="0" priority="42" operator="lessThanOrEqual">
       <formula>I11</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S12">
-    <cfRule type="cellIs" dxfId="0" priority="20" operator="lessThanOrEqual">
-      <formula>I12</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S13">
-    <cfRule type="cellIs" dxfId="0" priority="22" operator="lessThanOrEqual">
+  <conditionalFormatting sqref="Y13">
+    <cfRule type="cellIs" dxfId="0" priority="44" operator="lessThanOrEqual">
       <formula>I13</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S17">
-    <cfRule type="cellIs" dxfId="0" priority="24" operator="lessThanOrEqual">
-      <formula>I17</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S19">
-    <cfRule type="cellIs" dxfId="0" priority="26" operator="lessThanOrEqual">
-      <formula>I19</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S20">
-    <cfRule type="cellIs" dxfId="0" priority="28" operator="lessThanOrEqual">
-      <formula>I20</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S21">
-    <cfRule type="cellIs" dxfId="0" priority="30" operator="lessThanOrEqual">
-      <formula>I21</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S29">
-    <cfRule type="cellIs" dxfId="0" priority="32" operator="lessThanOrEqual">
+  <conditionalFormatting sqref="Y14">
+    <cfRule type="cellIs" dxfId="0" priority="46" operator="lessThanOrEqual">
+      <formula>I14</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y22">
+    <cfRule type="cellIs" dxfId="0" priority="48" operator="lessThanOrEqual">
+      <formula>I22</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y29">
+    <cfRule type="cellIs" dxfId="0" priority="50" operator="lessThanOrEqual">
       <formula>I29</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="X11">
-    <cfRule type="cellIs" dxfId="0" priority="33" operator="lessThanOrEqual">
-      <formula>H11</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="X12">
-    <cfRule type="cellIs" dxfId="0" priority="35" operator="lessThanOrEqual">
-      <formula>H12</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="X13">
-    <cfRule type="cellIs" dxfId="0" priority="37" operator="lessThanOrEqual">
-      <formula>H13</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="X17">
-    <cfRule type="cellIs" dxfId="0" priority="39" operator="lessThanOrEqual">
-      <formula>H17</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="X19">
-    <cfRule type="cellIs" dxfId="0" priority="41" operator="lessThanOrEqual">
-      <formula>H19</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="X21">
-    <cfRule type="cellIs" dxfId="0" priority="43" operator="lessThanOrEqual">
-      <formula>H21</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Y11">
-    <cfRule type="cellIs" dxfId="0" priority="34" operator="lessThanOrEqual">
-      <formula>I11</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Y12">
-    <cfRule type="cellIs" dxfId="0" priority="36" operator="lessThanOrEqual">
-      <formula>I12</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Y13">
+  <conditionalFormatting sqref="Y7">
     <cfRule type="cellIs" dxfId="0" priority="38" operator="lessThanOrEqual">
-      <formula>I13</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Y17">
+      <formula>I7</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y9">
     <cfRule type="cellIs" dxfId="0" priority="40" operator="lessThanOrEqual">
-      <formula>I17</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Y19">
-    <cfRule type="cellIs" dxfId="0" priority="42" operator="lessThanOrEqual">
-      <formula>I19</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Y21">
-    <cfRule type="cellIs" dxfId="0" priority="44" operator="lessThanOrEqual">
-      <formula>I21</formula>
+      <formula>I9</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="O10" r:id="rId1"/>
-    <hyperlink ref="U10" r:id="rId2"/>
-    <hyperlink ref="O11" r:id="rId3"/>
-    <hyperlink ref="U11" r:id="rId4"/>
-    <hyperlink ref="AA11" r:id="rId5"/>
-    <hyperlink ref="O12" r:id="rId6"/>
-    <hyperlink ref="U12" r:id="rId7"/>
-    <hyperlink ref="AA12" r:id="rId8"/>
-    <hyperlink ref="O13" r:id="rId9"/>
-    <hyperlink ref="U13" r:id="rId10"/>
-    <hyperlink ref="AA13" r:id="rId11"/>
-    <hyperlink ref="U17" r:id="rId12"/>
-    <hyperlink ref="AA17" r:id="rId13"/>
-    <hyperlink ref="O19" r:id="rId14"/>
-    <hyperlink ref="U19" r:id="rId15"/>
-    <hyperlink ref="AA19" r:id="rId16"/>
-    <hyperlink ref="U20" r:id="rId17"/>
-    <hyperlink ref="O21" r:id="rId18"/>
-    <hyperlink ref="U21" r:id="rId19"/>
-    <hyperlink ref="AA21" r:id="rId20"/>
-    <hyperlink ref="O29" r:id="rId21"/>
-    <hyperlink ref="U29" r:id="rId22"/>
+    <hyperlink ref="O7" r:id="rId1"/>
+    <hyperlink ref="U7" r:id="rId2"/>
+    <hyperlink ref="AA7" r:id="rId3"/>
+    <hyperlink ref="O9" r:id="rId4"/>
+    <hyperlink ref="U9" r:id="rId5"/>
+    <hyperlink ref="AA9" r:id="rId6"/>
+    <hyperlink ref="O11" r:id="rId7"/>
+    <hyperlink ref="U11" r:id="rId8"/>
+    <hyperlink ref="AA11" r:id="rId9"/>
+    <hyperlink ref="O13" r:id="rId10"/>
+    <hyperlink ref="U13" r:id="rId11"/>
+    <hyperlink ref="AA13" r:id="rId12"/>
+    <hyperlink ref="O14" r:id="rId13"/>
+    <hyperlink ref="U14" r:id="rId14"/>
+    <hyperlink ref="AA14" r:id="rId15"/>
+    <hyperlink ref="U18" r:id="rId16"/>
+    <hyperlink ref="O20" r:id="rId17"/>
+    <hyperlink ref="U20" r:id="rId18"/>
+    <hyperlink ref="O22" r:id="rId19"/>
+    <hyperlink ref="U22" r:id="rId20"/>
+    <hyperlink ref="AA22" r:id="rId21"/>
+    <hyperlink ref="O23" r:id="rId22"/>
+    <hyperlink ref="U23" r:id="rId23"/>
+    <hyperlink ref="U29" r:id="rId24"/>
+    <hyperlink ref="AA29" r:id="rId25"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId23"/>
+  <legacyDrawing r:id="rId26"/>
 </worksheet>
 </file>
</xml_diff>